<commit_message>
- Added support for multiple indicators per flow and flow carbon tracking. Carbon is now dynamically simulated along with the Solid Wood Equivalent value.
- Added utility methods to FlowSolver to request process total inflows in either evaluated Solid Wood Equivalent values or as in evaluated Carbon value

- Flow carbon content factor is by default 1.0 if value is not defined in data file.

- Bar charts now show information for each dynamic stock (SWE total, SWE change, Carbon total, Carbon change).
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184F3E62-F96C-4C96-8B54-71FD390548F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF410626-04C2-4A61-8137-D466F8EC7F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="116">
   <si>
     <t>Years</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Export</t>
   </si>
   <si>
-    <t xml:space="preserve">Conversion factor used </t>
-  </si>
-  <si>
     <t>Normalized X</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://excalidraw.com/#json=Lj-sDbAMDNeaA9bmCep8J,9nZyAhAf-Q5KkiQ4syeq1w </t>
-  </si>
-  <si>
-    <t>absolute (SWE), relative (%)</t>
   </si>
   <si>
     <t>SWE</t>
@@ -318,31 +312,7 @@
     </r>
   </si>
   <si>
-    <t>Source_process*</t>
-  </si>
-  <si>
     <t>Transformation_Stage*</t>
-  </si>
-  <si>
-    <t>Source_process_location*</t>
-  </si>
-  <si>
-    <t>Target_process*</t>
-  </si>
-  <si>
-    <t>Target_process_location*</t>
-  </si>
-  <si>
-    <t>Source _ID*</t>
-  </si>
-  <si>
-    <t>Target_ID*</t>
-  </si>
-  <si>
-    <t>Value*</t>
-  </si>
-  <si>
-    <t>Year*</t>
   </si>
   <si>
     <t xml:space="preserve">Must filled in cells </t>
@@ -480,6 +450,57 @@
       </rPr>
       <t xml:space="preserve"> (e.g. P3:EU -&gt; P5:EU with value: 100%)  </t>
     </r>
+  </si>
+  <si>
+    <t>m3, kg, %</t>
+  </si>
+  <si>
+    <t>2 columns needed for each indicator (value and comment)</t>
+  </si>
+  <si>
+    <t>Source_process</t>
+  </si>
+  <si>
+    <t>Transformation_Stage</t>
+  </si>
+  <si>
+    <t>Source_process_location</t>
+  </si>
+  <si>
+    <t>Target_process</t>
+  </si>
+  <si>
+    <t>Target_process_location</t>
+  </si>
+  <si>
+    <t>Source _ID</t>
+  </si>
+  <si>
+    <t>Target_ID</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Data_source_comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversion_factor_used </t>
+  </si>
+  <si>
+    <t>Carbon_content_factor</t>
+  </si>
+  <si>
+    <t>Carbon_content_source</t>
+  </si>
+  <si>
+    <t>Indicator0</t>
+  </si>
+  <si>
+    <t>Indicator1</t>
   </si>
 </sst>
 </file>
@@ -571,7 +592,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -579,12 +600,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -594,9 +656,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -628,18 +687,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -655,15 +702,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -825,7 +890,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1417501</xdr:colOff>
+      <xdr:colOff>1398451</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>164512</xdr:rowOff>
     </xdr:to>
@@ -1162,165 +1227,165 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="26" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="29" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="29" style="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="26"/>
+    <col min="5" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="21"/>
+      <c r="C2" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="25"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:5" s="22" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="29"/>
+    </row>
+    <row r="5" spans="1:5" s="22" customFormat="1" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" ht="144.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" s="27" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:5" s="27" customFormat="1" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:5" ht="144.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="28"/>
-    </row>
-    <row r="11" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="20"/>
+      <c r="D11" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1390,7 +1455,7 @@
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>12</v>
@@ -1410,7 +1475,7 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="9"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1428,28 +1493,28 @@
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>17</v>
@@ -1467,16 +1532,16 @@
         <v>21</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -1484,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -1507,13 +1572,13 @@
       </c>
       <c r="M4" s="5"/>
       <c r="P4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="Q4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="R4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -1521,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -1544,13 +1609,13 @@
       </c>
       <c r="M5" s="5"/>
       <c r="P5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="Q5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="R5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1558,7 +1623,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -1580,13 +1645,13 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="Q6" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="R6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1594,7 +1659,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -1616,13 +1681,13 @@
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="Q7" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="R7" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1630,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -1640,7 +1705,7 @@
         <v>P5:EU</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1652,13 +1717,13 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="Q8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" t="s">
         <v>93</v>
-      </c>
-      <c r="R8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1666,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -1688,13 +1753,13 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" t="s">
         <v>94</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>95</v>
-      </c>
-      <c r="R9" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1702,7 +1767,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -1724,13 +1789,13 @@
         <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="Q10" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="R10" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1741,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
-  <dimension ref="A1:O88"/>
+  <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,12 +1827,13 @@
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="40.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15" style="6" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1803,8 +1869,32 @@
       <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1818,58 +1908,87 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="L3" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="M3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q3" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="S3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T3" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="str">
         <f>+_xlfn.XLOOKUP(H4,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -1879,7 +1998,7 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="str">
         <f>+_xlfn.XLOOKUP(I4,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -1900,15 +2019,18 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L4">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="str">
         <f>+_xlfn.XLOOKUP(H5,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -1918,7 +2040,7 @@
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="str">
         <f>+_xlfn.XLOOKUP(I5,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -1939,15 +2061,18 @@
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L5">
         <v>2021</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="str">
         <f>+_xlfn.XLOOKUP(H6,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -1957,7 +2082,7 @@
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" t="str">
         <f>+_xlfn.XLOOKUP(I6,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -1978,16 +2103,19 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L6">
         <v>2021</v>
       </c>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="7"/>
+      <c r="P6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="str">
         <f>+_xlfn.XLOOKUP(H7,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -1997,7 +2125,7 @@
         <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" t="str">
         <f>+_xlfn.XLOOKUP(I7,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2018,16 +2146,19 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L7">
         <v>2021</v>
       </c>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="7"/>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="str">
         <f>+_xlfn.XLOOKUP(H8,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2037,7 +2168,7 @@
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" t="str">
         <f>+_xlfn.XLOOKUP(I8,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2063,11 +2194,14 @@
       <c r="L8">
         <v>2021</v>
       </c>
-      <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="7"/>
+      <c r="P8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="str">
         <f>+_xlfn.XLOOKUP(H9,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2077,7 +2211,7 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" t="str">
         <f>+_xlfn.XLOOKUP(I9,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2103,11 +2237,14 @@
       <c r="L9">
         <v>2021</v>
       </c>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="7"/>
+      <c r="P9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="str">
         <f>+_xlfn.XLOOKUP(H10,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2117,7 +2254,7 @@
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" t="str">
         <f>+_xlfn.XLOOKUP(I10,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2138,15 +2275,18 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L10">
         <v>2021</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="str">
         <f>+_xlfn.XLOOKUP(H11,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2156,7 +2296,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
@@ -2176,19 +2316,22 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L11">
         <v>2021</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="str">
         <f>+_xlfn.XLOOKUP(H13,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2198,7 +2341,7 @@
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" t="str">
         <f>+_xlfn.XLOOKUP(I13,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2219,15 +2362,18 @@
         <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L13">
         <v>2022</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="str">
         <f>+_xlfn.XLOOKUP(H14,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2237,7 +2383,7 @@
         <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" t="str">
         <f>+_xlfn.XLOOKUP(I14,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2258,15 +2404,18 @@
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L14">
         <v>2022</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" t="str">
         <f>+_xlfn.XLOOKUP(H15,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2276,7 +2425,7 @@
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" t="str">
         <f>+_xlfn.XLOOKUP(I15,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2297,16 +2446,19 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L15">
         <v>2022</v>
       </c>
-      <c r="N15" s="8"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="7"/>
+      <c r="P15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" t="str">
         <f>+_xlfn.XLOOKUP(H16,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2316,7 +2468,7 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" t="str">
         <f>+_xlfn.XLOOKUP(I16,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2337,16 +2489,19 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16">
         <v>2022</v>
       </c>
-      <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N16" s="7"/>
+      <c r="P16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="str">
         <f>+_xlfn.XLOOKUP(H17,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2356,7 +2511,7 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" t="str">
         <f>+_xlfn.XLOOKUP(I17,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2382,11 +2537,14 @@
       <c r="L17">
         <v>2022</v>
       </c>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="7"/>
+      <c r="P17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="str">
         <f>+_xlfn.XLOOKUP(H18,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2396,7 +2554,7 @@
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" t="str">
         <f>+_xlfn.XLOOKUP(I18,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2417,15 +2575,18 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L18">
         <v>2022</v>
       </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="str">
         <f>+_xlfn.XLOOKUP(H19,Processes!$D$4:$D$46,Processes!$E$4:$E$46)</f>
@@ -2435,7 +2596,7 @@
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
         <v>27</v>
@@ -2455,62 +2616,65 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L19">
         <v>2022</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="O31"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
@@ -2569,8 +2733,8 @@
       <c r="O41"/>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="10" t="s">
-        <v>52</v>
+      <c r="C42" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -2857,11 +3021,6 @@
       <c r="O88"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:M86" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:M20">
-      <sortCondition ref="L3"/>
-    </sortState>
-  </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C42" r:id="rId1" location="json=Lj-sDbAMDNeaA9bmCep8J,9nZyAhAf-Q5KkiQ4syeq1w " xr:uid="{37B4E084-5E8C-4C2B-AC88-5E1F4296DCE7}"/>
@@ -2882,6 +3041,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -3144,18 +3315,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
@@ -3165,6 +3324,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3181,21 +3357,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Comments for users on the Process tab.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B805BA-9E14-42F8-93B0-230D0489FB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47B6234-13E1-44A3-9626-4F9A57C2454F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-14505" yWindow="135" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -662,9 +662,6 @@
     <t>FoldedNormal</t>
   </si>
   <si>
-    <t xml:space="preserve">Distribution Type </t>
-  </si>
-  <si>
     <t>Source_process</t>
   </si>
   <si>
@@ -708,6 +705,9 @@
   </si>
   <si>
     <t xml:space="preserve">tuple </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution_parameters </t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1551,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1596,7 +1596,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>11</v>
@@ -1655,28 +1655,28 @@
     <row r="3" spans="1:18" s="36" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="34"/>
       <c r="B3" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="D3" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="E3" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>167</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>158</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>168</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="J3" s="35" t="s">
         <v>16</v>
@@ -2036,7 +2036,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameter" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I4:I1048576" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameter" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I5:I1048576 I4" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2060,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2182,31 +2182,31 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="E3" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="F3" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="G3" s="25" t="s">
+      <c r="H3" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="J3" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>164</v>
       </c>
       <c r="K3" s="25" t="s">
         <v>148</v>
@@ -2224,7 +2224,7 @@
         <v>61</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q3" s="26" t="s">
         <v>150</v>
@@ -8027,7 +8027,7 @@
   <dimension ref="C2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Implemented reading model parameters from Excel file and added Settings-sheet to example data file (example_data.xlsx)
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47B6234-13E1-44A3-9626-4F9A57C2454F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512B59A2-9EB0-4FAA-B1B1-D3ABC6AECAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="135" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
     <sheet name="Processes" sheetId="6" r:id="rId2"/>
     <sheet name="Flows" sheetId="1" r:id="rId3"/>
     <sheet name="DMFA results (example)" sheetId="8" r:id="rId4"/>
-    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId6"/>
+    <sheet name="Settings" sheetId="10" r:id="rId5"/>
+    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Flows!$B$3:$M$89</definedName>
+    <definedName name="Boolean">Sheet1!$D$2:$D$3</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -80,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="201">
   <si>
     <t>Years</t>
   </si>
@@ -709,6 +711,93 @@
   <si>
     <t xml:space="preserve">Distribution_parameters </t>
   </si>
+  <si>
+    <t>These are the settings for the scenario file</t>
+  </si>
+  <si>
+    <t>Parameter name</t>
+  </si>
+  <si>
+    <t>sheet_name_processes</t>
+  </si>
+  <si>
+    <t>column_range_processes</t>
+  </si>
+  <si>
+    <t>B:R</t>
+  </si>
+  <si>
+    <t>skip_num_rows_processes</t>
+  </si>
+  <si>
+    <t>sheet_name_flows</t>
+  </si>
+  <si>
+    <t>column_range_flows</t>
+  </si>
+  <si>
+    <t>skip_num_rows_flows</t>
+  </si>
+  <si>
+    <t>Sheet name that contains data for Processes, e.g. (Processes)</t>
+  </si>
+  <si>
+    <t>Number of rows to skip when reading data for Processes (e.g. 2). NOTE: Header row must be the first row to read!</t>
+  </si>
+  <si>
+    <t>Sheet name that contains data for Flows, (e.g. Flows)</t>
+  </si>
+  <si>
+    <t>Start column name and end column name separated by colon (e.g. B:R) that contain data for Flows</t>
+  </si>
+  <si>
+    <t>Start column name and end column name separated by colon (e.g. B:R) that contain data for Processes</t>
+  </si>
+  <si>
+    <t>start_year</t>
+  </si>
+  <si>
+    <t>B:U</t>
+  </si>
+  <si>
+    <t>Starting year of the model</t>
+  </si>
+  <si>
+    <t>end_year</t>
+  </si>
+  <si>
+    <t>detect_year_range</t>
+  </si>
+  <si>
+    <t>Boolean values</t>
+  </si>
+  <si>
+    <t>Detect the year range automatically from file</t>
+  </si>
+  <si>
+    <t>use_virtual_flows</t>
+  </si>
+  <si>
+    <t>Use virtual flows. If enabled, creates missing flows for Processes that have imbalance of input and output flows i.e. unreported flows</t>
+  </si>
+  <si>
+    <t>conversion_factor_c_to_co2</t>
+  </si>
+  <si>
+    <t>Conversion factor from C to CO2</t>
+  </si>
+  <si>
+    <t>Ending year of the model, included in in time range</t>
+  </si>
+  <si>
+    <t>Example: first parameter sheet_name_processes goes to cell B6 and value Processes goes to cell C6.</t>
+  </si>
+  <si>
+    <t>NOTE: The parameters are read columns B and C and from row 7 downward, including that row.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
 </sst>
 </file>
 
@@ -719,7 +808,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,6 +862,21 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="0.79998168889431442"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -864,7 +968,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -946,6 +1050,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -966,8 +1079,59 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1355,175 +1519,173 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="23" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="23" customWidth="1"/>
     <col min="3" max="3" width="29" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="21"/>
+    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="39"/>
-    </row>
-    <row r="2" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="46"/>
+    </row>
+    <row r="2" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="38"/>
-    </row>
-    <row r="4" spans="1:5" s="22" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="45"/>
+    </row>
+    <row r="4" spans="1:5" s="22" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="41"/>
-    </row>
-    <row r="5" spans="1:5" s="22" customFormat="1" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="1:5" s="22" customFormat="1" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="41"/>
-    </row>
-    <row r="6" spans="1:5" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="1:5" ht="144.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="37"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="44"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="40"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="47"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="37"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="44"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="40"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="47"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="40"/>
-    </row>
-    <row r="11" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="47"/>
+    </row>
+    <row r="11" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="37"/>
-    </row>
-    <row r="12" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="44"/>
+    </row>
+    <row r="12" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>126</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="D12" s="37"/>
-    </row>
-    <row r="13" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="44"/>
+    </row>
+    <row r="13" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>128</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="37"/>
+      <c r="D13" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1550,31 +1712,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" customWidth="1"/>
-    <col min="2" max="2" width="20.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" customWidth="1"/>
-    <col min="14" max="14" width="13.36328125" customWidth="1"/>
-    <col min="15" max="15" width="12.54296875" customWidth="1"/>
-    <col min="16" max="16" width="11.81640625" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" customWidth="1"/>
-    <col min="18" max="18" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -1626,7 +1788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1652,7 +1814,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="36" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="35" t="s">
         <v>164</v>
@@ -1706,7 +1868,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1743,7 +1905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1780,7 +1942,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1816,7 +1978,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1852,7 +2014,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1888,7 +2050,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1924,7 +2086,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1960,7 +2122,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1996,7 +2158,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2032,7 +2194,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
@@ -2064,28 +2226,28 @@
       <selection activeCell="D1" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="20.36328125" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="21.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.6328125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2150,7 +2312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2179,7 +2341,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="25" t="s">
         <v>156</v>
@@ -2242,7 +2404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -2294,7 +2456,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -2346,7 +2508,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -2398,7 +2560,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -2450,7 +2612,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -2502,7 +2664,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -2554,7 +2716,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -2606,7 +2768,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -2657,7 +2819,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -2709,7 +2871,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -2760,160 +2922,160 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="N14"/>
       <c r="Q14" s="29"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
       <c r="Q15" s="29"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
       <c r="Q16" s="29"/>
     </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
       <c r="Q17" s="29"/>
     </row>
-    <row r="18" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
       <c r="Q18" s="29"/>
     </row>
-    <row r="19" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
       <c r="Q21" s="29"/>
     </row>
-    <row r="22" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
       <c r="Q22" s="29"/>
     </row>
-    <row r="23" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
       <c r="Q23" s="29"/>
     </row>
-    <row r="24" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="O36"/>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="O37"/>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="O38"/>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
       <c r="O39"/>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
       <c r="O41"/>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
       <c r="O42"/>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
       <c r="O43"/>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C44" s="29" t="s">
         <v>147</v>
       </c>
@@ -2922,258 +3084,258 @@
       <c r="N44"/>
       <c r="O44"/>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
       <c r="O47"/>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
       <c r="O48"/>
     </row>
-    <row r="49" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
       <c r="O49"/>
     </row>
-    <row r="50" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
       <c r="O50"/>
     </row>
-    <row r="51" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
       <c r="O51"/>
     </row>
-    <row r="52" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
       <c r="O52"/>
     </row>
-    <row r="53" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
       <c r="O53"/>
     </row>
-    <row r="54" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
       <c r="O54"/>
     </row>
-    <row r="55" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
       <c r="O55"/>
     </row>
-    <row r="56" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
       <c r="O56"/>
     </row>
-    <row r="57" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
       <c r="O57"/>
     </row>
-    <row r="58" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
       <c r="O58"/>
     </row>
-    <row r="59" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
       <c r="O59"/>
     </row>
-    <row r="60" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
       <c r="O60"/>
     </row>
-    <row r="61" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
       <c r="O61"/>
     </row>
-    <row r="62" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
       <c r="O62"/>
     </row>
-    <row r="63" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
       <c r="O63"/>
     </row>
-    <row r="64" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
       <c r="O64"/>
     </row>
-    <row r="65" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
       <c r="O65"/>
     </row>
-    <row r="66" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
       <c r="O66"/>
     </row>
-    <row r="67" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
       <c r="O67"/>
     </row>
-    <row r="68" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
       <c r="O68"/>
     </row>
-    <row r="69" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
       <c r="O69"/>
     </row>
-    <row r="70" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
       <c r="O70"/>
     </row>
-    <row r="71" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
       <c r="O71"/>
     </row>
-    <row r="72" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
       <c r="O72"/>
     </row>
-    <row r="73" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
       <c r="O73"/>
     </row>
-    <row r="74" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
       <c r="O74"/>
     </row>
-    <row r="75" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
       <c r="O75"/>
     </row>
-    <row r="76" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
       <c r="O76"/>
     </row>
-    <row r="77" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
       <c r="O77"/>
     </row>
-    <row r="78" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
       <c r="O78"/>
     </row>
-    <row r="79" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
       <c r="O80"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
       <c r="O81"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
       <c r="O82"/>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
       <c r="O83"/>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
       <c r="O84"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
       <c r="O85"/>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N86"/>
       <c r="O86"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3184,25 +3346,25 @@
       <c r="N87"/>
       <c r="O87"/>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
       <c r="O88"/>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
       <c r="O89"/>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
       <c r="O90"/>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
@@ -3231,20 +3393,20 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
-    <col min="2" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" customWidth="1"/>
-    <col min="16" max="16" width="15.26953125" customWidth="1"/>
-    <col min="17" max="17" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.54296875" customWidth="1"/>
-    <col min="28" max="28" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.5703125" customWidth="1"/>
+    <col min="28" max="28" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>120</v>
       </c>
@@ -3252,7 +3414,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>121</v>
       </c>
@@ -3327,7 +3489,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2021</v>
       </c>
@@ -3407,7 +3569,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2022</v>
       </c>
@@ -3487,7 +3649,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2023</v>
       </c>
@@ -3567,7 +3729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2024</v>
       </c>
@@ -3647,7 +3809,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2025</v>
       </c>
@@ -3727,7 +3889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2026</v>
       </c>
@@ -3807,7 +3969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2027</v>
       </c>
@@ -3887,7 +4049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2028</v>
       </c>
@@ -3967,7 +4129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2029</v>
       </c>
@@ -4047,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2030</v>
       </c>
@@ -4127,7 +4289,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>151</v>
       </c>
@@ -4162,7 +4324,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
       <c r="C14">
         <v>2021</v>
@@ -4225,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
       <c r="B15">
         <v>2021</v>
@@ -4291,7 +4453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2022</v>
       </c>
@@ -4356,7 +4518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2023</v>
       </c>
@@ -4421,7 +4583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2024</v>
       </c>
@@ -4486,7 +4648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2025</v>
       </c>
@@ -4551,7 +4713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2026</v>
       </c>
@@ -4616,7 +4778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2027</v>
       </c>
@@ -4681,7 +4843,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2028</v>
       </c>
@@ -4747,7 +4909,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2029</v>
       </c>
@@ -4812,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2030</v>
       </c>
@@ -4877,7 +5039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>90</v>
       </c>
@@ -4912,7 +5074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26">
         <v>2021</v>
@@ -4975,7 +5137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2021</v>
       </c>
@@ -5040,7 +5202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2022</v>
       </c>
@@ -5105,7 +5267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2023</v>
       </c>
@@ -5170,7 +5332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2024</v>
       </c>
@@ -5235,7 +5397,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>2025</v>
       </c>
@@ -5300,7 +5462,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>2026</v>
       </c>
@@ -5365,7 +5527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>2027</v>
       </c>
@@ -5430,7 +5592,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2028</v>
       </c>
@@ -5495,7 +5657,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2029</v>
       </c>
@@ -5560,7 +5722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2030</v>
       </c>
@@ -5625,7 +5787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>91</v>
       </c>
@@ -5660,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B38" s="32"/>
       <c r="C38">
         <v>2021</v>
@@ -5723,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2021</v>
       </c>
@@ -5788,7 +5950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2022</v>
       </c>
@@ -5853,7 +6015,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="41" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>2023</v>
       </c>
@@ -5918,7 +6080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>2024</v>
       </c>
@@ -5983,7 +6145,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2025</v>
       </c>
@@ -6048,7 +6210,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>2026</v>
       </c>
@@ -6113,7 +6275,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2027</v>
       </c>
@@ -6178,7 +6340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>2028</v>
       </c>
@@ -6243,7 +6405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>2029</v>
       </c>
@@ -6308,7 +6470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>2030</v>
       </c>
@@ -6373,7 +6535,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="49" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W49">
         <v>2025</v>
       </c>
@@ -6405,7 +6567,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="50" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="50" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W50">
         <v>2025</v>
       </c>
@@ -6437,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="51" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W51">
         <v>2025</v>
       </c>
@@ -6469,7 +6631,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="52" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W52">
         <v>2025</v>
       </c>
@@ -6501,7 +6663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="53" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W53">
         <v>2026</v>
       </c>
@@ -6533,7 +6695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="54" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W54">
         <v>2026</v>
       </c>
@@ -6565,7 +6727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="55" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W55">
         <v>2026</v>
       </c>
@@ -6597,7 +6759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="56" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W56">
         <v>2026</v>
       </c>
@@ -6629,7 +6791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="57" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W57">
         <v>2026</v>
       </c>
@@ -6661,7 +6823,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="58" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W58">
         <v>2026</v>
       </c>
@@ -6693,7 +6855,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="59" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="59" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W59">
         <v>2026</v>
       </c>
@@ -6725,7 +6887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="60" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W60">
         <v>2026</v>
       </c>
@@ -6757,7 +6919,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="61" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W61">
         <v>2026</v>
       </c>
@@ -6789,7 +6951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="62" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W62">
         <v>2026</v>
       </c>
@@ -6821,7 +6983,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="63" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W63">
         <v>2027</v>
       </c>
@@ -6853,7 +7015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="64" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W64">
         <v>2027</v>
       </c>
@@ -6885,7 +7047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="65" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W65">
         <v>2027</v>
       </c>
@@ -6917,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="66" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W66">
         <v>2027</v>
       </c>
@@ -6949,7 +7111,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="67" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W67">
         <v>2027</v>
       </c>
@@ -6981,7 +7143,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="68" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="68" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W68">
         <v>2027</v>
       </c>
@@ -7013,7 +7175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="69" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W69">
         <v>2027</v>
       </c>
@@ -7045,7 +7207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="70" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W70">
         <v>2027</v>
       </c>
@@ -7077,7 +7239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="71" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W71">
         <v>2027</v>
       </c>
@@ -7109,7 +7271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="72" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W72">
         <v>2027</v>
       </c>
@@ -7141,7 +7303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="73" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W73">
         <v>2028</v>
       </c>
@@ -7173,7 +7335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="74" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W74">
         <v>2028</v>
       </c>
@@ -7205,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="75" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W75">
         <v>2028</v>
       </c>
@@ -7237,7 +7399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="76" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W76">
         <v>2028</v>
       </c>
@@ -7269,7 +7431,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="77" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="77" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W77">
         <v>2028</v>
       </c>
@@ -7301,7 +7463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="78" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W78">
         <v>2028</v>
       </c>
@@ -7333,7 +7495,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="79" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W79">
         <v>2028</v>
       </c>
@@ -7365,7 +7527,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="80" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W80">
         <v>2028</v>
       </c>
@@ -7397,7 +7559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="81" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W81">
         <v>2028</v>
       </c>
@@ -7429,7 +7591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="82" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W82">
         <v>2028</v>
       </c>
@@ -7461,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="83" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W83">
         <v>2029</v>
       </c>
@@ -7493,7 +7655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="84" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W84">
         <v>2029</v>
       </c>
@@ -7525,7 +7687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="85" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W85">
         <v>2029</v>
       </c>
@@ -7557,7 +7719,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="86" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="86" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W86">
         <v>2029</v>
       </c>
@@ -7589,7 +7751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="87" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W87">
         <v>2029</v>
       </c>
@@ -7621,7 +7783,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="88" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W88">
         <v>2029</v>
       </c>
@@ -7653,7 +7815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="89" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W89">
         <v>2029</v>
       </c>
@@ -7685,7 +7847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="90" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W90">
         <v>2029</v>
       </c>
@@ -7717,7 +7879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="91" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W91">
         <v>2029</v>
       </c>
@@ -7749,7 +7911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="92" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W92">
         <v>2029</v>
       </c>
@@ -7781,7 +7943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="93" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W93">
         <v>2030</v>
       </c>
@@ -7801,7 +7963,7 @@
         <v>12.205439999999999</v>
       </c>
     </row>
-    <row r="94" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="94" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W94">
         <v>2030</v>
       </c>
@@ -7821,7 +7983,7 @@
         <v>10.171200000000001</v>
       </c>
     </row>
-    <row r="95" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="95" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W95">
         <v>2030</v>
       </c>
@@ -7841,7 +8003,7 @@
         <v>3.6972</v>
       </c>
     </row>
-    <row r="96" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="96" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W96">
         <v>2030</v>
       </c>
@@ -7861,7 +8023,7 @@
         <v>5.5296000000000003</v>
       </c>
     </row>
-    <row r="97" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="97" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W97">
         <v>2030</v>
       </c>
@@ -7881,7 +8043,7 @@
         <v>3.456</v>
       </c>
     </row>
-    <row r="98" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="98" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W98">
         <v>2030</v>
       </c>
@@ -7901,7 +8063,7 @@
         <v>2.21184</v>
       </c>
     </row>
-    <row r="99" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="99" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W99">
         <v>2030</v>
       </c>
@@ -7921,7 +8083,7 @@
         <v>3.1103999999999998</v>
       </c>
     </row>
-    <row r="100" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="100" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W100">
         <v>2030</v>
       </c>
@@ -7941,7 +8103,7 @@
         <v>3.456</v>
       </c>
     </row>
-    <row r="101" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="101" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W101">
         <v>2030</v>
       </c>
@@ -7961,7 +8123,7 @@
         <v>4.0684800000000001</v>
       </c>
     </row>
-    <row r="102" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="102" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W102">
         <v>2030</v>
       </c>
@@ -7987,26 +8149,223 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE76F46E-F9E0-4FFD-9C15-07511C841BF9}">
+  <dimension ref="B2:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="103.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="41">
+        <v>2</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="41">
+        <v>2</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="41">
+        <v>2021</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="41">
+        <v>2030</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="41"/>
+      <c r="E16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="39">
+        <v>3.67</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C15:C16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16" xr:uid="{5D3B6C52-629A-48C0-B345-97745DEAC80B}">
+      <formula1>Boolean</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>132</v>
       </c>
@@ -8022,37 +8381,52 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
-  <dimension ref="C2:C6"/>
+  <dimension ref="C1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>154</v>
       </c>

</xml_diff>

<commit_message>
Implemented major quality-of-life improvements:
- Settings are now read from the Excel file
- Parameter checking is done automatically when data is read from Excel file and proper error message is shown to the user
- Mass balance summary
- Cleaned and refactored codebase
- Added some missing required Python package names to requirements.txt

aiphoria internal changes:
- Unified naming of aiphoria object properties
- Parametrization and automatic type checking is now done automatically for settings read from the Excel file. Error message is shown to the user when parameter does not match with the expected type (e.g. user set string "abc" when checker expected int). This allows easy way to add new parameters that needs to be read from Excel file
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512B59A2-9EB0-4FAA-B1B1-D3ABC6AECAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCB440C-CAE7-4CCD-8E7D-A81CDB95CF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="203">
   <si>
     <t>Years</t>
   </si>
@@ -797,6 +797,12 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>virtual_flows_epsilon</t>
+  </si>
+  <si>
+    <t>If using virtual flows, create virtual flow to process if process total inputs and outputs difference is greater than this value</t>
   </si>
 </sst>
 </file>
@@ -1079,37 +1085,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1712,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,7 +2174,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameter" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I5:I1048576 I4" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameter" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I4:I1048576" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2223,7 +2199,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD3"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2541,7 +2517,7 @@
         <v>Residues:FI</v>
       </c>
       <c r="J6">
-        <v>19.5</v>
+        <v>10</v>
       </c>
       <c r="K6" t="s">
         <v>136</v>
@@ -2612,7 +2588,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -8150,10 +8126,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE76F46E-F9E0-4FFD-9C15-07511C841BF9}">
-  <dimension ref="B2:E17"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8317,13 +8293,24 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>195</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C18" s="39">
         <v>3.67</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" t="s">
+      <c r="D18" s="39"/>
+      <c r="E18" t="s">
         <v>196</v>
       </c>
     </row>
@@ -8385,14 +8372,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
   <dimension ref="C1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.25">
@@ -8437,12 +8423,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8709,21 +8698,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8748,18 +8743,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated example_data.xlsx to include fill_missing_absolute_flows   & fill_missing_relative_flows in the Settings.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6731CD4-0D19-43E4-82B9-20AD9346CFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6666BAD6-E259-4FEE-A971-DD6056DBEE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="208">
   <si>
     <t>Years</t>
   </si>
@@ -165,15 +165,9 @@
     <t xml:space="preserve">float </t>
   </si>
   <si>
-    <t xml:space="preserve">Scenarios </t>
-  </si>
-  <si>
     <t>Please note</t>
   </si>
   <si>
-    <t>Dynamic case (multiple years with different scenarios)</t>
-  </si>
-  <si>
     <t>Process IDs</t>
   </si>
   <si>
@@ -202,18 +196,6 @@
   </si>
   <si>
     <t>Make sure that no whitespaces exist on the process IDs (at the end or beginning)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from the notebook. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must filled in cells </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cells to fill for running aiphoria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please check the starred (*) cells on the processes and flows sheets. </t>
   </si>
   <si>
     <t>General information</t>
@@ -712,32 +694,6 @@
     <t>If using virtual flows, create virtual flow to process if process total inputs and outputs difference is greater than this value</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">If the user wants to run different scenarios using relative value (shares) for the same process, they should add multiple flows (rows) on the flow sheet indicating the change in the value cell (e.g P3:EU -&gt; P5:EU and  value: 100% in 2021 and  P3:EU -&gt; P5:EU and value 50% in 2022). If the scenarios when using relative value (shares) remain the same throughtout the timeline indicated by the user; then aiphoria is </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>repeating the value given for the last year</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g. P3:EU -&gt; P5:EU with value: 50%)  </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">The carbon fraction sheet is only temprorary here and it is being used by thee Flows sheet. In the next version of aiphoria this will be moved. </t>
   </si>
   <si>
@@ -795,6 +751,33 @@
   <si>
     <t>https://excalidraw.com/#json=TH95eCDBsN1pfqczsMf84,S3TGIZvZiI-AUl8oZJcUYg</t>
   </si>
+  <si>
+    <t>fill_missing_relative_flows</t>
+  </si>
+  <si>
+    <t>fill_missing_absolute_flows</t>
+  </si>
+  <si>
+    <t>Fill in missing timestep with the last timestep provided by the user. Default value is True</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String </t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from Settings. </t>
+  </si>
 </sst>
 </file>
 
@@ -805,7 +788,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -851,14 +834,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1033,14 +1008,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1068,7 +1043,22 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1106,23 +1096,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>238497</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>162193</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>717176</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132512</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>68549</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>575283</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>45515</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Graphic 3">
+        <xdr:cNvPr id="3" name="Graphic 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A65083D5-FD42-D957-1C27-02B79123CF56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BABF4E-C7EF-DF86-E1EE-F6428C7FAEDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1144,8 +1134,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5023409" y="2750752"/>
-          <a:ext cx="9443385" cy="3130475"/>
+          <a:off x="4448735" y="3079659"/>
+          <a:ext cx="8912460" cy="2961003"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1468,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1495,7 +1485,7 @@
       </c>
       <c r="D1" s="44"/>
     </row>
-    <row r="2" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="135.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1503,12 +1493,12 @@
         <v>6</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D2" s="43"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
@@ -1516,57 +1506,57 @@
         <v>7</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:5" s="17" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" s="46"/>
     </row>
-    <row r="5" spans="1:5" s="17" customFormat="1" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="17" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D5" s="46"/>
     </row>
-    <row r="6" spans="1:5" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="42"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="45"/>
+    </row>
+    <row r="7" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="45"/>
+        <v>38</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="42"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
@@ -1575,86 +1565,60 @@
       <c r="B8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="45"/>
+    </row>
+    <row r="9" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="45"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="42"/>
+    </row>
+    <row r="10" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="45"/>
-    </row>
-    <row r="11" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>55</v>
+        <v>122</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="42"/>
+    </row>
+    <row r="11" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>53</v>
+        <v>191</v>
       </c>
       <c r="D11" s="42"/>
     </row>
-    <row r="12" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="D13" s="42"/>
-    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
+  <mergeCells count="11">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1663,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1678,17 +1642,17 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="35" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
@@ -1696,13 +1660,13 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="32" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E6" s="32" t="s">
         <v>4</v>
@@ -1710,149 +1674,210 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="37" t="s">
+        <v>205</v>
+      </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="37"/>
+        <v>164</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>205</v>
+      </c>
       <c r="E8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C9" s="36">
         <v>2</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="E9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C10" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="37" t="s">
+        <v>204</v>
+      </c>
       <c r="E10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="D11" s="37"/>
+        <v>175</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>204</v>
+      </c>
       <c r="E11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C12" s="36">
         <v>2</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="E12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C13" s="36">
         <v>2021</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="E13" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C14" s="36">
         <v>2030</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C15" s="38" t="b">
         <v>0</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" t="s">
+        <v>202</v>
+      </c>
       <c r="E15" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C16" s="38" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" t="s">
+        <v>202</v>
+      </c>
       <c r="E16" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C17" s="25">
         <v>0.1</v>
       </c>
+      <c r="D17" s="36" t="s">
+        <v>206</v>
+      </c>
       <c r="E17" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C18" s="34">
         <v>3.67</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="34" t="s">
+        <v>206</v>
+      </c>
       <c r="E18" t="s">
-        <v>190</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C15:C16">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:C20">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -1861,7 +1886,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C19:C20" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
@@ -1919,7 +1944,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>11</v>
@@ -1978,28 +2003,28 @@
     <row r="3" spans="1:18" s="31" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="29"/>
       <c r="B3" s="30" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J3" s="30" t="s">
         <v>16</v>
@@ -2026,7 +2051,7 @@
         <v>30</v>
       </c>
       <c r="R3" s="30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
@@ -2034,10 +2059,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(B4,":",C4)</f>
@@ -2050,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2063,7 +2088,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
@@ -2071,10 +2096,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D12" si="0">_xlfn.CONCAT(B5,":",C5)</f>
@@ -2087,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2100,7 +2125,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -2108,23 +2133,23 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Residues:FI</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2136,7 +2161,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="R6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -2144,10 +2169,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7" si="1">_xlfn.CONCAT(B7,":",C7)</f>
@@ -2160,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2172,7 +2197,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2180,23 +2205,23 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2208,7 +2233,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2216,23 +2241,23 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>Furniture:FI</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -2244,7 +2269,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -2252,7 +2277,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -2268,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2280,7 +2305,7 @@
         <v>0.81899999999999995</v>
       </c>
       <c r="R10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -2288,7 +2313,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -2304,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2316,7 +2341,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -2324,23 +2349,23 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>Incineration:FI</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -2352,7 +2377,7 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2384,7 +2409,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2487,7 +2512,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -2496,7 +2521,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -2505,61 +2530,61 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>157</v>
-      </c>
       <c r="K3" s="20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>26</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="S3" s="23" t="s">
         <v>21</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="U3" s="23" t="s">
         <v>21</v>
@@ -2567,27 +2592,27 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C4" t="str">
         <f>+_xlfn.XLOOKUP(H4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Source</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F4" t="str">
         <f>+_xlfn.XLOOKUP(I4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H4" s="4" t="str">
         <f t="shared" ref="H4:H13" si="0">_xlfn.CONCAT(B4,":",D4)</f>
@@ -2601,45 +2626,45 @@
         <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L4">
         <v>2021</v>
       </c>
       <c r="N4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P4">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C5" t="str">
         <f>+_xlfn.XLOOKUP(H5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F5" t="str">
         <f>+_xlfn.XLOOKUP(I5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2659,39 +2684,39 @@
         <v>2021</v>
       </c>
       <c r="N5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P5">
         <f>0.4238*'Carbon fraction (will be moved)'!C2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C6" t="str">
         <f>+_xlfn.XLOOKUP(H6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
         <v>63</v>
-      </c>
-      <c r="E6" t="s">
-        <v>69</v>
       </c>
       <c r="F6" t="str">
         <f>+_xlfn.XLOOKUP(I6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>by_prod</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2705,45 +2730,45 @@
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L6">
         <v>2021</v>
       </c>
       <c r="N6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P6">
         <f>0.395*'Carbon fraction (will be moved)'!C2</f>
         <v>0.18959999999999999</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C7" t="str">
         <f>+_xlfn.XLOOKUP(H7,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F7" t="str">
         <f>+_xlfn.XLOOKUP(I7,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2763,39 +2788,39 @@
         <v>2021</v>
       </c>
       <c r="N7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P7">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
       <c r="Q7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C8" t="str">
         <f>+_xlfn.XLOOKUP(H8,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F8" t="str">
         <f>+_xlfn.XLOOKUP(I8,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H8" s="4" t="str">
         <f>_xlfn.CONCAT(B8,":",D8)</f>
@@ -2815,39 +2840,39 @@
         <v>2021</v>
       </c>
       <c r="N8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P8">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C9" t="str">
         <f>+_xlfn.XLOOKUP(H9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F9" t="str">
         <f>+_xlfn.XLOOKUP(I9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2867,39 +2892,39 @@
         <v>2021</v>
       </c>
       <c r="N9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P9">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
       <c r="Q9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C10" t="str">
         <f>+_xlfn.XLOOKUP(H10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F10" t="str">
         <f>+_xlfn.XLOOKUP(I10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2919,38 +2944,38 @@
         <v>2021</v>
       </c>
       <c r="N10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P10">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F11" t="str">
         <f>+_xlfn.XLOOKUP(I11,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2970,32 +2995,32 @@
         <v>2021</v>
       </c>
       <c r="N11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P11">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C12" t="str">
         <f>+_xlfn.XLOOKUP(H12,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F12" t="str">
         <f>+_xlfn.XLOOKUP(I12,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
@@ -3016,28 +3041,28 @@
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L12">
         <v>2021</v>
       </c>
       <c r="N12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P12">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C13" t="str">
         <f>+_xlfn.XLOOKUP(H13,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
@@ -3047,13 +3072,13 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3067,20 +3092,20 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L13">
         <v>2021</v>
       </c>
       <c r="N13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P13">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q13" s="24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
@@ -3189,7 +3214,7 @@
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.35">
       <c r="E35" s="24" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3537,11 +3562,12 @@
     <hyperlink ref="Q4" r:id="rId1" xr:uid="{44BDC3E8-14C2-47A6-9A94-576E28D9D557}"/>
     <hyperlink ref="Q11:Q13" r:id="rId2" display="https://doi.org/10.1016/j.resconrec.2024.107476, assumed average conversion factor 80% soft 20% hard" xr:uid="{09224BB8-3720-400B-909A-BF395F73FAE2}"/>
     <hyperlink ref="Q13" r:id="rId3" xr:uid="{3D605790-367C-4E01-9AE5-AEF809643374}"/>
+    <hyperlink ref="E35" r:id="rId4" location="json=TH95eCDBsN1pfqczsMf84,S3TGIZvZiI-AUl8oZJcUYg" xr:uid="{26F0F99B-4281-4D67-B3C8-B1BC12D732B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3549,8 +3575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E839B9F-9E6A-42D1-BF39-12023C14C5F8}">
   <dimension ref="A1:AG102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3570,21 +3596,21 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="X1" s="32" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AD1" s="32" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2">
@@ -3618,43 +3644,43 @@
         <v>2030</v>
       </c>
       <c r="N2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="P2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="Q2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="S2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="X2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG2" t="s">
         <v>110</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>202</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.35">
@@ -3710,13 +3736,13 @@
         <v>2021</v>
       </c>
       <c r="X3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA3">
         <v>60</v>
@@ -3728,7 +3754,7 @@
         <v>2021</v>
       </c>
       <c r="AE3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -3790,13 +3816,13 @@
         <v>2021</v>
       </c>
       <c r="X4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA4">
         <v>50</v>
@@ -3808,7 +3834,7 @@
         <v>2021</v>
       </c>
       <c r="AE4" s="32" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF4">
         <v>60</v>
@@ -3870,13 +3896,13 @@
         <v>2021</v>
       </c>
       <c r="X5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA5">
         <v>10</v>
@@ -3888,7 +3914,7 @@
         <v>2021</v>
       </c>
       <c r="AE5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF5">
         <v>10</v>
@@ -3950,13 +3976,13 @@
         <v>2021</v>
       </c>
       <c r="X6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA6">
         <v>24</v>
@@ -3968,7 +3994,7 @@
         <v>2021</v>
       </c>
       <c r="AE6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF6">
         <v>60</v>
@@ -4030,13 +4056,13 @@
         <v>2021</v>
       </c>
       <c r="X7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y7" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z7" t="s">
         <v>95</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>101</v>
       </c>
       <c r="AA7">
         <v>16</v>
@@ -4048,7 +4074,7 @@
         <v>2021</v>
       </c>
       <c r="AE7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF7">
         <v>24</v>
@@ -4110,13 +4136,13 @@
         <v>2021</v>
       </c>
       <c r="X8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA8">
         <v>0</v>
@@ -4128,7 +4154,7 @@
         <v>2021</v>
       </c>
       <c r="AE8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF8">
         <v>16</v>
@@ -4190,13 +4216,13 @@
         <v>2021</v>
       </c>
       <c r="X9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -4208,7 +4234,7 @@
         <v>2021</v>
       </c>
       <c r="AE9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF9">
         <v>0</v>
@@ -4270,13 +4296,13 @@
         <v>2021</v>
       </c>
       <c r="X10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA10">
         <v>0</v>
@@ -4288,7 +4314,7 @@
         <v>2021</v>
       </c>
       <c r="AE10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF10">
         <v>20</v>
@@ -4350,13 +4376,13 @@
         <v>2021</v>
       </c>
       <c r="X11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA11">
         <v>20</v>
@@ -4368,7 +4394,7 @@
         <v>2021</v>
       </c>
       <c r="AE11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF11">
         <v>0</v>
@@ -4430,13 +4456,13 @@
         <v>2021</v>
       </c>
       <c r="X12" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA12">
         <v>10</v>
@@ -4448,7 +4474,7 @@
         <v>2022</v>
       </c>
       <c r="AE12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF12">
         <v>0</v>
@@ -4459,19 +4485,19 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C13" s="32" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="W13">
         <v>2022</v>
       </c>
       <c r="X13" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA13">
         <v>10</v>
@@ -4483,7 +4509,7 @@
         <v>2022</v>
       </c>
       <c r="AE13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF13">
         <v>60</v>
@@ -4528,13 +4554,13 @@
         <v>2022</v>
       </c>
       <c r="X14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y14" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA14">
         <v>20</v>
@@ -4546,7 +4572,7 @@
         <v>2022</v>
       </c>
       <c r="AE14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF14">
         <v>10</v>
@@ -4594,13 +4620,13 @@
         <v>2022</v>
       </c>
       <c r="X15" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA15">
         <v>5.1000000000000004E-4</v>
@@ -4612,7 +4638,7 @@
         <v>2022</v>
       </c>
       <c r="AE15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF15">
         <v>60</v>
@@ -4659,13 +4685,13 @@
         <v>2022</v>
       </c>
       <c r="X16" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z16" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA16">
         <v>0</v>
@@ -4677,7 +4703,7 @@
         <v>2022</v>
       </c>
       <c r="AE16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF16">
         <v>24</v>
@@ -4724,13 +4750,13 @@
         <v>2022</v>
       </c>
       <c r="X17" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z17" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA17">
         <v>0</v>
@@ -4742,7 +4768,7 @@
         <v>2022</v>
       </c>
       <c r="AE17" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF17">
         <v>16</v>
@@ -4789,13 +4815,13 @@
         <v>2022</v>
       </c>
       <c r="X18" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y18" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z18" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA18">
         <v>10</v>
@@ -4807,7 +4833,7 @@
         <v>2022</v>
       </c>
       <c r="AE18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF18">
         <v>0</v>
@@ -4854,13 +4880,13 @@
         <v>2022</v>
       </c>
       <c r="X19" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y19" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z19" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA19">
         <v>24</v>
@@ -4872,7 +4898,7 @@
         <v>2022</v>
       </c>
       <c r="AE19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF19">
         <v>20</v>
@@ -4919,13 +4945,13 @@
         <v>2022</v>
       </c>
       <c r="X20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z20" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA20">
         <v>50</v>
@@ -4937,7 +4963,7 @@
         <v>2022</v>
       </c>
       <c r="AE20" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF20">
         <v>5.1000000000000004E-4</v>
@@ -4984,13 +5010,13 @@
         <v>2022</v>
       </c>
       <c r="X21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z21" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA21">
         <v>60</v>
@@ -5002,7 +5028,7 @@
         <v>2023</v>
       </c>
       <c r="AE21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF21">
         <v>0</v>
@@ -5050,13 +5076,13 @@
         <v>2022</v>
       </c>
       <c r="X22" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y22" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z22" t="s">
         <v>95</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>101</v>
       </c>
       <c r="AA22">
         <v>16</v>
@@ -5068,7 +5094,7 @@
         <v>2023</v>
       </c>
       <c r="AE22" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF22">
         <v>60</v>
@@ -5115,13 +5141,13 @@
         <v>2023</v>
       </c>
       <c r="X23" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z23" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -5133,7 +5159,7 @@
         <v>2023</v>
       </c>
       <c r="AE23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF23">
         <v>10</v>
@@ -5180,13 +5206,13 @@
         <v>2023</v>
       </c>
       <c r="X24" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y24" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z24" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA24">
         <v>10</v>
@@ -5198,7 +5224,7 @@
         <v>2023</v>
       </c>
       <c r="AE24" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF24">
         <v>60</v>
@@ -5209,19 +5235,19 @@
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C25" s="32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="W25">
         <v>2023</v>
       </c>
       <c r="X25" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y25" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z25" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA25">
         <v>20</v>
@@ -5233,7 +5259,7 @@
         <v>2023</v>
       </c>
       <c r="AE25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF25">
         <v>24</v>
@@ -5278,13 +5304,13 @@
         <v>2023</v>
       </c>
       <c r="X26" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z26" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA26">
         <v>2.1600000000000001E-2</v>
@@ -5296,7 +5322,7 @@
         <v>2023</v>
       </c>
       <c r="AE26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF26">
         <v>16</v>
@@ -5344,13 +5370,13 @@
         <v>2023</v>
       </c>
       <c r="X27" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y27" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z27" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA27">
         <v>0</v>
@@ -5362,7 +5388,7 @@
         <v>2023</v>
       </c>
       <c r="AE27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF27">
         <v>0</v>
@@ -5410,13 +5436,13 @@
         <v>2023</v>
       </c>
       <c r="X28" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y28" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z28" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA28">
         <v>50</v>
@@ -5428,7 +5454,7 @@
         <v>2023</v>
       </c>
       <c r="AE28" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF28">
         <v>20</v>
@@ -5476,13 +5502,13 @@
         <v>2023</v>
       </c>
       <c r="X29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y29" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z29" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA29">
         <v>24</v>
@@ -5494,7 +5520,7 @@
         <v>2023</v>
       </c>
       <c r="AE29" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF29">
         <v>2.1600000000000001E-2</v>
@@ -5542,13 +5568,13 @@
         <v>2023</v>
       </c>
       <c r="X30" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y30" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA30">
         <v>10</v>
@@ -5560,7 +5586,7 @@
         <v>2024</v>
       </c>
       <c r="AE30" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF30">
         <v>0</v>
@@ -5608,13 +5634,13 @@
         <v>2023</v>
       </c>
       <c r="X31" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y31" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA31">
         <v>60</v>
@@ -5626,7 +5652,7 @@
         <v>2024</v>
       </c>
       <c r="AE31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF31">
         <v>60</v>
@@ -5674,13 +5700,13 @@
         <v>2023</v>
       </c>
       <c r="X32" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y32" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z32" t="s">
         <v>95</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>101</v>
       </c>
       <c r="AA32">
         <v>16</v>
@@ -5692,7 +5718,7 @@
         <v>2024</v>
       </c>
       <c r="AE32" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF32">
         <v>10</v>
@@ -5740,13 +5766,13 @@
         <v>2024</v>
       </c>
       <c r="X33" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y33" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA33">
         <v>10</v>
@@ -5758,7 +5784,7 @@
         <v>2024</v>
       </c>
       <c r="AE33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF33">
         <v>60</v>
@@ -5806,13 +5832,13 @@
         <v>2024</v>
       </c>
       <c r="X34" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y34" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z34" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA34">
         <v>20</v>
@@ -5824,7 +5850,7 @@
         <v>2024</v>
       </c>
       <c r="AE34" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF34">
         <v>24</v>
@@ -5872,13 +5898,13 @@
         <v>2024</v>
       </c>
       <c r="X35" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y35" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z35" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA35">
         <v>0.36399999999999999</v>
@@ -5890,7 +5916,7 @@
         <v>2024</v>
       </c>
       <c r="AE35" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF35">
         <v>16</v>
@@ -5938,13 +5964,13 @@
         <v>2024</v>
       </c>
       <c r="X36" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y36" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z36" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA36">
         <v>0</v>
@@ -5956,7 +5982,7 @@
         <v>2024</v>
       </c>
       <c r="AE36" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF36">
         <v>0</v>
@@ -5967,19 +5993,19 @@
     </row>
     <row r="37" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C37" s="32" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="W37">
         <v>2024</v>
       </c>
       <c r="X37" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y37" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z37" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA37">
         <v>0</v>
@@ -5991,7 +6017,7 @@
         <v>2024</v>
       </c>
       <c r="AE37" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF37">
         <v>20</v>
@@ -6036,13 +6062,13 @@
         <v>2024</v>
       </c>
       <c r="X38" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y38" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z38" t="s">
         <v>95</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>101</v>
       </c>
       <c r="AA38">
         <v>16</v>
@@ -6054,7 +6080,7 @@
         <v>2024</v>
       </c>
       <c r="AE38" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF38">
         <v>0.36399999999999999</v>
@@ -6101,13 +6127,13 @@
         <v>2024</v>
       </c>
       <c r="X39" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y39" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z39" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA39">
         <v>10</v>
@@ -6119,7 +6145,7 @@
         <v>2025</v>
       </c>
       <c r="AE39" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF39">
         <v>0</v>
@@ -6166,13 +6192,13 @@
         <v>2024</v>
       </c>
       <c r="X40" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y40" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z40" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA40">
         <v>50</v>
@@ -6184,7 +6210,7 @@
         <v>2025</v>
       </c>
       <c r="AE40" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF40">
         <v>60</v>
@@ -6231,13 +6257,13 @@
         <v>2024</v>
       </c>
       <c r="X41" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y41" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z41" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA41">
         <v>60</v>
@@ -6249,7 +6275,7 @@
         <v>2025</v>
       </c>
       <c r="AE41" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF41">
         <v>10</v>
@@ -6296,13 +6322,13 @@
         <v>2024</v>
       </c>
       <c r="X42" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y42" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z42" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA42">
         <v>24</v>
@@ -6314,7 +6340,7 @@
         <v>2025</v>
       </c>
       <c r="AE42" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF42">
         <v>60</v>
@@ -6361,13 +6387,13 @@
         <v>2025</v>
       </c>
       <c r="X43" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y43" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z43" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA43">
         <v>0</v>
@@ -6379,7 +6405,7 @@
         <v>2025</v>
       </c>
       <c r="AE43" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF43">
         <v>24</v>
@@ -6426,13 +6452,13 @@
         <v>2025</v>
       </c>
       <c r="X44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y44" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z44" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA44">
         <v>20</v>
@@ -6444,7 +6470,7 @@
         <v>2025</v>
       </c>
       <c r="AE44" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF44">
         <v>16</v>
@@ -6491,13 +6517,13 @@
         <v>2025</v>
       </c>
       <c r="X45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y45" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z45" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA45">
         <v>2.5384799999999998</v>
@@ -6509,7 +6535,7 @@
         <v>2025</v>
       </c>
       <c r="AE45" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF45">
         <v>0</v>
@@ -6556,13 +6582,13 @@
         <v>2025</v>
       </c>
       <c r="X46" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y46" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z46" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA46">
         <v>0</v>
@@ -6574,7 +6600,7 @@
         <v>2025</v>
       </c>
       <c r="AE46" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF46">
         <v>20</v>
@@ -6621,13 +6647,13 @@
         <v>2025</v>
       </c>
       <c r="X47" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y47" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z47" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA47">
         <v>10</v>
@@ -6639,7 +6665,7 @@
         <v>2025</v>
       </c>
       <c r="AE47" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF47">
         <v>2.5384799999999998</v>
@@ -6686,13 +6712,13 @@
         <v>2025</v>
       </c>
       <c r="X48" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y48" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z48" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA48">
         <v>24</v>
@@ -6704,7 +6730,7 @@
         <v>2026</v>
       </c>
       <c r="AE48" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF48">
         <v>0</v>
@@ -6718,13 +6744,13 @@
         <v>2025</v>
       </c>
       <c r="X49" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y49" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z49" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA49">
         <v>10</v>
@@ -6736,7 +6762,7 @@
         <v>2026</v>
       </c>
       <c r="AE49" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF49">
         <v>60</v>
@@ -6750,13 +6776,13 @@
         <v>2025</v>
       </c>
       <c r="X50" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y50" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z50" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA50">
         <v>50</v>
@@ -6768,7 +6794,7 @@
         <v>2026</v>
       </c>
       <c r="AE50" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF50">
         <v>10</v>
@@ -6782,13 +6808,13 @@
         <v>2025</v>
       </c>
       <c r="X51" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y51" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z51" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA51">
         <v>60</v>
@@ -6800,7 +6826,7 @@
         <v>2026</v>
       </c>
       <c r="AE51" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF51">
         <v>60</v>
@@ -6814,13 +6840,13 @@
         <v>2025</v>
       </c>
       <c r="X52" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y52" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z52" t="s">
         <v>95</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>101</v>
       </c>
       <c r="AA52">
         <v>16</v>
@@ -6832,7 +6858,7 @@
         <v>2026</v>
       </c>
       <c r="AE52" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF52">
         <v>24</v>
@@ -6846,13 +6872,13 @@
         <v>2026</v>
       </c>
       <c r="X53" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y53" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z53" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA53">
         <v>20</v>
@@ -6864,7 +6890,7 @@
         <v>2026</v>
       </c>
       <c r="AE53" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF53">
         <v>16</v>
@@ -6878,13 +6904,13 @@
         <v>2026</v>
       </c>
       <c r="X54" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y54" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z54" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA54">
         <v>8</v>
@@ -6896,7 +6922,7 @@
         <v>2026</v>
       </c>
       <c r="AE54" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF54">
         <v>0</v>
@@ -6910,13 +6936,13 @@
         <v>2026</v>
       </c>
       <c r="X55" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y55" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z55" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA55">
         <v>0</v>
@@ -6928,7 +6954,7 @@
         <v>2026</v>
       </c>
       <c r="AE55" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF55">
         <v>20</v>
@@ -6942,13 +6968,13 @@
         <v>2026</v>
       </c>
       <c r="X56" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y56" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z56" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA56">
         <v>0</v>
@@ -6960,7 +6986,7 @@
         <v>2026</v>
       </c>
       <c r="AE56" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF56">
         <v>8</v>
@@ -6974,13 +7000,13 @@
         <v>2026</v>
       </c>
       <c r="X57" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y57" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z57" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA57">
         <v>10</v>
@@ -6992,7 +7018,7 @@
         <v>2027</v>
       </c>
       <c r="AE57" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF57">
         <v>0</v>
@@ -7006,13 +7032,13 @@
         <v>2026</v>
       </c>
       <c r="X58" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y58" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z58" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA58">
         <v>24</v>
@@ -7024,7 +7050,7 @@
         <v>2027</v>
       </c>
       <c r="AE58" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF58">
         <v>60.000300000000003</v>
@@ -7038,13 +7064,13 @@
         <v>2026</v>
       </c>
       <c r="X59" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y59" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z59" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA59">
         <v>10</v>
@@ -7056,7 +7082,7 @@
         <v>2027</v>
       </c>
       <c r="AE59" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF59">
         <v>10</v>
@@ -7070,13 +7096,13 @@
         <v>2026</v>
       </c>
       <c r="X60" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y60" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z60" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA60">
         <v>50</v>
@@ -7088,7 +7114,7 @@
         <v>2027</v>
       </c>
       <c r="AE60" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF60">
         <v>60.000300000000003</v>
@@ -7102,13 +7128,13 @@
         <v>2026</v>
       </c>
       <c r="X61" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y61" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z61" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA61">
         <v>60</v>
@@ -7120,7 +7146,7 @@
         <v>2027</v>
       </c>
       <c r="AE61" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF61">
         <v>24.00018</v>
@@ -7134,13 +7160,13 @@
         <v>2026</v>
       </c>
       <c r="X62" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y62" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z62" t="s">
         <v>95</v>
-      </c>
-      <c r="Z62" t="s">
-        <v>101</v>
       </c>
       <c r="AA62">
         <v>16</v>
@@ -7152,7 +7178,7 @@
         <v>2027</v>
       </c>
       <c r="AE62" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF62">
         <v>16.000119999999999</v>
@@ -7166,13 +7192,13 @@
         <v>2027</v>
       </c>
       <c r="X63" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y63" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z63" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA63">
         <v>10</v>
@@ -7184,7 +7210,7 @@
         <v>2027</v>
       </c>
       <c r="AE63" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF63">
         <v>0</v>
@@ -7198,13 +7224,13 @@
         <v>2027</v>
       </c>
       <c r="X64" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y64" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z64" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA64">
         <v>20</v>
@@ -7216,7 +7242,7 @@
         <v>2027</v>
       </c>
       <c r="AE64" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF64">
         <v>20</v>
@@ -7230,13 +7256,13 @@
         <v>2027</v>
       </c>
       <c r="X65" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y65" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z65" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA65">
         <v>13.46152</v>
@@ -7248,7 +7274,7 @@
         <v>2027</v>
       </c>
       <c r="AE65" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF65">
         <v>13.461970000000001</v>
@@ -7262,13 +7288,13 @@
         <v>2027</v>
       </c>
       <c r="X66" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y66" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z66" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA66">
         <v>4.6000000000000001E-4</v>
@@ -7280,7 +7306,7 @@
         <v>2028</v>
       </c>
       <c r="AE66" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF66">
         <v>0</v>
@@ -7294,13 +7320,13 @@
         <v>2027</v>
       </c>
       <c r="X67" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y67" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z67" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA67">
         <v>2.9999999999999997E-4</v>
@@ -7312,7 +7338,7 @@
         <v>2028</v>
       </c>
       <c r="AE67" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF67">
         <v>60.01296</v>
@@ -7326,13 +7352,13 @@
         <v>2027</v>
       </c>
       <c r="X68" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y68" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z68" t="s">
         <v>95</v>
-      </c>
-      <c r="Z68" t="s">
-        <v>101</v>
       </c>
       <c r="AA68">
         <v>16.000119999999999</v>
@@ -7344,7 +7370,7 @@
         <v>2028</v>
       </c>
       <c r="AE68" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF68">
         <v>10</v>
@@ -7358,13 +7384,13 @@
         <v>2027</v>
       </c>
       <c r="X69" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y69" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z69" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA69">
         <v>10</v>
@@ -7376,7 +7402,7 @@
         <v>2028</v>
       </c>
       <c r="AE69" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF69">
         <v>60.01296</v>
@@ -7390,13 +7416,13 @@
         <v>2027</v>
       </c>
       <c r="X70" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y70" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z70" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA70">
         <v>50.000300000000003</v>
@@ -7408,7 +7434,7 @@
         <v>2028</v>
       </c>
       <c r="AE70" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF70">
         <v>24.00778</v>
@@ -7422,13 +7448,13 @@
         <v>2027</v>
       </c>
       <c r="X71" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y71" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z71" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA71">
         <v>60</v>
@@ -7440,7 +7466,7 @@
         <v>2028</v>
       </c>
       <c r="AE71" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF71">
         <v>16.005179999999999</v>
@@ -7454,13 +7480,13 @@
         <v>2027</v>
       </c>
       <c r="X72" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y72" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z72" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA72">
         <v>24.00018</v>
@@ -7472,7 +7498,7 @@
         <v>2028</v>
       </c>
       <c r="AE72" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF72">
         <v>0</v>
@@ -7486,13 +7512,13 @@
         <v>2028</v>
       </c>
       <c r="X73" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y73" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z73" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA73">
         <v>1.9439999999999999E-2</v>
@@ -7504,7 +7530,7 @@
         <v>2028</v>
       </c>
       <c r="AE73" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF73">
         <v>20</v>
@@ -7518,13 +7544,13 @@
         <v>2028</v>
       </c>
       <c r="X74" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y74" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z74" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA74">
         <v>20</v>
@@ -7536,7 +7562,7 @@
         <v>2028</v>
       </c>
       <c r="AE74" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF74">
         <v>15.65544</v>
@@ -7550,13 +7576,13 @@
         <v>2028</v>
       </c>
       <c r="X75" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y75" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z75" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA75">
         <v>15.635999999999999</v>
@@ -7568,7 +7594,7 @@
         <v>2029</v>
       </c>
       <c r="AE75" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF75">
         <v>0</v>
@@ -7582,13 +7608,13 @@
         <v>2028</v>
       </c>
       <c r="X76" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y76" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z76" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA76">
         <v>10</v>
@@ -7600,7 +7626,7 @@
         <v>2029</v>
       </c>
       <c r="AE76" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF76">
         <v>60.218400000000003</v>
@@ -7614,13 +7640,13 @@
         <v>2028</v>
       </c>
       <c r="X77" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y77" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z77" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA77">
         <v>1.2959999999999999E-2</v>
@@ -7632,7 +7658,7 @@
         <v>2029</v>
       </c>
       <c r="AE77" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF77">
         <v>10</v>
@@ -7646,13 +7672,13 @@
         <v>2028</v>
       </c>
       <c r="X78" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y78" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z78" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA78">
         <v>10</v>
@@ -7664,7 +7690,7 @@
         <v>2029</v>
       </c>
       <c r="AE78" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF78">
         <v>60.218400000000003</v>
@@ -7678,13 +7704,13 @@
         <v>2028</v>
       </c>
       <c r="X79" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y79" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z79" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA79">
         <v>24.00778</v>
@@ -7696,7 +7722,7 @@
         <v>2029</v>
       </c>
       <c r="AE79" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF79">
         <v>24.131039999999999</v>
@@ -7710,13 +7736,13 @@
         <v>2028</v>
       </c>
       <c r="X80" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y80" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z80" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA80">
         <v>50.01296</v>
@@ -7728,7 +7754,7 @@
         <v>2029</v>
       </c>
       <c r="AE80" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF80">
         <v>16.08736</v>
@@ -7742,13 +7768,13 @@
         <v>2028</v>
       </c>
       <c r="X81" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y81" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z81" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA81">
         <v>60</v>
@@ -7760,7 +7786,7 @@
         <v>2029</v>
       </c>
       <c r="AE81" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF81">
         <v>0</v>
@@ -7774,13 +7800,13 @@
         <v>2028</v>
       </c>
       <c r="X82" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y82" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z82" t="s">
         <v>95</v>
-      </c>
-      <c r="Z82" t="s">
-        <v>101</v>
       </c>
       <c r="AA82">
         <v>16.005179999999999</v>
@@ -7792,7 +7818,7 @@
         <v>2029</v>
       </c>
       <c r="AE82" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF82">
         <v>20</v>
@@ -7806,13 +7832,13 @@
         <v>2029</v>
       </c>
       <c r="X83" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y83" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z83" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA83">
         <v>10</v>
@@ -7824,7 +7850,7 @@
         <v>2029</v>
       </c>
       <c r="AE83" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF83">
         <v>16.306000000000001</v>
@@ -7838,13 +7864,13 @@
         <v>2029</v>
       </c>
       <c r="X84" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y84" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z84" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA84">
         <v>20</v>
@@ -7856,7 +7882,7 @@
         <v>2030</v>
       </c>
       <c r="AE84" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AF84">
         <v>0</v>
@@ -7870,13 +7896,13 @@
         <v>2029</v>
       </c>
       <c r="X85" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y85" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z85" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA85">
         <v>0.3276</v>
@@ -7888,7 +7914,7 @@
         <v>2030</v>
       </c>
       <c r="AE85" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AF85">
         <v>61.523090000000003</v>
@@ -7902,13 +7928,13 @@
         <v>2029</v>
       </c>
       <c r="X86" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y86" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z86" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA86">
         <v>0.21840000000000001</v>
@@ -7920,7 +7946,7 @@
         <v>2030</v>
       </c>
       <c r="AE86" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AF86">
         <v>10</v>
@@ -7934,13 +7960,13 @@
         <v>2029</v>
       </c>
       <c r="X87" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y87" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z87" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA87">
         <v>15.978400000000001</v>
@@ -7952,7 +7978,7 @@
         <v>2030</v>
       </c>
       <c r="AE87" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AF87">
         <v>61.523090000000003</v>
@@ -7966,13 +7992,13 @@
         <v>2029</v>
       </c>
       <c r="X88" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y88" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z88" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA88">
         <v>24.131039999999999</v>
@@ -7984,7 +8010,7 @@
         <v>2030</v>
       </c>
       <c r="AE88" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AF88">
         <v>24.91385</v>
@@ -7998,13 +8024,13 @@
         <v>2029</v>
       </c>
       <c r="X89" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y89" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z89" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA89">
         <v>10</v>
@@ -8016,7 +8042,7 @@
         <v>2030</v>
       </c>
       <c r="AE89" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="AF89">
         <v>16.60924</v>
@@ -8030,13 +8056,13 @@
         <v>2029</v>
       </c>
       <c r="X90" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y90" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z90" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA90">
         <v>50.218400000000003</v>
@@ -8048,7 +8074,7 @@
         <v>2030</v>
       </c>
       <c r="AE90" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="AF90">
         <v>0</v>
@@ -8062,13 +8088,13 @@
         <v>2029</v>
       </c>
       <c r="X91" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y91" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z91" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA91">
         <v>60</v>
@@ -8080,7 +8106,7 @@
         <v>2030</v>
       </c>
       <c r="AE91" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AF91">
         <v>20</v>
@@ -8094,13 +8120,13 @@
         <v>2029</v>
       </c>
       <c r="X92" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y92" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z92" t="s">
         <v>95</v>
-      </c>
-      <c r="Z92" t="s">
-        <v>101</v>
       </c>
       <c r="AA92">
         <v>16.08736</v>
@@ -8112,7 +8138,7 @@
         <v>2030</v>
       </c>
       <c r="AE92" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AF92">
         <v>18.284140000000001</v>
@@ -8126,13 +8152,13 @@
         <v>2030</v>
       </c>
       <c r="X93" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="Y93" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z93" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AA93">
         <v>20</v>
@@ -8146,13 +8172,13 @@
         <v>2030</v>
       </c>
       <c r="X94" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Y94" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Z94" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA94">
         <v>60</v>
@@ -8166,13 +8192,13 @@
         <v>2030</v>
       </c>
       <c r="X95" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Y95" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z95" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA95">
         <v>51.523090000000003</v>
@@ -8186,13 +8212,13 @@
         <v>2030</v>
       </c>
       <c r="X96" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Y96" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Z96" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AA96">
         <v>10</v>
@@ -8206,13 +8232,13 @@
         <v>2030</v>
       </c>
       <c r="X97" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Y97" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Z97" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="AA97">
         <v>24.91385</v>
@@ -8226,13 +8252,13 @@
         <v>2030</v>
       </c>
       <c r="X98" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Y98" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z98" t="s">
         <v>95</v>
-      </c>
-      <c r="Z98" t="s">
-        <v>101</v>
       </c>
       <c r="AA98">
         <v>16.60924</v>
@@ -8246,13 +8272,13 @@
         <v>2030</v>
       </c>
       <c r="X99" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Y99" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z99" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA99">
         <v>1.5230900000000001</v>
@@ -8266,13 +8292,13 @@
         <v>2030</v>
       </c>
       <c r="X100" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="Y100" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z100" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA100">
         <v>2.28464</v>
@@ -8286,13 +8312,13 @@
         <v>2030</v>
       </c>
       <c r="X101" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="Y101" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Z101" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AA101">
         <v>15.999510000000001</v>
@@ -8306,13 +8332,13 @@
         <v>2030</v>
       </c>
       <c r="X102" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="Y102" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Z102" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AA102">
         <v>10</v>
@@ -8348,13 +8374,13 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>0.48</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -8379,15 +8405,15 @@
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C1" s="32" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -8395,7 +8421,7 @@
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -8403,17 +8429,17 @@
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -8685,6 +8711,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
@@ -8694,15 +8729,6 @@
     <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8725,6 +8751,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -8739,12 +8773,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated example_data.xlsx to include simple decay function
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6666BAD6-E259-4FEE-A971-DD6056DBEE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2658169B-D7C9-4FC4-8430-F24756A243BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$B$3:$M$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$U$14</definedName>
     <definedName name="Boolean">Sheet1!$D$2:$D$3</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="219">
   <si>
     <t>Years</t>
   </si>
@@ -777,6 +777,39 @@
   </si>
   <si>
     <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from Settings. </t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chair </t>
+  </si>
+  <si>
+    <t>Recycle</t>
+  </si>
+  <si>
+    <t>fill_method</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Interpolate</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeros </t>
+  </si>
+  <si>
+    <t>Simple</t>
   </si>
 </sst>
 </file>
@@ -940,7 +973,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1023,6 +1056,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1103,7 +1141,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>575283</xdr:colOff>
+      <xdr:colOff>581633</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>45515</xdr:rowOff>
     </xdr:to>
@@ -1460,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -1480,10 +1518,10 @@
       <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="44"/>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:5" ht="135.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -1492,10 +1530,10 @@
       <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1505,10 +1543,10 @@
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:5" s="17" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
@@ -1517,10 +1555,10 @@
       <c r="B4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:5" s="17" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40" t="s">
@@ -1529,10 +1567,10 @@
       <c r="B5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
@@ -1541,10 +1579,10 @@
       <c r="B6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="48"/>
     </row>
     <row r="7" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
@@ -1553,10 +1591,10 @@
       <c r="B7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="42"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
@@ -1565,10 +1603,10 @@
       <c r="B8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="45"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
@@ -1577,10 +1615,10 @@
       <c r="B9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="45"/>
     </row>
     <row r="10" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
@@ -1589,10 +1627,10 @@
       <c r="B10" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="42"/>
+      <c r="D10" s="45"/>
     </row>
     <row r="11" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
@@ -1601,10 +1639,10 @@
       <c r="B11" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="42"/>
+      <c r="D11" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1627,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1866,6 +1904,17 @@
       </c>
       <c r="E20" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1891,6 +1940,18 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A95900C-A9EB-48AB-A762-0F120DA62856}">
+          <x14:formula1>
+            <xm:f>Sheet1!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1898,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2102,7 +2163,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D5:D12" si="0">_xlfn.CONCAT(B5,":",C5)</f>
+        <f t="shared" ref="D5:D15" si="0">_xlfn.CONCAT(B5,":",C5)</f>
         <v>Sawmilling:FI</v>
       </c>
       <c r="E5" t="s">
@@ -2221,7 +2282,7 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>218</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2257,7 +2318,7 @@
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>218</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -2380,10 +2441,91 @@
         <v>80</v>
       </c>
     </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Chair:FI</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Table:FI</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Recycle:FI</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>211</v>
+      </c>
+    </row>
     <row r="18" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations xWindow="558" yWindow="395" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameter" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I4:I1048576" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sankey diagram positioning" prompt="Sankey diagram X and Y node positioning. Check / adjust positioning after you run case and see coordinates. " sqref="P4:Q1048576 Q2" xr:uid="{167D7519-74A2-4731-8D99-C2A980321CC9}"/>
   </dataValidations>
@@ -2391,12 +2533,18 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="558" yWindow="395" count="2">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{0258C8E4-0AAB-48FF-93D5-AADF99BF39C4}">
           <x14:formula1>
             <xm:f>Sheet1!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:H1048576</xm:sqref>
+          <xm:sqref>H16:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{61770E9E-9EFD-4B63-8C83-80C1E833E691}">
+          <x14:formula1>
+            <xm:f>Sheet1!$C$2:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>H4:H15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2409,7 +2557,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2798,7 +2946,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -2850,107 +2998,109 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="28" t="str">
         <f>+_xlfn.XLOOKUP(H9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F9" s="28" t="str">
         <f>+_xlfn.XLOOKUP(I9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="4" t="str">
+      <c r="H9" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I9" s="4" t="str">
+      <c r="I9" s="42" t="str">
         <f t="shared" si="1"/>
         <v>Sawmilling:FI</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="28">
         <v>40</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="28">
         <v>2021</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="P9">
+      <c r="O9" s="43"/>
+      <c r="P9" s="28">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:21" s="28" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="28" t="str">
         <f>+_xlfn.XLOOKUP(H10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F10" s="28" t="str">
         <f>+_xlfn.XLOOKUP(I10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="4" t="str">
+      <c r="H10" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I10" s="4" t="str">
+      <c r="I10" s="42" t="str">
         <f t="shared" si="1"/>
         <v>Incineration:FI</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="28">
         <v>60</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="28">
         <v>2021</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="P10">
+      <c r="O10" s="43"/>
+      <c r="P10" s="28">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="28" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3074,8 +3224,9 @@
       <c r="E13" t="s">
         <v>59</v>
       </c>
-      <c r="F13" t="s">
-        <v>25</v>
+      <c r="F13" t="str">
+        <f>+_xlfn.XLOOKUP(I13,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
+        <v>Second</v>
       </c>
       <c r="G13" t="s">
         <v>57</v>
@@ -3108,11 +3259,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="N14"/>
-      <c r="Q14" s="24"/>
+    <row r="14" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="O14" s="43"/>
+      <c r="Q14" s="44"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="H15" s="4"/>
@@ -3557,6 +3708,7 @@
       <c r="O91"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:U14" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1" xr:uid="{44BDC3E8-14C2-47A6-9A94-576E28D9D557}"/>
@@ -8390,10 +8542,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
-  <dimension ref="C1:D6"/>
+  <dimension ref="C1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8403,51 +8555,93 @@
     <col min="11" max="11" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C1" s="32" t="s">
         <v>194</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>140</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>68</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>142</v>
       </c>
     </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -8710,28 +8904,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8748,29 +8946,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implemented target value functionality to flow modifiers. Updated settings to example_data.xlsx.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2658169B-D7C9-4FC4-8430-F24756A243BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F772D17-35DC-4B39-AC03-C3949F0C65E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Readme" sheetId="4" r:id="rId1"/>
-    <sheet name="Settings" sheetId="11" r:id="rId2"/>
+    <sheet name="Settings" sheetId="11" r:id="rId1"/>
+    <sheet name="Readme" sheetId="4" r:id="rId2"/>
     <sheet name="Processes" sheetId="6" r:id="rId3"/>
     <sheet name="Flows" sheetId="1" r:id="rId4"/>
-    <sheet name="DMFA results (example)" sheetId="8" r:id="rId5"/>
-    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
+    <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
+    <sheet name="DMFA results (example)" sheetId="8" r:id="rId6"/>
+    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$U$14</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="237">
   <si>
     <t>Years</t>
   </si>
@@ -810,6 +811,104 @@
   </si>
   <si>
     <t>Simple</t>
+  </si>
+  <si>
+    <t>sheet_name_scenarios</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Sheet name that contains scenarios (flow variations)</t>
+  </si>
+  <si>
+    <t>create_network_graphs</t>
+  </si>
+  <si>
+    <t>Create network graphs to visualize process connections for each scenario</t>
+  </si>
+  <si>
+    <t>create_sankey_charts</t>
+  </si>
+  <si>
+    <t>Create Sankey charts for each scenario</t>
+  </si>
+  <si>
+    <t>Scenario name</t>
+  </si>
+  <si>
+    <t>Source process ID</t>
+  </si>
+  <si>
+    <t>Target process ID</t>
+  </si>
+  <si>
+    <t>Change in value (delta)</t>
+  </si>
+  <si>
+    <t>Target value (potentially)</t>
+  </si>
+  <si>
+    <t>Change type (Value or % = proportional)</t>
+  </si>
+  <si>
+    <t>Start year (included)</t>
+  </si>
+  <si>
+    <t>End year (included)</t>
+  </si>
+  <si>
+    <t>Function type</t>
+  </si>
+  <si>
+    <t>Target process ID (where the opposite change is applied)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fill method if either </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fill_missing_absolute_flows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fill_missing_relative_flows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is enabled</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -887,7 +986,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -915,6 +1014,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -973,7 +1078,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1076,12 +1181,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1495,23 +1616,369 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
+  <dimension ref="B2:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="103.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="36">
+        <v>2</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="E11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="36">
+        <v>2</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="36">
+        <v>2021</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="36">
+        <v>2030</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="E17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="34">
+        <v>3.67</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C15:C16">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:C20">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:C24">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C19:C20 C23:C24" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
+      <formula1>Boolean</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A95900C-A9EB-48AB-A762-0F120DA62856}">
+          <x14:formula1>
+            <xm:f>Sheet1!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="18" customWidth="1"/>
     <col min="3" max="3" width="29" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="16"/>
+    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1523,7 +1990,7 @@
       </c>
       <c r="D1" s="47"/>
     </row>
-    <row r="2" spans="1:5" ht="135.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1536,7 +2003,7 @@
       <c r="D2" s="46"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
@@ -1548,7 +2015,7 @@
       </c>
       <c r="D3" s="46"/>
     </row>
-    <row r="4" spans="1:5" s="17" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="17" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>35</v>
       </c>
@@ -1560,7 +2027,7 @@
       </c>
       <c r="D4" s="49"/>
     </row>
-    <row r="5" spans="1:5" s="17" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="17" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>44</v>
       </c>
@@ -1572,7 +2039,7 @@
       </c>
       <c r="D5" s="49"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
@@ -1584,7 +2051,7 @@
       </c>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
@@ -1596,7 +2063,7 @@
       </c>
       <c r="D7" s="45"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>40</v>
       </c>
@@ -1608,7 +2075,7 @@
       </c>
       <c r="D8" s="48"/>
     </row>
-    <row r="9" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>49</v>
       </c>
@@ -1620,7 +2087,7 @@
       </c>
       <c r="D9" s="45"/>
     </row>
-    <row r="10" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>118</v>
       </c>
@@ -1632,7 +2099,7 @@
       </c>
       <c r="D10" s="45"/>
     </row>
-    <row r="11" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>120</v>
       </c>
@@ -1663,327 +2130,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="33.81640625" customWidth="1"/>
-    <col min="3" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="103.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="B2" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="35" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="36">
-        <v>2</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="E9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="E10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="E11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="36">
-        <v>2</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="E12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="36">
-        <v>2021</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="E13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C14" s="36">
-        <v>2030</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="E14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>178</v>
-      </c>
-      <c r="C15" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>202</v>
-      </c>
-      <c r="E15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>181</v>
-      </c>
-      <c r="C16" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>202</v>
-      </c>
-      <c r="E16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C17" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="E17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="34">
-        <v>3.67</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="E18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>202</v>
-      </c>
-      <c r="E19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>199</v>
-      </c>
-      <c r="C20" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>202</v>
-      </c>
-      <c r="E20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>212</v>
-      </c>
-      <c r="C21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C15:C16">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C20">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C19:C20" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
-      <formula1>Boolean</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A95900C-A9EB-48AB-A762-0F120DA62856}">
-          <x14:formula1>
-            <xm:f>Sheet1!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C21</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="9.81640625" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" customWidth="1"/>
-    <col min="15" max="15" width="12.54296875" customWidth="1"/>
-    <col min="16" max="16" width="11.81640625" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" customWidth="1"/>
-    <col min="18" max="18" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -2035,7 +2212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2061,7 +2238,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="31" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="29"/>
       <c r="B3" s="30" t="s">
         <v>152</v>
@@ -2115,7 +2292,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2152,7 +2329,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2189,7 +2366,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2225,7 +2402,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2261,7 +2438,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2297,7 +2474,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2333,7 +2510,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2369,7 +2546,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2405,7 +2582,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2441,7 +2618,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>209</v>
       </c>
@@ -2468,7 +2645,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>208</v>
       </c>
@@ -2495,7 +2672,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>211</v>
       </c>
@@ -2522,7 +2699,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations xWindow="558" yWindow="395" count="2">
@@ -2557,31 +2734,31 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="21.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.54296875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2646,7 +2823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2675,7 +2852,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="20" t="s">
         <v>144</v>
@@ -2738,7 +2915,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -2790,7 +2967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -2842,7 +3019,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -2894,7 +3071,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>133</v>
       </c>
@@ -2946,7 +3123,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -2998,7 +3175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>130</v>
       </c>
@@ -3051,7 +3228,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="28" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" s="28" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>131</v>
       </c>
@@ -3104,7 +3281,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -3155,7 +3332,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -3207,7 +3384,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -3259,420 +3436,420 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H14" s="42"/>
       <c r="I14" s="42"/>
       <c r="O14" s="43"/>
       <c r="Q14" s="44"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
       <c r="Q15" s="24"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
       <c r="Q16" s="24"/>
     </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
       <c r="Q17" s="24"/>
     </row>
-    <row r="18" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
       <c r="Q18" s="24"/>
     </row>
-    <row r="19" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
       <c r="Q21" s="24"/>
     </row>
-    <row r="22" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
       <c r="Q23" s="24"/>
     </row>
-    <row r="24" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E35" s="24" t="s">
         <v>198</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="O36"/>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="O37"/>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="O38"/>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
       <c r="O39"/>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
       <c r="O41"/>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
       <c r="O42"/>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
       <c r="O43"/>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="N44"/>
       <c r="O44"/>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
       <c r="O47"/>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
       <c r="O48"/>
     </row>
-    <row r="49" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
       <c r="O49"/>
     </row>
-    <row r="50" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
       <c r="O50"/>
     </row>
-    <row r="51" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
       <c r="O51"/>
     </row>
-    <row r="52" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
       <c r="O52"/>
     </row>
-    <row r="53" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
       <c r="O53"/>
     </row>
-    <row r="54" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
       <c r="O54"/>
     </row>
-    <row r="55" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
       <c r="O55"/>
     </row>
-    <row r="56" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
       <c r="O56"/>
     </row>
-    <row r="57" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
       <c r="O57"/>
     </row>
-    <row r="58" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
       <c r="O58"/>
     </row>
-    <row r="59" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
       <c r="O59"/>
     </row>
-    <row r="60" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
       <c r="O60"/>
     </row>
-    <row r="61" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
       <c r="O61"/>
     </row>
-    <row r="62" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
       <c r="O62"/>
     </row>
-    <row r="63" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
       <c r="O63"/>
     </row>
-    <row r="64" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
       <c r="O64"/>
     </row>
-    <row r="65" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
       <c r="O65"/>
     </row>
-    <row r="66" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
       <c r="O66"/>
     </row>
-    <row r="67" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
       <c r="O67"/>
     </row>
-    <row r="68" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
       <c r="O68"/>
     </row>
-    <row r="69" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
       <c r="O69"/>
     </row>
-    <row r="70" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
       <c r="O70"/>
     </row>
-    <row r="71" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
       <c r="O71"/>
     </row>
-    <row r="72" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
       <c r="O72"/>
     </row>
-    <row r="73" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
       <c r="O73"/>
     </row>
-    <row r="74" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
       <c r="O74"/>
     </row>
-    <row r="75" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
       <c r="O75"/>
     </row>
-    <row r="76" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
       <c r="O76"/>
     </row>
-    <row r="77" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
       <c r="O77"/>
     </row>
-    <row r="78" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
       <c r="O78"/>
     </row>
-    <row r="79" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
       <c r="O80"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
       <c r="O81"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
       <c r="O82"/>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
       <c r="O83"/>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
       <c r="O84"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
       <c r="O85"/>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N86"/>
       <c r="O86"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3683,25 +3860,25 @@
       <c r="N87"/>
       <c r="O87"/>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
       <c r="O88"/>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
       <c r="O89"/>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
       <c r="O90"/>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
@@ -3724,6 +3901,68 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="52.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E839B9F-9E6A-42D1-BF39-12023C14C5F8}">
   <dimension ref="A1:AG102"/>
   <sheetViews>
@@ -3731,22 +3970,22 @@
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
-    <col min="2" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" customWidth="1"/>
-    <col min="16" max="16" width="15.26953125" customWidth="1"/>
-    <col min="17" max="17" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.36328125" customWidth="1"/>
-    <col min="26" max="26" width="19.36328125" customWidth="1"/>
-    <col min="27" max="27" width="18.54296875" customWidth="1"/>
-    <col min="28" max="28" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" customWidth="1"/>
+    <col min="27" max="27" width="18.5703125" customWidth="1"/>
+    <col min="28" max="28" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>112</v>
       </c>
@@ -3760,7 +3999,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>113</v>
       </c>
@@ -3835,7 +4074,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2021</v>
       </c>
@@ -3915,7 +4154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2022</v>
       </c>
@@ -3995,7 +4234,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2023</v>
       </c>
@@ -4075,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2024</v>
       </c>
@@ -4155,7 +4394,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2025</v>
       </c>
@@ -4235,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2026</v>
       </c>
@@ -4315,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2027</v>
       </c>
@@ -4395,7 +4634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2028</v>
       </c>
@@ -4475,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2029</v>
       </c>
@@ -4555,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2030</v>
       </c>
@@ -4635,7 +4874,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C13" s="32" t="s">
         <v>139</v>
       </c>
@@ -4670,7 +4909,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14">
         <v>2021</v>
@@ -4733,7 +4972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15">
         <v>2021</v>
@@ -4799,7 +5038,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2022</v>
       </c>
@@ -4864,7 +5103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2023</v>
       </c>
@@ -4929,7 +5168,7 @@
         <v>5.1000000000000004E-4</v>
       </c>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2024</v>
       </c>
@@ -4994,7 +5233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2025</v>
       </c>
@@ -5059,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2026</v>
       </c>
@@ -5124,7 +5363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2027</v>
       </c>
@@ -5189,7 +5428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2028</v>
       </c>
@@ -5255,7 +5494,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2029</v>
       </c>
@@ -5320,7 +5559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2030</v>
       </c>
@@ -5385,7 +5624,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C25" s="32" t="s">
         <v>83</v>
       </c>
@@ -5420,7 +5659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B26" s="27"/>
       <c r="C26">
         <v>2021</v>
@@ -5483,7 +5722,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2021</v>
       </c>
@@ -5549,7 +5788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2022</v>
       </c>
@@ -5615,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2023</v>
       </c>
@@ -5681,7 +5920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2024</v>
       </c>
@@ -5747,7 +5986,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>2025</v>
       </c>
@@ -5813,7 +6052,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>2026</v>
       </c>
@@ -5879,7 +6118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>2027</v>
       </c>
@@ -5945,7 +6184,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2028</v>
       </c>
@@ -6011,7 +6250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2029</v>
       </c>
@@ -6077,7 +6316,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2030</v>
       </c>
@@ -6143,7 +6382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C37" s="32" t="s">
         <v>84</v>
       </c>
@@ -6178,7 +6417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B38" s="27"/>
       <c r="C38">
         <v>2021</v>
@@ -6241,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2021</v>
       </c>
@@ -6306,7 +6545,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2022</v>
       </c>
@@ -6371,7 +6610,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>2023</v>
       </c>
@@ -6436,7 +6675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>2024</v>
       </c>
@@ -6501,7 +6740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2025</v>
       </c>
@@ -6566,7 +6805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>2026</v>
       </c>
@@ -6631,7 +6870,7 @@
         <v>2.5384799999999998</v>
       </c>
     </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2027</v>
       </c>
@@ -6696,7 +6935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>2028</v>
       </c>
@@ -6761,7 +7000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>2029</v>
       </c>
@@ -6826,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:33" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>2030</v>
       </c>
@@ -6891,7 +7130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="49" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W49">
         <v>2025</v>
       </c>
@@ -6923,7 +7162,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="50" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W50">
         <v>2025</v>
       </c>
@@ -6955,7 +7194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="51" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W51">
         <v>2025</v>
       </c>
@@ -6987,7 +7226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="52" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W52">
         <v>2025</v>
       </c>
@@ -7019,7 +7258,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="53" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="53" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W53">
         <v>2026</v>
       </c>
@@ -7051,7 +7290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="54" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W54">
         <v>2026</v>
       </c>
@@ -7083,7 +7322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="55" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W55">
         <v>2026</v>
       </c>
@@ -7115,7 +7354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="56" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W56">
         <v>2026</v>
       </c>
@@ -7147,7 +7386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="57" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W57">
         <v>2026</v>
       </c>
@@ -7179,7 +7418,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="58" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W58">
         <v>2026</v>
       </c>
@@ -7211,7 +7450,7 @@
         <v>60.000300000000003</v>
       </c>
     </row>
-    <row r="59" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="59" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W59">
         <v>2026</v>
       </c>
@@ -7243,7 +7482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="60" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W60">
         <v>2026</v>
       </c>
@@ -7275,7 +7514,7 @@
         <v>60.000300000000003</v>
       </c>
     </row>
-    <row r="61" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="61" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W61">
         <v>2026</v>
       </c>
@@ -7307,7 +7546,7 @@
         <v>7.6000000000000004E-4</v>
       </c>
     </row>
-    <row r="62" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="62" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W62">
         <v>2026</v>
       </c>
@@ -7339,7 +7578,7 @@
         <v>13.46152</v>
       </c>
     </row>
-    <row r="63" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="63" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W63">
         <v>2027</v>
       </c>
@@ -7371,7 +7610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="64" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W64">
         <v>2027</v>
       </c>
@@ -7403,7 +7642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="65" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W65">
         <v>2027</v>
       </c>
@@ -7435,7 +7674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="66" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W66">
         <v>2027</v>
       </c>
@@ -7467,7 +7706,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="67" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W67">
         <v>2027</v>
       </c>
@@ -7499,7 +7738,7 @@
         <v>60.01296</v>
       </c>
     </row>
-    <row r="68" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="68" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W68">
         <v>2027</v>
       </c>
@@ -7531,7 +7770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="69" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W69">
         <v>2027</v>
       </c>
@@ -7563,7 +7802,7 @@
         <v>60.01296</v>
       </c>
     </row>
-    <row r="70" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="70" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W70">
         <v>2027</v>
       </c>
@@ -7595,7 +7834,7 @@
         <v>3.2399999999999998E-2</v>
       </c>
     </row>
-    <row r="71" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="71" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W71">
         <v>2027</v>
       </c>
@@ -7627,7 +7866,7 @@
         <v>15.635999999999999</v>
       </c>
     </row>
-    <row r="72" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="72" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W72">
         <v>2027</v>
       </c>
@@ -7659,7 +7898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="73" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W73">
         <v>2028</v>
       </c>
@@ -7691,7 +7930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="74" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W74">
         <v>2028</v>
       </c>
@@ -7723,7 +7962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="75" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W75">
         <v>2028</v>
       </c>
@@ -7755,7 +7994,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="76" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W76">
         <v>2028</v>
       </c>
@@ -7787,7 +8026,7 @@
         <v>60.218400000000003</v>
       </c>
     </row>
-    <row r="77" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="77" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W77">
         <v>2028</v>
       </c>
@@ -7819,7 +8058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="78" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W78">
         <v>2028</v>
       </c>
@@ -7851,7 +8090,7 @@
         <v>60.218400000000003</v>
       </c>
     </row>
-    <row r="79" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="79" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W79">
         <v>2028</v>
       </c>
@@ -7883,7 +8122,7 @@
         <v>0.54600000000000004</v>
       </c>
     </row>
-    <row r="80" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="80" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W80">
         <v>2028</v>
       </c>
@@ -7915,7 +8154,7 @@
         <v>15.978400000000001</v>
       </c>
     </row>
-    <row r="81" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="81" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W81">
         <v>2028</v>
       </c>
@@ -7947,7 +8186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="82" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W82">
         <v>2028</v>
       </c>
@@ -7979,7 +8218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="83" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W83">
         <v>2029</v>
       </c>
@@ -8011,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="84" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W84">
         <v>2029</v>
       </c>
@@ -8043,7 +8282,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="85" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W85">
         <v>2029</v>
       </c>
@@ -8075,7 +8314,7 @@
         <v>61.523090000000003</v>
       </c>
     </row>
-    <row r="86" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="86" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W86">
         <v>2029</v>
       </c>
@@ -8107,7 +8346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="87" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W87">
         <v>2029</v>
       </c>
@@ -8139,7 +8378,7 @@
         <v>61.523090000000003</v>
       </c>
     </row>
-    <row r="88" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="88" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W88">
         <v>2029</v>
       </c>
@@ -8171,7 +8410,7 @@
         <v>3.8077299999999998</v>
       </c>
     </row>
-    <row r="89" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="89" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W89">
         <v>2029</v>
       </c>
@@ -8203,7 +8442,7 @@
         <v>15.999510000000001</v>
       </c>
     </row>
-    <row r="90" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="90" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W90">
         <v>2029</v>
       </c>
@@ -8235,7 +8474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="91" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W91">
         <v>2029</v>
       </c>
@@ -8267,7 +8506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="92" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W92">
         <v>2029</v>
       </c>
@@ -8299,7 +8538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="93" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W93">
         <v>2030</v>
       </c>
@@ -8319,7 +8558,7 @@
         <v>4.0684800000000001</v>
       </c>
     </row>
-    <row r="94" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="94" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W94">
         <v>2030</v>
       </c>
@@ -8339,7 +8578,7 @@
         <v>12.205439999999999</v>
       </c>
     </row>
-    <row r="95" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="95" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W95">
         <v>2030</v>
       </c>
@@ -8359,7 +8598,7 @@
         <v>10.481030000000001</v>
       </c>
     </row>
-    <row r="96" spans="23:33" x14ac:dyDescent="0.35">
+    <row r="96" spans="23:33" x14ac:dyDescent="0.25">
       <c r="W96">
         <v>2030</v>
       </c>
@@ -8379,7 +8618,7 @@
         <v>1.8959999999999999</v>
       </c>
     </row>
-    <row r="97" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="97" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W97">
         <v>2030</v>
       </c>
@@ -8399,7 +8638,7 @@
         <v>5.7401499999999999</v>
       </c>
     </row>
-    <row r="98" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="98" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W98">
         <v>2030</v>
       </c>
@@ -8419,7 +8658,7 @@
         <v>3.5876000000000001</v>
       </c>
     </row>
-    <row r="99" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="99" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W99">
         <v>2030</v>
       </c>
@@ -8439,7 +8678,7 @@
         <v>0.35092000000000001</v>
       </c>
     </row>
-    <row r="100" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="100" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W100">
         <v>2030</v>
       </c>
@@ -8459,7 +8698,7 @@
         <v>0.49347999999999997</v>
       </c>
     </row>
-    <row r="101" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="101" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W101">
         <v>2030</v>
       </c>
@@ -8479,7 +8718,7 @@
         <v>3.4558900000000001</v>
       </c>
     </row>
-    <row r="102" spans="23:28" x14ac:dyDescent="0.35">
+    <row r="102" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W102">
         <v>2030</v>
       </c>
@@ -8504,7 +8743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
   <dimension ref="B1:D2"/>
   <sheetViews>
@@ -8512,19 +8751,19 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>123</v>
       </c>
@@ -8540,7 +8779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
   <dimension ref="C1:E7"/>
   <sheetViews>
@@ -8548,14 +8787,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
-    <col min="11" max="11" width="30.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C1" s="32" t="s">
         <v>194</v>
       </c>
@@ -8566,7 +8806,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>140</v>
       </c>
@@ -8577,7 +8817,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>68</v>
       </c>
@@ -8588,7 +8828,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>141</v>
       </c>
@@ -8596,7 +8836,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>143</v>
       </c>
@@ -8604,12 +8844,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>218</v>
       </c>
@@ -8621,6 +8861,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
@@ -8630,15 +8879,6 @@
     <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8905,6 +9145,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -8917,14 +9165,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated example_data.xlsx and example.ipynb
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F772D17-35DC-4B39-AC03-C3949F0C65E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42634D5-5D6A-4516-8D72-BDB495C28BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -1166,6 +1166,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1181,7 +1182,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1255,23 +1255,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>717176</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>132512</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>539805</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>64113</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581633</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>45515</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1002229</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>167367</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Graphic 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BABF4E-C7EF-DF86-E1EE-F6428C7FAEDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38CE90A0-1D4A-FAFE-60B0-0D24A3BEE1B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1280,21 +1280,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4448735" y="3079659"/>
-          <a:ext cx="8912460" cy="2961003"/>
+          <a:off x="2701980" y="2969238"/>
+          <a:ext cx="8501524" cy="3151254"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1619,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1773,7 @@
         <v>178</v>
       </c>
       <c r="C15" s="38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>202</v>
@@ -1985,10 +1979,10 @@
       <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -1997,10 +1991,10 @@
       <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2010,10 +2004,10 @@
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="47"/>
     </row>
     <row r="4" spans="1:5" s="17" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
@@ -2022,10 +2016,10 @@
       <c r="B4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="50"/>
     </row>
     <row r="5" spans="1:5" s="17" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
@@ -2034,10 +2028,10 @@
       <c r="B5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="50"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -2046,10 +2040,10 @@
       <c r="B6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -2058,10 +2052,10 @@
       <c r="B7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="45"/>
+      <c r="D7" s="46"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2070,10 +2064,10 @@
       <c r="B8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="49"/>
     </row>
     <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -2082,10 +2076,10 @@
       <c r="B9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="45"/>
+      <c r="D9" s="46"/>
     </row>
     <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -2094,10 +2088,10 @@
       <c r="B10" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="46"/>
     </row>
     <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -2106,10 +2100,10 @@
       <c r="B11" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="45"/>
+      <c r="D11" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2135,7 +2129,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2733,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3923,37 +3917,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="45" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="45" t="s">
         <v>235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed multiple duplicate sections in example.ipynb, cleaned example_data.xlsx and removed code block in datavisualizer.py that was causing issues with Plotly.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42634D5-5D6A-4516-8D72-BDB495C28BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627BF555-DDE6-45C8-9B30-F3AAB3FAB6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Settings" sheetId="11" r:id="rId1"/>
-    <sheet name="Readme" sheetId="4" r:id="rId2"/>
+    <sheet name="Readme" sheetId="4" r:id="rId1"/>
+    <sheet name="Settings" sheetId="11" r:id="rId2"/>
     <sheet name="Processes" sheetId="6" r:id="rId3"/>
     <sheet name="Flows" sheetId="1" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
     <sheet name="DMFA results (example)" sheetId="8" r:id="rId6"/>
     <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="Data validation parameters" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$U$14</definedName>
-    <definedName name="Boolean">Sheet1!$D$2:$D$3</definedName>
+    <definedName name="Boolean">'Data validation parameters'!$C$6:$C$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="240">
   <si>
     <t>Years</t>
   </si>
@@ -909,6 +909,15 @@
       </rPr>
       <t xml:space="preserve"> is enabled</t>
     </r>
+  </si>
+  <si>
+    <t>This sheet contains helper parameters to make changing settings easier inside Excel and to reduce possibilities of typos.</t>
+  </si>
+  <si>
+    <t>All of these settings are strings that can be used as it is in Settings-sheet and in Scenarios-sheet</t>
+  </si>
+  <si>
+    <t>Change type</t>
   </si>
 </sst>
 </file>
@@ -1161,11 +1170,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1181,6 +1185,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1610,11 +1619,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="29" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="44"/>
+    </row>
+    <row r="4" spans="1:5" s="17" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="47"/>
+    </row>
+    <row r="5" spans="1:5" s="17" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="47"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="43"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="46"/>
+    </row>
+    <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="43"/>
+    </row>
+    <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="43"/>
+    </row>
+    <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,7 +2123,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A95900C-A9EB-48AB-A762-0F120DA62856}">
           <x14:formula1>
-            <xm:f>Sheet1!$E$2:$E$5</xm:f>
+            <xm:f>'Data validation parameters'!$D$6:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>C21</xm:sqref>
         </x14:dataValidation>
@@ -1955,181 +2133,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.85546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="29" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="48"/>
-    </row>
-    <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="47"/>
-    </row>
-    <row r="4" spans="1:5" s="17" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="50"/>
-    </row>
-    <row r="5" spans="1:5" s="17" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="50"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="49"/>
-    </row>
-    <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="D7" s="46"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="49"/>
-    </row>
-    <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="46"/>
-    </row>
-    <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="46"/>
-    </row>
-    <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="46"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C9:D9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,13 +2716,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="558" yWindow="395" count="2">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{0258C8E4-0AAB-48FF-93D5-AADF99BF39C4}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$6</xm:f>
+            <xm:f>'Data validation parameters'!$B$6:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>H16:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{61770E9E-9EFD-4B63-8C83-80C1E833E691}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$7</xm:f>
+            <xm:f>'Data validation parameters'!$B$6:$B$11</xm:f>
           </x14:formula1>
           <xm:sqref>H4:H15</xm:sqref>
         </x14:dataValidation>
@@ -2727,8 +2736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,109 +3178,109 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="28" t="str">
+      <c r="C9" s="48" t="str">
         <f>+_xlfn.XLOOKUP(H9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="28" t="str">
+      <c r="F9" s="48" t="str">
         <f>+_xlfn.XLOOKUP(I9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="42" t="str">
+      <c r="H9" s="49" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I9" s="42" t="str">
+      <c r="I9" s="49" t="str">
         <f t="shared" si="1"/>
         <v>Sawmilling:FI</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="48">
         <v>40</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="48">
         <v>2021</v>
       </c>
-      <c r="N9" s="28" t="s">
+      <c r="N9" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="43"/>
-      <c r="P9" s="28">
+      <c r="O9" s="50"/>
+      <c r="P9" s="48">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
-      <c r="Q9" s="28" t="s">
+      <c r="Q9" s="48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="28" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:21" s="48" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="28" t="str">
+      <c r="C10" s="48" t="str">
         <f>+_xlfn.XLOOKUP(H10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="28" t="str">
+      <c r="F10" s="48" t="str">
         <f>+_xlfn.XLOOKUP(I10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="42" t="str">
+      <c r="H10" s="49" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I10" s="42" t="str">
+      <c r="I10" s="49" t="str">
         <f t="shared" si="1"/>
         <v>Incineration:FI</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="48">
         <v>60</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="48">
         <v>2021</v>
       </c>
-      <c r="N10" s="28" t="s">
+      <c r="N10" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="43"/>
-      <c r="P10" s="28">
+      <c r="O10" s="50"/>
+      <c r="P10" s="48">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
-      <c r="Q10" s="28" t="s">
+      <c r="Q10" s="48" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3430,11 +3439,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="O14" s="43"/>
-      <c r="Q14" s="44"/>
+    <row r="14" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="O14" s="50"/>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
@@ -3898,8 +3907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,42 +3926,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="42" t="s">
         <v>235</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21908276-F864-4CA4-BA65-3DBA76B06B97}">
+          <x14:formula1>
+            <xm:f>'Data validation parameters'!$E$6:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8775,76 +8796,96 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
-  <dimension ref="C1:E7"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="32" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="C5" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="D5" s="32" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="E5" s="32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="b">
+      <c r="C6" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D6" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="E6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>141</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D8" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>143</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D9" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>218</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now output is directed to "output" directory. Directory is created under the "output" for each scenario and scenario-related results are saved there.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627BF555-DDE6-45C8-9B30-F3AAB3FAB6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E45439-6B6E-4350-A924-7D4E5AA5C103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
@@ -1087,7 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1185,11 +1185,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1792,7 +1787,7 @@
   <dimension ref="B2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,109 +3173,107 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="48" t="str">
+      <c r="C9" t="str">
         <f>+_xlfn.XLOOKUP(H9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="48" t="str">
+      <c r="F9" t="str">
         <f>+_xlfn.XLOOKUP(I9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
-      <c r="G9" s="48" t="s">
+      <c r="G9" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="49" t="str">
+      <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I9" s="49" t="str">
+      <c r="I9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Sawmilling:FI</v>
       </c>
-      <c r="J9" s="48">
+      <c r="J9">
         <v>40</v>
       </c>
-      <c r="K9" s="48" t="s">
+      <c r="K9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="48">
+      <c r="L9">
         <v>2021</v>
       </c>
-      <c r="N9" s="48" t="s">
+      <c r="N9" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="50"/>
-      <c r="P9" s="48">
+      <c r="P9">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
-      <c r="Q9" s="48" t="s">
+      <c r="Q9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="48" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+    <row r="10" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="48" t="str">
+      <c r="C10" t="str">
         <f>+_xlfn.XLOOKUP(H10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="48" t="str">
+      <c r="F10" t="str">
         <f>+_xlfn.XLOOKUP(I10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="49" t="str">
+      <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I10" s="49" t="str">
+      <c r="I10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Incineration:FI</v>
       </c>
-      <c r="J10" s="48">
+      <c r="J10">
         <v>60</v>
       </c>
-      <c r="K10" s="48" t="s">
+      <c r="K10" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="48">
+      <c r="L10">
         <v>2021</v>
       </c>
-      <c r="N10" s="48" t="s">
+      <c r="N10" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="50"/>
-      <c r="P10" s="48">
+      <c r="P10">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
-      <c r="Q10" s="48" t="s">
+      <c r="Q10" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3439,10 +3432,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="O14" s="50"/>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="N14"/>
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -8896,27 +8889,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -9179,10 +9151,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9205,20 +9209,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated output path detection to example.ipynb and cleaned example.xlsx.
Removed path detection from dataprovider.py
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E45439-6B6E-4350-A924-7D4E5AA5C103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C579A881-51F1-4402-A2EC-7802EBC03897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
@@ -18,9 +18,9 @@
     <sheet name="Processes" sheetId="6" r:id="rId3"/>
     <sheet name="Flows" sheetId="1" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
-    <sheet name="DMFA results (example)" sheetId="8" r:id="rId6"/>
-    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId7"/>
-    <sheet name="Data validation parameters" sheetId="9" r:id="rId8"/>
+    <sheet name="Data validation parameters" sheetId="9" r:id="rId6"/>
+    <sheet name="DMFA results (example)" sheetId="8" r:id="rId7"/>
+    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$U$14</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="244">
   <si>
     <t>Years</t>
   </si>
@@ -918,6 +918,18 @@
   </si>
   <si>
     <t>Change type</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Exponential</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1799,7 @@
   <dimension ref="B2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2145,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,10 +2403,10 @@
         <v>1</v>
       </c>
       <c r="P6">
-        <v>0.40300000000000002</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="Q6">
-        <v>0.10100000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="R6" t="s">
         <v>76</v>
@@ -2535,10 +2547,10 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>0.26400000000000001</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="Q10">
-        <v>0.81899999999999995</v>
+        <v>0.9</v>
       </c>
       <c r="R10" t="s">
         <v>81</v>
@@ -2702,7 +2714,7 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations xWindow="558" yWindow="395" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameter" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I4:I1048576" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sankey diagram positioning" prompt="Sankey diagram X and Y node positioning. Check / adjust positioning after you run case and see coordinates. " sqref="P4:Q1048576 Q2" xr:uid="{167D7519-74A2-4731-8D99-C2A980321CC9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sankey diagram positioning" prompt="Sankey diagram X and Y node positioning. Check / adjust positioning after you run case and see coordinates. " sqref="Q2 P4:Q1048576" xr:uid="{167D7519-74A2-4731-8D99-C2A980321CC9}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2732,7 +2744,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,7 +3913,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3957,12 +3969,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21908276-F864-4CA4-BA65-3DBA76B06B97}">
           <x14:formula1>
             <xm:f>'Data validation parameters'!$E$6:$E$7</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{283A9876-07D1-4356-BD7B-618A4AD94BB4}">
+          <x14:formula1>
+            <xm:f>'Data validation parameters'!$F$6:$F$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3971,6 +3989,123 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E839B9F-9E6A-42D1-BF39-12023C14C5F8}">
   <dimension ref="A1:AG102"/>
   <sheetViews>
@@ -8751,7 +8886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
   <dimension ref="B1:D2"/>
   <sheetViews>
@@ -8787,108 +8922,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
-  <dimension ref="B2:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>214</v>
-      </c>
-      <c r="E6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>215</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -9151,42 +9206,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9209,9 +9232,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added 1 alternative scenario to example_data.xlsx
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A37C4E6-D985-491E-A9C8-11749158EB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C34F668-96B0-4505-9134-22977D4DB67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="237">
   <si>
     <t>Years</t>
   </si>
@@ -888,6 +888,9 @@
   </si>
   <si>
     <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>Reduce sawmilling residues by 50% between 2025 and 2030</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1105,29 +1108,17 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1136,21 +1127,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1574,57 +1562,57 @@
       <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="34" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="34" customWidth="1"/>
     <col min="3" max="3" width="29" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.54296875" style="36" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="10"/>
+    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="45"/>
-    </row>
-    <row r="2" spans="1:5" ht="135.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="38"/>
-    </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="43" t="s">
@@ -1632,89 +1620,89 @@
       </c>
       <c r="D4" s="43"/>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D5" s="48"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="D5" s="40"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="40"/>
-    </row>
-    <row r="7" spans="1:5" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
+      <c r="D6" s="42"/>
+    </row>
+    <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="D7" s="38"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="39" t="s">
+      <c r="D7" s="40"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="40"/>
-    </row>
-    <row r="9" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="D8" s="42"/>
+    </row>
+    <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="38"/>
-    </row>
-    <row r="10" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39" t="s">
+      <c r="D9" s="40"/>
+    </row>
+    <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="38"/>
-    </row>
-    <row r="11" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1739,28 +1727,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.81640625" customWidth="1"/>
-    <col min="3" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="103.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="103.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="25" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>182</v>
       </c>
@@ -1768,7 +1756,7 @@
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>157</v>
       </c>
@@ -1782,7 +1770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>158</v>
       </c>
@@ -1796,7 +1784,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>159</v>
       </c>
@@ -1810,7 +1798,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>161</v>
       </c>
@@ -1824,7 +1812,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>162</v>
       </c>
@@ -1838,7 +1826,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>163</v>
       </c>
@@ -1852,7 +1840,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>164</v>
       </c>
@@ -1866,7 +1854,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>170</v>
       </c>
@@ -1880,7 +1868,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>173</v>
       </c>
@@ -1894,7 +1882,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>174</v>
       </c>
@@ -1908,7 +1896,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>177</v>
       </c>
@@ -1922,7 +1910,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>185</v>
       </c>
@@ -1936,7 +1924,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>179</v>
       </c>
@@ -1950,7 +1938,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>196</v>
       </c>
@@ -1964,7 +1952,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>195</v>
       </c>
@@ -1978,7 +1966,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>204</v>
       </c>
@@ -1992,7 +1980,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>211</v>
       </c>
@@ -2006,7 +1994,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>214</v>
       </c>
@@ -2020,7 +2008,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>216</v>
       </c>
@@ -2086,32 +2074,32 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -2163,7 +2151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2189,7 +2177,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="23" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="22" t="s">
         <v>148</v>
@@ -2243,7 +2231,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2280,7 +2268,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2317,7 +2305,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2353,7 +2341,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2389,7 +2377,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2425,7 +2413,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2461,7 +2449,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2497,7 +2485,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2533,7 +2521,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2569,7 +2557,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations xWindow="794" yWindow="485" count="2">
@@ -2610,31 +2598,31 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="H6" sqref="H6:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="21.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.54296875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2699,7 +2687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2728,7 +2716,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="12" t="s">
         <v>140</v>
@@ -2791,7 +2779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -2841,7 +2829,7 @@
       </c>
       <c r="Q4" s="16"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -2891,7 +2879,7 @@
       </c>
       <c r="Q5" s="16"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -2941,7 +2929,7 @@
       </c>
       <c r="Q6" s="16"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -2993,7 +2981,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -3045,7 +3033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -3097,7 +3085,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -3149,7 +3137,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -3194,7 +3182,7 @@
       </c>
       <c r="Q11" s="16"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -3240,7 +3228,7 @@
       </c>
       <c r="Q12" s="16"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>133</v>
       </c>
@@ -3286,420 +3274,420 @@
       </c>
       <c r="Q13" s="16"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="N14"/>
       <c r="Q14" s="9"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
       <c r="Q17" s="16"/>
     </row>
-    <row r="18" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
       <c r="Q18" s="16"/>
     </row>
-    <row r="19" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
       <c r="Q21" s="16"/>
     </row>
-    <row r="22" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
       <c r="Q22" s="16"/>
     </row>
-    <row r="23" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
       <c r="Q23" s="16"/>
     </row>
-    <row r="24" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E35" s="16" t="s">
         <v>194</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="O36"/>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="O37"/>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="O38"/>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
       <c r="O39"/>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
       <c r="O41"/>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
       <c r="O42"/>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
       <c r="O43"/>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="N44"/>
       <c r="O44"/>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
       <c r="O47"/>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
       <c r="O48"/>
     </row>
-    <row r="49" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
       <c r="O49"/>
     </row>
-    <row r="50" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
       <c r="O50"/>
     </row>
-    <row r="51" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
       <c r="O51"/>
     </row>
-    <row r="52" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
       <c r="O52"/>
     </row>
-    <row r="53" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
       <c r="O53"/>
     </row>
-    <row r="54" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
       <c r="O54"/>
     </row>
-    <row r="55" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
       <c r="O55"/>
     </row>
-    <row r="56" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
       <c r="O56"/>
     </row>
-    <row r="57" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
       <c r="O57"/>
     </row>
-    <row r="58" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
       <c r="O58"/>
     </row>
-    <row r="59" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
       <c r="O59"/>
     </row>
-    <row r="60" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
       <c r="O60"/>
     </row>
-    <row r="61" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
       <c r="O61"/>
     </row>
-    <row r="62" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
       <c r="O62"/>
     </row>
-    <row r="63" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
       <c r="O63"/>
     </row>
-    <row r="64" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
       <c r="O64"/>
     </row>
-    <row r="65" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
       <c r="O65"/>
     </row>
-    <row r="66" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
       <c r="O66"/>
     </row>
-    <row r="67" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
       <c r="O67"/>
     </row>
-    <row r="68" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
       <c r="O68"/>
     </row>
-    <row r="69" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
       <c r="O69"/>
     </row>
-    <row r="70" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
       <c r="O70"/>
     </row>
-    <row r="71" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
       <c r="O71"/>
     </row>
-    <row r="72" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
       <c r="O72"/>
     </row>
-    <row r="73" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
       <c r="O73"/>
     </row>
-    <row r="74" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
       <c r="O74"/>
     </row>
-    <row r="75" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
       <c r="O75"/>
     </row>
-    <row r="76" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
       <c r="O76"/>
     </row>
-    <row r="77" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
       <c r="O77"/>
     </row>
-    <row r="78" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
       <c r="O78"/>
     </row>
-    <row r="79" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
       <c r="O80"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
       <c r="O81"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
       <c r="O82"/>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
       <c r="O83"/>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
       <c r="O84"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
       <c r="O85"/>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N86"/>
       <c r="O86"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3710,25 +3698,25 @@
       <c r="N87"/>
       <c r="O87"/>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
       <c r="O88"/>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
       <c r="O89"/>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
       <c r="O90"/>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
@@ -3748,27 +3736,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="52.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>218</v>
       </c>
@@ -3802,6 +3790,36 @@
       <c r="K1" s="32" t="s">
         <v>227</v>
       </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>-50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>2025</v>
+      </c>
+      <c r="H2">
+        <v>2030</v>
+      </c>
+      <c r="I2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3834,27 +3852,27 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>190</v>
       </c>
@@ -3871,7 +3889,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>136</v>
       </c>
@@ -3888,7 +3906,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>68</v>
       </c>
@@ -3905,7 +3923,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>137</v>
       </c>
@@ -3916,7 +3934,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>139</v>
       </c>
@@ -3927,12 +3945,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>210</v>
       </c>
@@ -3951,22 +3969,22 @@
       <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
-    <col min="2" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" customWidth="1"/>
-    <col min="15" max="15" width="18.7265625" customWidth="1"/>
-    <col min="16" max="16" width="19.90625" customWidth="1"/>
-    <col min="17" max="17" width="18.26953125" customWidth="1"/>
-    <col min="23" max="23" width="17.453125" customWidth="1"/>
-    <col min="24" max="24" width="19.453125" customWidth="1"/>
-    <col min="25" max="25" width="18.54296875" customWidth="1"/>
-    <col min="28" max="28" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" customWidth="1"/>
+    <col min="25" max="25" width="18.5703125" customWidth="1"/>
+    <col min="28" max="28" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>110</v>
       </c>
@@ -3992,7 +4010,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>111</v>
       </c>
@@ -4052,7 +4070,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2021</v>
       </c>
@@ -4094,7 +4112,7 @@
         <v>16</v>
       </c>
       <c r="P3" s="18">
-        <f>O3-N3</f>
+        <f t="shared" ref="P3:P12" si="0">O3-N3</f>
         <v>15.999995413574849</v>
       </c>
       <c r="Q3" s="18">
@@ -4129,7 +4147,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2022</v>
       </c>
@@ -4164,14 +4182,14 @@
         <v>0</v>
       </c>
       <c r="N4" s="18">
-        <f t="shared" ref="N4:N12" si="0">SUM(C4:L4)</f>
+        <f t="shared" ref="N4:N12" si="1">SUM(C4:L4)</f>
         <v>5.0673986932991955E-4</v>
       </c>
       <c r="O4">
         <v>16</v>
       </c>
       <c r="P4" s="18">
-        <f>O4-N4</f>
+        <f t="shared" si="0"/>
         <v>15.99949326013067</v>
       </c>
       <c r="Q4" s="18">
@@ -4206,7 +4224,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2023</v>
       </c>
@@ -4241,14 +4259,14 @@
         <v>0</v>
       </c>
       <c r="N5" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1598368506081621E-2</v>
       </c>
       <c r="O5">
         <v>16</v>
       </c>
       <c r="P5" s="18">
-        <f>O5-N5</f>
+        <f t="shared" si="0"/>
         <v>15.978401631493918</v>
       </c>
       <c r="Q5" s="18">
@@ -4283,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2024</v>
       </c>
@@ -4318,14 +4336,14 @@
         <v>0</v>
       </c>
       <c r="N6" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.36400211117086662</v>
       </c>
       <c r="O6">
         <v>16</v>
       </c>
       <c r="P6" s="18">
-        <f>O6-N6</f>
+        <f t="shared" si="0"/>
         <v>15.635997888829133</v>
       </c>
       <c r="Q6" s="18">
@@ -4360,7 +4378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2025</v>
       </c>
@@ -4395,14 +4413,14 @@
         <v>0</v>
       </c>
       <c r="N7" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5384840629033087</v>
       </c>
       <c r="O7">
         <v>16</v>
       </c>
       <c r="P7" s="18">
-        <f>O7-N7</f>
+        <f t="shared" si="0"/>
         <v>13.461515937096692</v>
       </c>
       <c r="Q7" s="18">
@@ -4437,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2026</v>
       </c>
@@ -4472,14 +4490,14 @@
         <v>0</v>
       </c>
       <c r="N8" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0000000000004299</v>
       </c>
       <c r="O8">
         <v>16</v>
       </c>
       <c r="P8" s="18">
-        <f>O8-N8</f>
+        <f t="shared" si="0"/>
         <v>7.9999999999995701</v>
       </c>
       <c r="Q8" s="18">
@@ -4514,7 +4532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2027</v>
       </c>
@@ -4549,14 +4567,14 @@
         <v>0</v>
       </c>
       <c r="N9" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.461515937171171</v>
       </c>
       <c r="O9">
         <v>16</v>
       </c>
       <c r="P9" s="18">
-        <f>O9-N9</f>
+        <f t="shared" si="0"/>
         <v>2.5384840628288288</v>
       </c>
       <c r="Q9" s="18">
@@ -4591,7 +4609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2028</v>
       </c>
@@ -4626,14 +4644,14 @@
         <v>0</v>
       </c>
       <c r="N10" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.635997895664687</v>
       </c>
       <c r="O10">
         <v>16</v>
       </c>
       <c r="P10" s="18">
-        <f>O10-N10</f>
+        <f t="shared" si="0"/>
         <v>0.36400210433531299</v>
       </c>
       <c r="Q10" s="18">
@@ -4668,7 +4686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2029</v>
       </c>
@@ -4703,14 +4721,14 @@
         <v>0</v>
       </c>
       <c r="N11" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.978402003613578</v>
       </c>
       <c r="O11">
         <v>16</v>
       </c>
       <c r="P11" s="18">
-        <f>O11-N11</f>
+        <f t="shared" si="0"/>
         <v>2.1597996386422125E-2</v>
       </c>
       <c r="Q11" s="18">
@@ -4745,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2030</v>
       </c>
@@ -4780,14 +4798,14 @@
         <v>4.7610636570993796E-6</v>
       </c>
       <c r="N12" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.99950576325014</v>
       </c>
       <c r="O12">
         <v>16</v>
       </c>
       <c r="P12" s="18">
-        <f>O12-N12</f>
+        <f t="shared" si="0"/>
         <v>4.9423674986037724E-4</v>
       </c>
       <c r="Q12" s="18">
@@ -4822,7 +4840,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C13" s="24" t="s">
         <v>135</v>
       </c>
@@ -4854,7 +4872,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14">
         <v>2021</v>
@@ -4914,7 +4932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15">
         <v>2021</v>
@@ -4977,7 +4995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2022</v>
       </c>
@@ -5039,7 +5057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2023</v>
       </c>
@@ -5101,7 +5119,7 @@
         <v>5.1000000000000004E-4</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2024</v>
       </c>
@@ -5163,7 +5181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2025</v>
       </c>
@@ -5225,7 +5243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2026</v>
       </c>
@@ -5287,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2027</v>
       </c>
@@ -5349,7 +5367,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2028</v>
       </c>
@@ -5412,7 +5430,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2029</v>
       </c>
@@ -5474,7 +5492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2030</v>
       </c>
@@ -5536,7 +5554,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C25" s="24" t="s">
         <v>82</v>
       </c>
@@ -5568,7 +5586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" s="19"/>
       <c r="C26">
         <v>2021</v>
@@ -5628,7 +5646,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2021</v>
       </c>
@@ -5691,7 +5709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2022</v>
       </c>
@@ -5754,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2023</v>
       </c>
@@ -5816,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2024</v>
       </c>
@@ -5879,7 +5897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>2025</v>
       </c>
@@ -5942,7 +5960,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>2026</v>
       </c>
@@ -6004,7 +6022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>2027</v>
       </c>
@@ -6067,7 +6085,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2028</v>
       </c>
@@ -6130,7 +6148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2029</v>
       </c>
@@ -6193,7 +6211,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2030</v>
       </c>
@@ -6256,7 +6274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C37" s="24" t="s">
         <v>83</v>
       </c>
@@ -6288,7 +6306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B38" s="19"/>
       <c r="C38">
         <v>2021</v>
@@ -6348,7 +6366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2021</v>
       </c>
@@ -6410,7 +6428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2022</v>
       </c>
@@ -6472,7 +6490,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>2023</v>
       </c>
@@ -6534,7 +6552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>2024</v>
       </c>
@@ -6596,7 +6614,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2025</v>
       </c>
@@ -6658,7 +6676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>2026</v>
       </c>
@@ -6720,7 +6738,7 @@
         <v>2.5384799999999998</v>
       </c>
     </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2027</v>
       </c>
@@ -6782,7 +6800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>2028</v>
       </c>
@@ -6844,7 +6862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>2029</v>
       </c>
@@ -6906,7 +6924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>2030</v>
       </c>
@@ -6968,7 +6986,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U49">
         <v>2025</v>
       </c>
@@ -6997,7 +7015,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U50">
         <v>2025</v>
       </c>
@@ -7026,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U51">
         <v>2025</v>
       </c>
@@ -7055,7 +7073,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U52">
         <v>2025</v>
       </c>
@@ -7084,7 +7102,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="53" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U53">
         <v>2026</v>
       </c>
@@ -7113,7 +7131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U54">
         <v>2026</v>
       </c>
@@ -7142,7 +7160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U55">
         <v>2026</v>
       </c>
@@ -7171,7 +7189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U56">
         <v>2026</v>
       </c>
@@ -7200,7 +7218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U57">
         <v>2026</v>
       </c>
@@ -7229,7 +7247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U58">
         <v>2026</v>
       </c>
@@ -7258,7 +7276,7 @@
         <v>60.000300000000003</v>
       </c>
     </row>
-    <row r="59" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U59">
         <v>2026</v>
       </c>
@@ -7287,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="60" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U60">
         <v>2026</v>
       </c>
@@ -7316,7 +7334,7 @@
         <v>60.000300000000003</v>
       </c>
     </row>
-    <row r="61" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="61" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U61">
         <v>2026</v>
       </c>
@@ -7345,7 +7363,7 @@
         <v>7.6000000000000004E-4</v>
       </c>
     </row>
-    <row r="62" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="62" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U62">
         <v>2026</v>
       </c>
@@ -7374,7 +7392,7 @@
         <v>13.46152</v>
       </c>
     </row>
-    <row r="63" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="63" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U63">
         <v>2027</v>
       </c>
@@ -7403,7 +7421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="64" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U64">
         <v>2027</v>
       </c>
@@ -7432,7 +7450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="65" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U65">
         <v>2027</v>
       </c>
@@ -7461,7 +7479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="66" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U66">
         <v>2027</v>
       </c>
@@ -7490,7 +7508,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="67" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U67">
         <v>2027</v>
       </c>
@@ -7519,7 +7537,7 @@
         <v>60.01296</v>
       </c>
     </row>
-    <row r="68" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="68" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U68">
         <v>2027</v>
       </c>
@@ -7548,7 +7566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="69" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U69">
         <v>2027</v>
       </c>
@@ -7577,7 +7595,7 @@
         <v>60.01296</v>
       </c>
     </row>
-    <row r="70" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="70" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U70">
         <v>2027</v>
       </c>
@@ -7606,7 +7624,7 @@
         <v>3.2399999999999998E-2</v>
       </c>
     </row>
-    <row r="71" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="71" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U71">
         <v>2027</v>
       </c>
@@ -7635,7 +7653,7 @@
         <v>15.635999999999999</v>
       </c>
     </row>
-    <row r="72" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="72" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U72">
         <v>2027</v>
       </c>
@@ -7664,7 +7682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="73" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U73">
         <v>2028</v>
       </c>
@@ -7693,7 +7711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="74" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U74">
         <v>2028</v>
       </c>
@@ -7722,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="75" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U75">
         <v>2028</v>
       </c>
@@ -7751,7 +7769,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="76" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U76">
         <v>2028</v>
       </c>
@@ -7780,7 +7798,7 @@
         <v>60.218400000000003</v>
       </c>
     </row>
-    <row r="77" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="77" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U77">
         <v>2028</v>
       </c>
@@ -7809,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="78" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U78">
         <v>2028</v>
       </c>
@@ -7838,7 +7856,7 @@
         <v>60.218400000000003</v>
       </c>
     </row>
-    <row r="79" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="79" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U79">
         <v>2028</v>
       </c>
@@ -7867,7 +7885,7 @@
         <v>0.54600000000000004</v>
       </c>
     </row>
-    <row r="80" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="80" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U80">
         <v>2028</v>
       </c>
@@ -7896,7 +7914,7 @@
         <v>15.978400000000001</v>
       </c>
     </row>
-    <row r="81" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="81" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U81">
         <v>2028</v>
       </c>
@@ -7925,7 +7943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="82" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U82">
         <v>2028</v>
       </c>
@@ -7954,7 +7972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="83" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U83">
         <v>2029</v>
       </c>
@@ -7983,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="84" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U84">
         <v>2029</v>
       </c>
@@ -8012,7 +8030,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="85" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U85">
         <v>2029</v>
       </c>
@@ -8041,7 +8059,7 @@
         <v>61.523090000000003</v>
       </c>
     </row>
-    <row r="86" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="86" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U86">
         <v>2029</v>
       </c>
@@ -8070,7 +8088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="87" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U87">
         <v>2029</v>
       </c>
@@ -8099,7 +8117,7 @@
         <v>61.523090000000003</v>
       </c>
     </row>
-    <row r="88" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="88" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U88">
         <v>2029</v>
       </c>
@@ -8128,7 +8146,7 @@
         <v>3.8077299999999998</v>
       </c>
     </row>
-    <row r="89" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="89" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U89">
         <v>2029</v>
       </c>
@@ -8157,7 +8175,7 @@
         <v>15.999510000000001</v>
       </c>
     </row>
-    <row r="90" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="90" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U90">
         <v>2029</v>
       </c>
@@ -8186,7 +8204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="91" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U91">
         <v>2029</v>
       </c>
@@ -8215,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="92" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U92">
         <v>2029</v>
       </c>
@@ -8244,7 +8262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="93" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U93">
         <v>2030</v>
       </c>
@@ -8261,7 +8279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="94" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U94">
         <v>2030</v>
       </c>
@@ -8278,7 +8296,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="95" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U95">
         <v>2030</v>
       </c>
@@ -8295,7 +8313,7 @@
         <v>51.523090000000003</v>
       </c>
     </row>
-    <row r="96" spans="21:30" x14ac:dyDescent="0.35">
+    <row r="96" spans="21:30" x14ac:dyDescent="0.25">
       <c r="U96">
         <v>2030</v>
       </c>
@@ -8312,7 +8330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="21:25" x14ac:dyDescent="0.35">
+    <row r="97" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U97">
         <v>2030</v>
       </c>
@@ -8329,7 +8347,7 @@
         <v>24.91385</v>
       </c>
     </row>
-    <row r="98" spans="21:25" x14ac:dyDescent="0.35">
+    <row r="98" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U98">
         <v>2030</v>
       </c>
@@ -8346,7 +8364,7 @@
         <v>16.60924</v>
       </c>
     </row>
-    <row r="99" spans="21:25" x14ac:dyDescent="0.35">
+    <row r="99" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U99">
         <v>2030</v>
       </c>
@@ -8363,7 +8381,7 @@
         <v>1.5230900000000001</v>
       </c>
     </row>
-    <row r="100" spans="21:25" x14ac:dyDescent="0.35">
+    <row r="100" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U100">
         <v>2030</v>
       </c>
@@ -8380,7 +8398,7 @@
         <v>2.28464</v>
       </c>
     </row>
-    <row r="101" spans="21:25" x14ac:dyDescent="0.35">
+    <row r="101" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U101">
         <v>2030</v>
       </c>
@@ -8397,7 +8415,7 @@
         <v>15.999510000000001</v>
       </c>
     </row>
-    <row r="102" spans="21:25" x14ac:dyDescent="0.35">
+    <row r="102" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U102">
         <v>2030</v>
       </c>
@@ -8428,19 +8446,19 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>121</v>
       </c>
@@ -8457,15 +8475,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
@@ -8475,6 +8484,15 @@
     <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8741,14 +8759,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -8761,6 +8771,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Implemented reading list of variables from settings (now used with visualize_inflows_to_processes). Now plot is done automatically for the process IDs defined in the parameter visualize_inflows_to_processes.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C34F668-96B0-4505-9134-22977D4DB67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA55E94-BAF5-4785-A3D8-40FC92425069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Processes" sheetId="6" r:id="rId3"/>
     <sheet name="Flows" sheetId="1" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
-    <sheet name="Data validation parameters" sheetId="9" r:id="rId6"/>
-    <sheet name="DMFA results (example)" sheetId="8" r:id="rId7"/>
-    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId8"/>
+    <sheet name="Transformation stage colors" sheetId="13" r:id="rId6"/>
+    <sheet name="Data validation parameters" sheetId="9" r:id="rId7"/>
+    <sheet name="DMFA results (example)" sheetId="8" r:id="rId8"/>
+    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$U$14</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="240">
   <si>
     <t>Years</t>
   </si>
@@ -890,7 +891,16 @@
     <t>Sigmoid</t>
   </si>
   <si>
-    <t>Reduce sawmilling residues by 50% between 2025 and 2030</t>
+    <t>visualize_inflows_to_processes</t>
+  </si>
+  <si>
+    <t>Create inflow visualization and export data for process IDs defined in here. Each process ID must be separated by comma (',')</t>
+  </si>
+  <si>
+    <t>List of strings</t>
+  </si>
+  <si>
+    <t>Incineration:FI,  Sawmilling:FI, Sawnwood:FI</t>
   </si>
 </sst>
 </file>
@@ -1725,17 +1735,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="103.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="115.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
@@ -2013,13 +2024,27 @@
         <v>216</v>
       </c>
       <c r="C24" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>198</v>
       </c>
       <c r="E24" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C25" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E25" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2074,7 +2099,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,7 +2623,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:I6"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,8 +2643,9 @@
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.5703125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28" customWidth="1"/>
+    <col min="17" max="17" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="53.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -3738,9 +3764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3792,30 +3816,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2">
-        <v>-50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>2025</v>
-      </c>
-      <c r="H2">
-        <v>2030</v>
-      </c>
-      <c r="I2" t="s">
-        <v>233</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -3845,6 +3847,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA92C4F1-884F-4740-8793-4A0AB47EED3D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
   <dimension ref="B2:F11"/>
   <sheetViews>
@@ -3961,7 +3977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E839B9F-9E6A-42D1-BF39-12023C14C5F8}">
   <dimension ref="A1:AD102"/>
   <sheetViews>
@@ -8438,7 +8454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
   <dimension ref="B1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added: - Checking if start year is set before any earliest flow data year - Reading base unit name from settings file (with default value "Mm3 SWE" if not found) - Sheet for transformation stage colors in settings file - Stock data is now exported to CSV per scenario
Changed:
DataChecker now raises Exception if any errors occur
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA55E94-BAF5-4785-A3D8-40FC92425069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764901BD-7DED-42A9-AED0-E3206316D288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="257">
   <si>
     <t>Years</t>
   </si>
@@ -267,33 +267,6 @@
   </si>
   <si>
     <t xml:space="preserve">Random input values </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 Roundwood </t>
-  </si>
-  <si>
-    <t>1 Sawmilling</t>
-  </si>
-  <si>
-    <t>2 By products</t>
-  </si>
-  <si>
-    <t>3 Sawnwood</t>
-  </si>
-  <si>
-    <t>4 Construction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 Furnitute </t>
-  </si>
-  <si>
-    <t>8 Incineration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 Import </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 Export </t>
   </si>
   <si>
     <t>Carbon OC</t>
@@ -900,7 +873,85 @@
     <t>List of strings</t>
   </si>
   <si>
-    <t>Incineration:FI,  Sawmilling:FI, Sawnwood:FI</t>
+    <t>Incineration:FI, Sawmilling:FI</t>
+  </si>
+  <si>
+    <t>base_unit_name</t>
+  </si>
+  <si>
+    <t>Base unit name. This is used with relative flows when exporting flow data to CSVs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 Roundwood </t>
+  </si>
+  <si>
+    <t>1 Sawmilling</t>
+  </si>
+  <si>
+    <t>2 By products</t>
+  </si>
+  <si>
+    <t>3 Sawnwood</t>
+  </si>
+  <si>
+    <t>4 Construction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Import </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 Export </t>
+  </si>
+  <si>
+    <t>8 Incineration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Furniture </t>
+  </si>
+  <si>
+    <t>Transformation stage name</t>
+  </si>
+  <si>
+    <t>Color (hex code)</t>
+  </si>
+  <si>
+    <t>Reduce sawmilling residues by 50% between 2025 and 2030</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Virtual</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>#7DDA60</t>
+  </si>
+  <si>
+    <t>#eb5e34</t>
+  </si>
+  <si>
+    <t>#8c76cf</t>
+  </si>
+  <si>
+    <t>#5BAA11</t>
+  </si>
+  <si>
+    <t>#3281db</t>
+  </si>
+  <si>
+    <t>#61b053</t>
+  </si>
+  <si>
+    <t>#EFC3CA</t>
+  </si>
+  <si>
+    <t>#DFC57B</t>
+  </si>
+  <si>
+    <t>#707070</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1151,6 +1202,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1569,7 +1623,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:D8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1655,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D2" s="40"/>
       <c r="E2" s="1"/>
@@ -1614,7 +1668,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D3" s="40"/>
     </row>
@@ -1638,7 +1692,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D5" s="40"/>
     </row>
@@ -1662,7 +1716,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D7" s="40"/>
     </row>
@@ -1692,25 +1746,25 @@
     </row>
     <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D11" s="40"/>
     </row>
@@ -1735,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E25"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,17 +1805,17 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="25" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -1769,13 +1823,13 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>4</v>
@@ -1783,268 +1837,282 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C8" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" t="s">
         <v>160</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C9" s="28">
         <v>2</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C12" s="28">
         <v>2</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C13" s="28">
         <v>2021</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E13" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C14" s="28">
         <v>2030</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E14" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C15" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E15" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C16" s="30" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C17" s="17">
         <v>0.1</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E17" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C18" s="26">
         <v>3.67</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E18" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C19" s="30" t="b">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C20" s="30" t="b">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E20" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C21" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C22" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D22" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E22" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C23" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E23" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C24" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E24" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D25" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E25" t="s">
-        <v>237</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2099,7 +2167,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2214,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>11</v>
@@ -2205,28 +2273,28 @@
     <row r="3" spans="1:18" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="22" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>16</v>
@@ -2277,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2290,7 +2358,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>73</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -2314,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2327,7 +2395,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>74</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2351,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2363,7 +2431,7 @@
         <v>0.05</v>
       </c>
       <c r="R6" t="s">
-        <v>75</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2387,7 +2455,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2399,7 +2467,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>76</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2435,7 +2503,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>77</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2471,7 +2539,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>78</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2495,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2507,7 +2575,7 @@
         <v>0.9</v>
       </c>
       <c r="R10" t="s">
-        <v>80</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2531,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2543,7 +2611,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>81</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2567,7 +2635,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -2579,7 +2647,7 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>79</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2691,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,31 +2813,31 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="12" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>12</v>
@@ -2787,10 +2855,10 @@
         <v>54</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="R3" s="14" t="s">
         <v>55</v>
@@ -2807,7 +2875,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
         <v>58</v>
@@ -2841,7 +2909,7 @@
         <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="L4">
         <v>2021</v>
@@ -2857,7 +2925,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
@@ -2907,7 +2975,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -2941,7 +3009,7 @@
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="L6">
         <v>2021</v>
@@ -2957,7 +3025,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>59</v>
@@ -3009,7 +3077,7 @@
     </row>
     <row r="8" spans="1:21" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
@@ -3061,7 +3129,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>61</v>
@@ -3113,7 +3181,7 @@
     </row>
     <row r="10" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -3165,7 +3233,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -3210,7 +3278,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
@@ -3244,7 +3312,7 @@
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="L12">
         <v>2021</v>
@@ -3256,7 +3324,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
         <v>59</v>
@@ -3290,7 +3358,7 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="L13">
         <v>2021</v>
@@ -3406,7 +3474,7 @@
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E35" s="16" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3764,7 +3832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3782,42 +3852,65 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="G1" s="32" t="s">
+      <c r="K1" s="32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="45">
+        <v>-50</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="45">
+        <v>2025</v>
+      </c>
+      <c r="H2" s="45">
+        <v>2030</v>
+      </c>
+      <c r="I2" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="H1" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -3848,14 +3941,107 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA92C4F1-884F-4740-8793-4A0AB47EED3D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3880,46 +4066,46 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F6" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -3930,45 +4116,45 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F8" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F9" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4002,33 +4188,33 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="N1" s="24" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="P1" s="24" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="Q1" s="24" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="V1" s="24" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="AA1" s="24" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2">
@@ -4062,28 +4248,28 @@
         <v>2030</v>
       </c>
       <c r="V2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="W2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="X2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="Y2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="AA2" t="s">
         <v>52</v>
       </c>
       <c r="AB2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AC2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="AD2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -4139,13 +4325,13 @@
         <v>2021</v>
       </c>
       <c r="V3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y3">
         <v>60</v>
@@ -4154,7 +4340,7 @@
         <v>2021</v>
       </c>
       <c r="AB3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -4216,13 +4402,13 @@
         <v>2021</v>
       </c>
       <c r="V4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y4">
         <v>50</v>
@@ -4231,7 +4417,7 @@
         <v>2021</v>
       </c>
       <c r="AB4" s="24" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC4">
         <v>60</v>
@@ -4293,13 +4479,13 @@
         <v>2021</v>
       </c>
       <c r="V5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y5">
         <v>10</v>
@@ -4308,7 +4494,7 @@
         <v>2021</v>
       </c>
       <c r="AB5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC5">
         <v>10</v>
@@ -4370,13 +4556,13 @@
         <v>2021</v>
       </c>
       <c r="V6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y6">
         <v>24</v>
@@ -4385,7 +4571,7 @@
         <v>2021</v>
       </c>
       <c r="AB6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC6">
         <v>60</v>
@@ -4447,13 +4633,13 @@
         <v>2021</v>
       </c>
       <c r="V7" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X7" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y7">
         <v>16</v>
@@ -4462,7 +4648,7 @@
         <v>2021</v>
       </c>
       <c r="AB7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC7">
         <v>24</v>
@@ -4524,13 +4710,13 @@
         <v>2021</v>
       </c>
       <c r="V8" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -4539,7 +4725,7 @@
         <v>2021</v>
       </c>
       <c r="AB8" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC8">
         <v>16</v>
@@ -4601,13 +4787,13 @@
         <v>2021</v>
       </c>
       <c r="V9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -4616,7 +4802,7 @@
         <v>2021</v>
       </c>
       <c r="AB9" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -4678,13 +4864,13 @@
         <v>2021</v>
       </c>
       <c r="V10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W10" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X10" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -4693,7 +4879,7 @@
         <v>2021</v>
       </c>
       <c r="AB10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC10">
         <v>20</v>
@@ -4755,13 +4941,13 @@
         <v>2021</v>
       </c>
       <c r="V11" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W11" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X11" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y11">
         <v>20</v>
@@ -4770,7 +4956,7 @@
         <v>2021</v>
       </c>
       <c r="AB11" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -4832,13 +5018,13 @@
         <v>2021</v>
       </c>
       <c r="V12" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W12" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y12">
         <v>10</v>
@@ -4847,7 +5033,7 @@
         <v>2022</v>
       </c>
       <c r="AB12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -4858,19 +5044,19 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C13" s="24" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="U13">
         <v>2022</v>
       </c>
       <c r="V13" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W13" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X13" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y13">
         <v>10</v>
@@ -4879,7 +5065,7 @@
         <v>2022</v>
       </c>
       <c r="AB13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC13">
         <v>60</v>
@@ -4924,13 +5110,13 @@
         <v>2022</v>
       </c>
       <c r="V14" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W14" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X14" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y14">
         <v>20</v>
@@ -4939,7 +5125,7 @@
         <v>2022</v>
       </c>
       <c r="AB14" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC14">
         <v>10</v>
@@ -4987,13 +5173,13 @@
         <v>2022</v>
       </c>
       <c r="V15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W15" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X15" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y15">
         <v>5.1000000000000004E-4</v>
@@ -5002,7 +5188,7 @@
         <v>2022</v>
       </c>
       <c r="AB15" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC15">
         <v>60</v>
@@ -5049,13 +5235,13 @@
         <v>2022</v>
       </c>
       <c r="V16" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W16" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X16" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y16">
         <v>0</v>
@@ -5064,7 +5250,7 @@
         <v>2022</v>
       </c>
       <c r="AB16" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC16">
         <v>24</v>
@@ -5111,13 +5297,13 @@
         <v>2022</v>
       </c>
       <c r="V17" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W17" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X17" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y17">
         <v>0</v>
@@ -5126,7 +5312,7 @@
         <v>2022</v>
       </c>
       <c r="AB17" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC17">
         <v>16</v>
@@ -5173,13 +5359,13 @@
         <v>2022</v>
       </c>
       <c r="V18" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W18" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X18" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y18">
         <v>10</v>
@@ -5188,7 +5374,7 @@
         <v>2022</v>
       </c>
       <c r="AB18" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC18">
         <v>0</v>
@@ -5235,13 +5421,13 @@
         <v>2022</v>
       </c>
       <c r="V19" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W19" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y19">
         <v>24</v>
@@ -5250,7 +5436,7 @@
         <v>2022</v>
       </c>
       <c r="AB19" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC19">
         <v>20</v>
@@ -5297,13 +5483,13 @@
         <v>2022</v>
       </c>
       <c r="V20" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W20" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X20" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y20">
         <v>50</v>
@@ -5312,7 +5498,7 @@
         <v>2022</v>
       </c>
       <c r="AB20" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC20">
         <v>5.1000000000000004E-4</v>
@@ -5359,13 +5545,13 @@
         <v>2022</v>
       </c>
       <c r="V21" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W21" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X21" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y21">
         <v>60</v>
@@ -5374,7 +5560,7 @@
         <v>2023</v>
       </c>
       <c r="AB21" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC21">
         <v>0</v>
@@ -5422,13 +5608,13 @@
         <v>2022</v>
       </c>
       <c r="V22" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W22" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X22" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y22">
         <v>16</v>
@@ -5437,7 +5623,7 @@
         <v>2023</v>
       </c>
       <c r="AB22" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC22">
         <v>60</v>
@@ -5484,13 +5670,13 @@
         <v>2023</v>
       </c>
       <c r="V23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W23" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y23">
         <v>0</v>
@@ -5499,7 +5685,7 @@
         <v>2023</v>
       </c>
       <c r="AB23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC23">
         <v>10</v>
@@ -5546,13 +5732,13 @@
         <v>2023</v>
       </c>
       <c r="V24" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W24" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X24" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y24">
         <v>10</v>
@@ -5561,7 +5747,7 @@
         <v>2023</v>
       </c>
       <c r="AB24" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC24">
         <v>60</v>
@@ -5572,19 +5758,19 @@
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C25" s="24" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="U25">
         <v>2023</v>
       </c>
       <c r="V25" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W25" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X25" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y25">
         <v>20</v>
@@ -5593,7 +5779,7 @@
         <v>2023</v>
       </c>
       <c r="AB25" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC25">
         <v>24</v>
@@ -5638,13 +5824,13 @@
         <v>2023</v>
       </c>
       <c r="V26" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W26" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X26" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y26">
         <v>2.1600000000000001E-2</v>
@@ -5653,7 +5839,7 @@
         <v>2023</v>
       </c>
       <c r="AB26" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC26">
         <v>16</v>
@@ -5701,13 +5887,13 @@
         <v>2023</v>
       </c>
       <c r="V27" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W27" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X27" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y27">
         <v>0</v>
@@ -5716,7 +5902,7 @@
         <v>2023</v>
       </c>
       <c r="AB27" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC27">
         <v>0</v>
@@ -5764,13 +5950,13 @@
         <v>2023</v>
       </c>
       <c r="V28" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X28" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y28">
         <v>50</v>
@@ -5779,7 +5965,7 @@
         <v>2023</v>
       </c>
       <c r="AB28" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC28">
         <v>20</v>
@@ -5826,13 +6012,13 @@
         <v>2023</v>
       </c>
       <c r="V29" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W29" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X29" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y29">
         <v>24</v>
@@ -5841,7 +6027,7 @@
         <v>2023</v>
       </c>
       <c r="AB29" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC29">
         <v>2.1600000000000001E-2</v>
@@ -5889,13 +6075,13 @@
         <v>2023</v>
       </c>
       <c r="V30" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W30" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X30" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y30">
         <v>10</v>
@@ -5904,7 +6090,7 @@
         <v>2024</v>
       </c>
       <c r="AB30" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC30">
         <v>0</v>
@@ -5952,13 +6138,13 @@
         <v>2023</v>
       </c>
       <c r="V31" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W31" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X31" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y31">
         <v>60</v>
@@ -5967,7 +6153,7 @@
         <v>2024</v>
       </c>
       <c r="AB31" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC31">
         <v>60</v>
@@ -6014,13 +6200,13 @@
         <v>2023</v>
       </c>
       <c r="V32" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W32" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X32" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y32">
         <v>16</v>
@@ -6029,7 +6215,7 @@
         <v>2024</v>
       </c>
       <c r="AB32" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC32">
         <v>10</v>
@@ -6077,13 +6263,13 @@
         <v>2024</v>
       </c>
       <c r="V33" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W33" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X33" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y33">
         <v>10</v>
@@ -6092,7 +6278,7 @@
         <v>2024</v>
       </c>
       <c r="AB33" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC33">
         <v>60</v>
@@ -6140,13 +6326,13 @@
         <v>2024</v>
       </c>
       <c r="V34" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W34" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X34" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y34">
         <v>20</v>
@@ -6155,7 +6341,7 @@
         <v>2024</v>
       </c>
       <c r="AB34" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC34">
         <v>24</v>
@@ -6203,13 +6389,13 @@
         <v>2024</v>
       </c>
       <c r="V35" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W35" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X35" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y35">
         <v>0.36399999999999999</v>
@@ -6218,7 +6404,7 @@
         <v>2024</v>
       </c>
       <c r="AB35" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC35">
         <v>16</v>
@@ -6266,13 +6452,13 @@
         <v>2024</v>
       </c>
       <c r="V36" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W36" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X36" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y36">
         <v>0</v>
@@ -6281,7 +6467,7 @@
         <v>2024</v>
       </c>
       <c r="AB36" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC36">
         <v>0</v>
@@ -6292,19 +6478,19 @@
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C37" s="24" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="U37">
         <v>2024</v>
       </c>
       <c r="V37" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W37" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X37" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y37">
         <v>0</v>
@@ -6313,7 +6499,7 @@
         <v>2024</v>
       </c>
       <c r="AB37" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC37">
         <v>20</v>
@@ -6358,13 +6544,13 @@
         <v>2024</v>
       </c>
       <c r="V38" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W38" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X38" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y38">
         <v>16</v>
@@ -6373,7 +6559,7 @@
         <v>2024</v>
       </c>
       <c r="AB38" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC38">
         <v>0.36399999999999999</v>
@@ -6420,13 +6606,13 @@
         <v>2024</v>
       </c>
       <c r="V39" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W39" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X39" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y39">
         <v>10</v>
@@ -6435,7 +6621,7 @@
         <v>2025</v>
       </c>
       <c r="AB39" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC39">
         <v>0</v>
@@ -6482,13 +6668,13 @@
         <v>2024</v>
       </c>
       <c r="V40" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W40" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X40" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y40">
         <v>50</v>
@@ -6497,7 +6683,7 @@
         <v>2025</v>
       </c>
       <c r="AB40" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC40">
         <v>60</v>
@@ -6544,13 +6730,13 @@
         <v>2024</v>
       </c>
       <c r="V41" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W41" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X41" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y41">
         <v>60</v>
@@ -6559,7 +6745,7 @@
         <v>2025</v>
       </c>
       <c r="AB41" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC41">
         <v>10</v>
@@ -6606,13 +6792,13 @@
         <v>2024</v>
       </c>
       <c r="V42" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W42" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X42" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y42">
         <v>24</v>
@@ -6621,7 +6807,7 @@
         <v>2025</v>
       </c>
       <c r="AB42" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC42">
         <v>60</v>
@@ -6668,13 +6854,13 @@
         <v>2025</v>
       </c>
       <c r="V43" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W43" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X43" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y43">
         <v>0</v>
@@ -6683,7 +6869,7 @@
         <v>2025</v>
       </c>
       <c r="AB43" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC43">
         <v>24</v>
@@ -6730,13 +6916,13 @@
         <v>2025</v>
       </c>
       <c r="V44" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W44" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X44" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y44">
         <v>20</v>
@@ -6745,7 +6931,7 @@
         <v>2025</v>
       </c>
       <c r="AB44" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC44">
         <v>16</v>
@@ -6792,13 +6978,13 @@
         <v>2025</v>
       </c>
       <c r="V45" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W45" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X45" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y45">
         <v>2.5384799999999998</v>
@@ -6807,7 +6993,7 @@
         <v>2025</v>
       </c>
       <c r="AB45" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC45">
         <v>0</v>
@@ -6854,13 +7040,13 @@
         <v>2025</v>
       </c>
       <c r="V46" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W46" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X46" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y46">
         <v>0</v>
@@ -6869,7 +7055,7 @@
         <v>2025</v>
       </c>
       <c r="AB46" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC46">
         <v>20</v>
@@ -6916,13 +7102,13 @@
         <v>2025</v>
       </c>
       <c r="V47" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W47" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X47" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y47">
         <v>10</v>
@@ -6931,7 +7117,7 @@
         <v>2025</v>
       </c>
       <c r="AB47" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC47">
         <v>2.5384799999999998</v>
@@ -6978,13 +7164,13 @@
         <v>2025</v>
       </c>
       <c r="V48" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W48" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X48" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y48">
         <v>24</v>
@@ -6993,7 +7179,7 @@
         <v>2026</v>
       </c>
       <c r="AB48" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC48">
         <v>0</v>
@@ -7007,13 +7193,13 @@
         <v>2025</v>
       </c>
       <c r="V49" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W49" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X49" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y49">
         <v>10</v>
@@ -7022,7 +7208,7 @@
         <v>2026</v>
       </c>
       <c r="AB49" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC49">
         <v>60</v>
@@ -7036,13 +7222,13 @@
         <v>2025</v>
       </c>
       <c r="V50" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W50" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X50" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y50">
         <v>50</v>
@@ -7051,7 +7237,7 @@
         <v>2026</v>
       </c>
       <c r="AB50" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC50">
         <v>10</v>
@@ -7065,13 +7251,13 @@
         <v>2025</v>
       </c>
       <c r="V51" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W51" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X51" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y51">
         <v>60</v>
@@ -7080,7 +7266,7 @@
         <v>2026</v>
       </c>
       <c r="AB51" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC51">
         <v>60</v>
@@ -7094,13 +7280,13 @@
         <v>2025</v>
       </c>
       <c r="V52" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W52" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X52" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y52">
         <v>16</v>
@@ -7109,7 +7295,7 @@
         <v>2026</v>
       </c>
       <c r="AB52" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC52">
         <v>24</v>
@@ -7123,13 +7309,13 @@
         <v>2026</v>
       </c>
       <c r="V53" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W53" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X53" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y53">
         <v>20</v>
@@ -7138,7 +7324,7 @@
         <v>2026</v>
       </c>
       <c r="AB53" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC53">
         <v>16</v>
@@ -7152,13 +7338,13 @@
         <v>2026</v>
       </c>
       <c r="V54" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W54" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X54" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y54">
         <v>8</v>
@@ -7167,7 +7353,7 @@
         <v>2026</v>
       </c>
       <c r="AB54" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC54">
         <v>0</v>
@@ -7181,13 +7367,13 @@
         <v>2026</v>
       </c>
       <c r="V55" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W55" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X55" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y55">
         <v>0</v>
@@ -7196,7 +7382,7 @@
         <v>2026</v>
       </c>
       <c r="AB55" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC55">
         <v>20</v>
@@ -7210,13 +7396,13 @@
         <v>2026</v>
       </c>
       <c r="V56" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W56" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X56" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y56">
         <v>0</v>
@@ -7225,7 +7411,7 @@
         <v>2026</v>
       </c>
       <c r="AB56" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC56">
         <v>8</v>
@@ -7239,13 +7425,13 @@
         <v>2026</v>
       </c>
       <c r="V57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W57" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X57" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y57">
         <v>10</v>
@@ -7254,7 +7440,7 @@
         <v>2027</v>
       </c>
       <c r="AB57" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC57">
         <v>0</v>
@@ -7268,13 +7454,13 @@
         <v>2026</v>
       </c>
       <c r="V58" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W58" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X58" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y58">
         <v>24</v>
@@ -7283,7 +7469,7 @@
         <v>2027</v>
       </c>
       <c r="AB58" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC58">
         <v>60.000300000000003</v>
@@ -7297,13 +7483,13 @@
         <v>2026</v>
       </c>
       <c r="V59" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W59" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X59" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y59">
         <v>10</v>
@@ -7312,7 +7498,7 @@
         <v>2027</v>
       </c>
       <c r="AB59" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC59">
         <v>10</v>
@@ -7326,13 +7512,13 @@
         <v>2026</v>
       </c>
       <c r="V60" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W60" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X60" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y60">
         <v>50</v>
@@ -7341,7 +7527,7 @@
         <v>2027</v>
       </c>
       <c r="AB60" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC60">
         <v>60.000300000000003</v>
@@ -7355,13 +7541,13 @@
         <v>2026</v>
       </c>
       <c r="V61" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W61" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X61" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y61">
         <v>60</v>
@@ -7370,7 +7556,7 @@
         <v>2027</v>
       </c>
       <c r="AB61" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC61">
         <v>24.00018</v>
@@ -7384,13 +7570,13 @@
         <v>2026</v>
       </c>
       <c r="V62" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W62" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X62" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y62">
         <v>16</v>
@@ -7399,7 +7585,7 @@
         <v>2027</v>
       </c>
       <c r="AB62" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC62">
         <v>16.000119999999999</v>
@@ -7413,13 +7599,13 @@
         <v>2027</v>
       </c>
       <c r="V63" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W63" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X63" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y63">
         <v>10</v>
@@ -7428,7 +7614,7 @@
         <v>2027</v>
       </c>
       <c r="AB63" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC63">
         <v>0</v>
@@ -7442,13 +7628,13 @@
         <v>2027</v>
       </c>
       <c r="V64" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W64" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X64" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y64">
         <v>20</v>
@@ -7457,7 +7643,7 @@
         <v>2027</v>
       </c>
       <c r="AB64" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC64">
         <v>20</v>
@@ -7471,13 +7657,13 @@
         <v>2027</v>
       </c>
       <c r="V65" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W65" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X65" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y65">
         <v>13.46152</v>
@@ -7486,7 +7672,7 @@
         <v>2027</v>
       </c>
       <c r="AB65" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC65">
         <v>13.461970000000001</v>
@@ -7500,13 +7686,13 @@
         <v>2027</v>
       </c>
       <c r="V66" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W66" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X66" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y66">
         <v>4.6000000000000001E-4</v>
@@ -7515,7 +7701,7 @@
         <v>2028</v>
       </c>
       <c r="AB66" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC66">
         <v>0</v>
@@ -7529,13 +7715,13 @@
         <v>2027</v>
       </c>
       <c r="V67" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W67" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X67" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y67">
         <v>2.9999999999999997E-4</v>
@@ -7544,7 +7730,7 @@
         <v>2028</v>
       </c>
       <c r="AB67" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC67">
         <v>60.01296</v>
@@ -7558,13 +7744,13 @@
         <v>2027</v>
       </c>
       <c r="V68" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W68" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X68" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y68">
         <v>16.000119999999999</v>
@@ -7573,7 +7759,7 @@
         <v>2028</v>
       </c>
       <c r="AB68" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC68">
         <v>10</v>
@@ -7587,13 +7773,13 @@
         <v>2027</v>
       </c>
       <c r="V69" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W69" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X69" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y69">
         <v>10</v>
@@ -7602,7 +7788,7 @@
         <v>2028</v>
       </c>
       <c r="AB69" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC69">
         <v>60.01296</v>
@@ -7616,13 +7802,13 @@
         <v>2027</v>
       </c>
       <c r="V70" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W70" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X70" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y70">
         <v>50.000300000000003</v>
@@ -7631,7 +7817,7 @@
         <v>2028</v>
       </c>
       <c r="AB70" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC70">
         <v>24.00778</v>
@@ -7645,13 +7831,13 @@
         <v>2027</v>
       </c>
       <c r="V71" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W71" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X71" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y71">
         <v>60</v>
@@ -7660,7 +7846,7 @@
         <v>2028</v>
       </c>
       <c r="AB71" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC71">
         <v>16.005179999999999</v>
@@ -7674,13 +7860,13 @@
         <v>2027</v>
       </c>
       <c r="V72" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W72" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X72" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y72">
         <v>24.00018</v>
@@ -7689,7 +7875,7 @@
         <v>2028</v>
       </c>
       <c r="AB72" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC72">
         <v>0</v>
@@ -7703,13 +7889,13 @@
         <v>2028</v>
       </c>
       <c r="V73" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W73" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X73" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y73">
         <v>1.9439999999999999E-2</v>
@@ -7718,7 +7904,7 @@
         <v>2028</v>
       </c>
       <c r="AB73" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC73">
         <v>20</v>
@@ -7732,13 +7918,13 @@
         <v>2028</v>
       </c>
       <c r="V74" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W74" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X74" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y74">
         <v>20</v>
@@ -7747,7 +7933,7 @@
         <v>2028</v>
       </c>
       <c r="AB74" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC74">
         <v>15.65544</v>
@@ -7761,13 +7947,13 @@
         <v>2028</v>
       </c>
       <c r="V75" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W75" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X75" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y75">
         <v>15.635999999999999</v>
@@ -7776,7 +7962,7 @@
         <v>2029</v>
       </c>
       <c r="AB75" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC75">
         <v>0</v>
@@ -7790,13 +7976,13 @@
         <v>2028</v>
       </c>
       <c r="V76" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W76" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X76" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y76">
         <v>10</v>
@@ -7805,7 +7991,7 @@
         <v>2029</v>
       </c>
       <c r="AB76" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC76">
         <v>60.218400000000003</v>
@@ -7819,13 +8005,13 @@
         <v>2028</v>
       </c>
       <c r="V77" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W77" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X77" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y77">
         <v>1.2959999999999999E-2</v>
@@ -7834,7 +8020,7 @@
         <v>2029</v>
       </c>
       <c r="AB77" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC77">
         <v>10</v>
@@ -7848,13 +8034,13 @@
         <v>2028</v>
       </c>
       <c r="V78" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W78" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X78" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y78">
         <v>10</v>
@@ -7863,7 +8049,7 @@
         <v>2029</v>
       </c>
       <c r="AB78" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC78">
         <v>60.218400000000003</v>
@@ -7877,13 +8063,13 @@
         <v>2028</v>
       </c>
       <c r="V79" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W79" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X79" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y79">
         <v>24.00778</v>
@@ -7892,7 +8078,7 @@
         <v>2029</v>
       </c>
       <c r="AB79" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC79">
         <v>24.131039999999999</v>
@@ -7906,13 +8092,13 @@
         <v>2028</v>
       </c>
       <c r="V80" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W80" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X80" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y80">
         <v>50.01296</v>
@@ -7921,7 +8107,7 @@
         <v>2029</v>
       </c>
       <c r="AB80" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC80">
         <v>16.08736</v>
@@ -7935,13 +8121,13 @@
         <v>2028</v>
       </c>
       <c r="V81" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W81" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X81" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y81">
         <v>60</v>
@@ -7950,7 +8136,7 @@
         <v>2029</v>
       </c>
       <c r="AB81" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC81">
         <v>0</v>
@@ -7964,13 +8150,13 @@
         <v>2028</v>
       </c>
       <c r="V82" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W82" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X82" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y82">
         <v>16.005179999999999</v>
@@ -7979,7 +8165,7 @@
         <v>2029</v>
       </c>
       <c r="AB82" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC82">
         <v>20</v>
@@ -7993,13 +8179,13 @@
         <v>2029</v>
       </c>
       <c r="V83" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W83" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X83" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y83">
         <v>10</v>
@@ -8008,7 +8194,7 @@
         <v>2029</v>
       </c>
       <c r="AB83" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC83">
         <v>16.306000000000001</v>
@@ -8022,13 +8208,13 @@
         <v>2029</v>
       </c>
       <c r="V84" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W84" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X84" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y84">
         <v>20</v>
@@ -8037,7 +8223,7 @@
         <v>2030</v>
       </c>
       <c r="AB84" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AC84">
         <v>0</v>
@@ -8051,13 +8237,13 @@
         <v>2029</v>
       </c>
       <c r="V85" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W85" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X85" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y85">
         <v>0.3276</v>
@@ -8066,7 +8252,7 @@
         <v>2030</v>
       </c>
       <c r="AB85" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC85">
         <v>61.523090000000003</v>
@@ -8080,13 +8266,13 @@
         <v>2029</v>
       </c>
       <c r="V86" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W86" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X86" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y86">
         <v>0.21840000000000001</v>
@@ -8095,7 +8281,7 @@
         <v>2030</v>
       </c>
       <c r="AB86" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AC86">
         <v>10</v>
@@ -8109,13 +8295,13 @@
         <v>2029</v>
       </c>
       <c r="V87" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W87" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X87" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y87">
         <v>15.978400000000001</v>
@@ -8124,7 +8310,7 @@
         <v>2030</v>
       </c>
       <c r="AB87" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC87">
         <v>61.523090000000003</v>
@@ -8138,13 +8324,13 @@
         <v>2029</v>
       </c>
       <c r="V88" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W88" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X88" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y88">
         <v>24.131039999999999</v>
@@ -8153,7 +8339,7 @@
         <v>2030</v>
       </c>
       <c r="AB88" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="AC88">
         <v>24.91385</v>
@@ -8167,13 +8353,13 @@
         <v>2029</v>
       </c>
       <c r="V89" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W89" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X89" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y89">
         <v>10</v>
@@ -8182,7 +8368,7 @@
         <v>2030</v>
       </c>
       <c r="AB89" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC89">
         <v>16.60924</v>
@@ -8196,13 +8382,13 @@
         <v>2029</v>
       </c>
       <c r="V90" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W90" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X90" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y90">
         <v>50.218400000000003</v>
@@ -8211,7 +8397,7 @@
         <v>2030</v>
       </c>
       <c r="AB90" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="AC90">
         <v>0</v>
@@ -8225,13 +8411,13 @@
         <v>2029</v>
       </c>
       <c r="V91" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W91" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X91" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y91">
         <v>60</v>
@@ -8240,7 +8426,7 @@
         <v>2030</v>
       </c>
       <c r="AB91" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AC91">
         <v>20</v>
@@ -8254,13 +8440,13 @@
         <v>2029</v>
       </c>
       <c r="V92" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W92" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X92" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y92">
         <v>16.08736</v>
@@ -8269,7 +8455,7 @@
         <v>2030</v>
       </c>
       <c r="AB92" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="AC92">
         <v>18.284140000000001</v>
@@ -8283,13 +8469,13 @@
         <v>2030</v>
       </c>
       <c r="V93" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W93" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X93" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y93">
         <v>20</v>
@@ -8300,13 +8486,13 @@
         <v>2030</v>
       </c>
       <c r="V94" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="W94" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="X94" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y94">
         <v>60</v>
@@ -8317,13 +8503,13 @@
         <v>2030</v>
       </c>
       <c r="V95" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="W95" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X95" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y95">
         <v>51.523090000000003</v>
@@ -8334,13 +8520,13 @@
         <v>2030</v>
       </c>
       <c r="V96" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="W96" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="X96" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="Y96">
         <v>10</v>
@@ -8351,13 +8537,13 @@
         <v>2030</v>
       </c>
       <c r="V97" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="W97" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X97" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Y97">
         <v>24.91385</v>
@@ -8368,13 +8554,13 @@
         <v>2030</v>
       </c>
       <c r="V98" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="W98" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X98" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y98">
         <v>16.60924</v>
@@ -8385,13 +8571,13 @@
         <v>2030</v>
       </c>
       <c r="V99" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W99" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X99" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Y99">
         <v>1.5230900000000001</v>
@@ -8402,13 +8588,13 @@
         <v>2030</v>
       </c>
       <c r="V100" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="W100" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="X100" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y100">
         <v>2.28464</v>
@@ -8419,13 +8605,13 @@
         <v>2030</v>
       </c>
       <c r="V101" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="W101" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X101" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="Y101">
         <v>15.999510000000001</v>
@@ -8436,13 +8622,13 @@
         <v>2030</v>
       </c>
       <c r="V102" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W102" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="X102" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Y102">
         <v>10</v>
@@ -8476,7 +8662,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C2">
         <v>0.48</v>

</xml_diff>

<commit_message>
Added: - Parameters for reading color information from settings file: SheetNameColors, ColumnRangeColors, and SkipNumRowsColors - Color-class for storing color data - DataProvider now reads color information from sheet name defined in parameter "sheet_name_colors" - Updated FlowSolver docstrings for internal methods - DataVisualizer now creates default color palette (8 colors) and uses colors in that palette to fill any missing transformation stage color definition
Changed:
- Updated example_data.xlsx with Colors-sheet for defining transformation stage colors
- Updated example.ipynb to use the color definitions from settings file
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764901BD-7DED-42A9-AED0-E3206316D288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730E94AA-1844-4B31-A320-70D5F6A9D0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Processes" sheetId="6" r:id="rId3"/>
     <sheet name="Flows" sheetId="1" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
-    <sheet name="Transformation stage colors" sheetId="13" r:id="rId6"/>
+    <sheet name="Colors" sheetId="13" r:id="rId6"/>
     <sheet name="Data validation parameters" sheetId="9" r:id="rId7"/>
     <sheet name="DMFA results (example)" sheetId="8" r:id="rId8"/>
     <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId9"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="262">
   <si>
     <t>Years</t>
   </si>
@@ -639,9 +639,6 @@
     <t>If using virtual flows, create virtual flow to process if process total inputs and outputs difference is greater than this value</t>
   </si>
   <si>
-    <t xml:space="preserve">The carbon fraction sheet is only temprorary here and it is being used by thee Flows sheet. In the next version of aiphoria this will be moved. </t>
-  </si>
-  <si>
     <t xml:space="preserve">This is the input file of aiphoria where the user defines the processes/nodes and flows/arrows/edges within the preferred system. aiphoria supports both static and dynamic assessments (e.g from 2021 to 2050). If can be used to assess any system and both product or process based MFAs. </t>
   </si>
   <si>
@@ -927,31 +924,49 @@
     <t>Other</t>
   </si>
   <si>
-    <t>#7DDA60</t>
-  </si>
-  <si>
     <t>#eb5e34</t>
   </si>
   <si>
     <t>#8c76cf</t>
   </si>
   <si>
-    <t>#5BAA11</t>
-  </si>
-  <si>
     <t>#3281db</t>
   </si>
   <si>
     <t>#61b053</t>
   </si>
   <si>
-    <t>#EFC3CA</t>
-  </si>
-  <si>
-    <t>#DFC57B</t>
-  </si>
-  <si>
     <t>#707070</t>
+  </si>
+  <si>
+    <t>sheet_name_colors</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Sheet name that contains data for transformation stage colors (e.g. Colors)</t>
+  </si>
+  <si>
+    <t>#808080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The carbon fraction sheet is only temporary here and it is being used by the Flows sheet. In the next version of aiphoria this will be moved. </t>
+  </si>
+  <si>
+    <t>#7dda60</t>
+  </si>
+  <si>
+    <t>#5baa11</t>
+  </si>
+  <si>
+    <t>#efc3ca</t>
+  </si>
+  <si>
+    <t>#fdc57b</t>
+  </si>
+  <si>
+    <t>NOTE: Virtual flows are assigned to this transformation stage by default</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1202,9 +1217,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1622,9 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1655,7 +1665,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" s="40"/>
       <c r="E2" s="1"/>
@@ -1692,7 +1702,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D5" s="40"/>
     </row>
@@ -1716,7 +1726,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D7" s="40"/>
     </row>
@@ -1764,7 +1774,7 @@
         <v>110</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>178</v>
+        <v>256</v>
       </c>
       <c r="D11" s="40"/>
     </row>
@@ -1789,16 +1799,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E26"/>
+  <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="115.5703125" customWidth="1"/>
   </cols>
@@ -1843,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" t="s">
         <v>156</v>
@@ -1857,7 +1867,7 @@
         <v>151</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" t="s">
         <v>160</v>
@@ -1871,7 +1881,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" t="s">
         <v>157</v>
@@ -1885,7 +1895,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
         <v>158</v>
@@ -1899,7 +1909,7 @@
         <v>162</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
         <v>159</v>
@@ -1913,7 +1923,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E12" t="s">
         <v>157</v>
@@ -1927,7 +1937,7 @@
         <v>2021</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E13" t="s">
         <v>163</v>
@@ -1941,7 +1951,7 @@
         <v>2030</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E14" t="s">
         <v>172</v>
@@ -1955,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E15" t="s">
         <v>167</v>
@@ -1969,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E16" t="s">
         <v>169</v>
@@ -1983,7 +1993,7 @@
         <v>0.1</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E17" t="s">
         <v>177</v>
@@ -1997,7 +2007,7 @@
         <v>3.67</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E18" t="s">
         <v>171</v>
@@ -2005,114 +2015,128 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="30" t="b">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C20" s="30" t="b">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" t="s">
         <v>195</v>
       </c>
-      <c r="C21" t="s">
-        <v>196</v>
-      </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" t="s">
         <v>202</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" t="s">
         <v>203</v>
-      </c>
-      <c r="D22" t="s">
-        <v>191</v>
-      </c>
-      <c r="E22" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" t="s">
         <v>205</v>
-      </c>
-      <c r="C23" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>189</v>
-      </c>
-      <c r="E23" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C24" s="30" t="b">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>226</v>
+      </c>
+      <c r="C25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" t="s">
+        <v>228</v>
+      </c>
+      <c r="E25" t="s">
         <v>227</v>
-      </c>
-      <c r="C25" t="s">
-        <v>230</v>
-      </c>
-      <c r="D25" t="s">
-        <v>229</v>
-      </c>
-      <c r="E25" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C26" t="s">
         <v>114</v>
       </c>
       <c r="D26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E26" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2167,7 +2191,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,8 +2211,7 @@
     <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2314,7 +2337,7 @@
       <c r="O3" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="Q3" s="22" t="s">
@@ -2358,7 +2381,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -2395,7 +2418,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2431,7 +2454,7 @@
         <v>0.05</v>
       </c>
       <c r="R6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2467,7 +2490,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2503,7 +2526,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2539,7 +2562,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2575,7 +2598,7 @@
         <v>0.9</v>
       </c>
       <c r="R10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2611,7 +2634,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2647,7 +2670,7 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2691,7 +2714,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,7 +3497,7 @@
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E35" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3833,7 +3856,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3852,64 +3875,63 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="32" t="s">
-        <v>218</v>
-      </c>
       <c r="K1" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B2" s="46" t="s">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2">
         <v>-50</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="45">
+      <c r="G2">
         <v>2025</v>
       </c>
-      <c r="H2" s="45">
+      <c r="H2">
         <v>2030</v>
       </c>
-      <c r="I2" s="45" t="s">
-        <v>224</v>
+      <c r="I2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3941,10 +3963,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA92C4F1-884F-4740-8793-4A0AB47EED3D}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3953,96 +3975,100 @@
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="44" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
       <c r="B9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>246</v>
       </c>
-      <c r="B10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>247</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>256</v>
+      <c r="B11" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4066,29 +4092,29 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>166</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -4099,13 +4125,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" t="s">
         <v>138</v>
       </c>
       <c r="F6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -4116,13 +4142,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -4130,10 +4156,10 @@
         <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -4141,10 +4167,10 @@
         <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -4154,7 +4180,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4206,10 +4232,10 @@
         <v>106</v>
       </c>
       <c r="V1" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA1" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -4254,7 +4280,7 @@
         <v>95</v>
       </c>
       <c r="X2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Y2" t="s">
         <v>96</v>
@@ -8677,27 +8703,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -8960,7 +8965,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -8977,29 +9022,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added: - New parameters: ignore_columns_processes, ignore_columns_flows, ignore_columns_scenarios, ignore_columns_colors. Those parameters accept list of Excel column names and those columns are automatically ignored when reading data from settings file
Changed:
- User does not need to define anymore column range where data for Flows, Processes, Scenarios, and Colors are read from. This is now done automatically
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730E94AA-1844-4B31-A320-70D5F6A9D0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E09E6FB-417C-4B86-AA06-302D62C5F728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
@@ -1802,7 +1802,7 @@
   <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E4" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change: - Updated and prettified utility DataFrame building methods in FlowSolver: now *_as_dataframe()-methods include year column. Flow evaluated indicator values are also outputted
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C908704-BA60-4E86-8D4F-3F0D62C1455A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B11B4C-CC0E-4E7D-B81F-E8C366A6227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
@@ -1029,13 +1029,13 @@
     <t>2 columns needed for each indicator (name and comment)</t>
   </si>
   <si>
-    <t>SWE</t>
-  </si>
-  <si>
     <t>New parameter</t>
   </si>
   <si>
     <t>Reduce sawmilling residues by 50%</t>
+  </si>
+  <si>
+    <t>Solid wood equivalent</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1156,6 +1156,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1304,6 +1310,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1891,7 +1906,7 @@
   <dimension ref="A2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,7 +1966,7 @@
     </row>
     <row r="8" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>226</v>
@@ -1996,7 +2011,7 @@
     </row>
     <row r="11" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>227</v>
@@ -2097,13 +2112,13 @@
     </row>
     <row r="18" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>267</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D18" s="40" t="s">
         <v>161</v>
@@ -2114,7 +2129,7 @@
     </row>
     <row r="19" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" s="40" t="s">
         <v>268</v>
@@ -2201,7 +2216,7 @@
     </row>
     <row r="25" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>248</v>
@@ -2232,7 +2247,7 @@
         <v>177</v>
       </c>
       <c r="C27" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>159</v>
@@ -2271,7 +2286,7 @@
     </row>
     <row r="30" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B30" s="40" t="s">
         <v>249</v>
@@ -2337,7 +2352,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:T91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,9 +2929,9 @@
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26" style="6" customWidth="1"/>
-    <col min="16" max="16" width="29.28515625" customWidth="1"/>
-    <col min="17" max="17" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" style="49" customWidth="1"/>
+    <col min="16" max="16" width="29.28515625" style="50" customWidth="1"/>
+    <col min="17" max="17" width="45.7109375" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="45.7109375" customWidth="1"/>
     <col min="19" max="19" width="57.42578125" customWidth="1"/>
     <col min="20" max="20" width="46.28515625" bestFit="1" customWidth="1"/>
@@ -2965,13 +2980,13 @@
       <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="47" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="3"/>
@@ -3001,9 +3016,9 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3" t="s">
         <v>273</v>
@@ -3053,13 +3068,13 @@
       <c r="N3" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="48" t="s">
         <v>260</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="48" t="s">
         <v>262</v>
       </c>
       <c r="R3" s="42" t="s">
@@ -3116,11 +3131,11 @@
       <c r="N4" t="s">
         <v>62</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="50">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
-      <c r="Q4" s="16"/>
+      <c r="Q4" s="51"/>
       <c r="R4" s="16"/>
       <c r="S4">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
@@ -3172,11 +3187,11 @@
       <c r="N5" t="s">
         <v>62</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="50">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
-      <c r="Q5" s="16"/>
+      <c r="Q5" s="51"/>
       <c r="R5" s="16"/>
       <c r="S5">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
@@ -3228,11 +3243,11 @@
       <c r="N6" t="s">
         <v>62</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="50">
         <f>0.395*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.18959999999999999</v>
       </c>
-      <c r="Q6" s="16"/>
+      <c r="Q6" s="51"/>
       <c r="R6" s="16"/>
       <c r="S6">
         <f>0.395*'Carbon fraction (will be moved)'!$C$2</f>
@@ -3284,11 +3299,11 @@
       <c r="N7" t="s">
         <v>62</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="50">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="50" t="s">
         <v>60</v>
       </c>
       <c r="S7">
@@ -3343,11 +3358,11 @@
       <c r="N8" t="s">
         <v>62</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="50">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="50" t="s">
         <v>61</v>
       </c>
       <c r="S8">
@@ -3402,11 +3417,11 @@
       <c r="N9" t="s">
         <v>62</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="50">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="50" t="s">
         <v>60</v>
       </c>
       <c r="S9">
@@ -3461,11 +3476,11 @@
       <c r="N10" t="s">
         <v>62</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="50">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="50" t="s">
         <v>263</v>
       </c>
       <c r="S10">
@@ -3519,7 +3534,7 @@
       <c r="N11" t="s">
         <v>62</v>
       </c>
-      <c r="Q11" s="16"/>
+      <c r="Q11" s="51"/>
       <c r="R11" s="16"/>
       <c r="T11" s="16"/>
     </row>
@@ -3567,7 +3582,7 @@
       <c r="N12" t="s">
         <v>62</v>
       </c>
-      <c r="Q12" s="16"/>
+      <c r="Q12" s="51"/>
       <c r="R12" s="16"/>
       <c r="T12" s="16"/>
     </row>
@@ -3615,7 +3630,7 @@
       <c r="N13" t="s">
         <v>62</v>
       </c>
-      <c r="Q13" s="16"/>
+      <c r="Q13" s="51"/>
       <c r="R13" s="16"/>
       <c r="T13" s="16"/>
     </row>
@@ -3623,35 +3638,35 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="N14"/>
-      <c r="Q14" s="9"/>
+      <c r="Q14" s="51"/>
       <c r="R14" s="9"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
-      <c r="Q15" s="16"/>
+      <c r="Q15" s="51"/>
       <c r="R15" s="16"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
-      <c r="Q16" s="16"/>
+      <c r="Q16" s="51"/>
       <c r="R16" s="16"/>
     </row>
     <row r="17" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
-      <c r="Q17" s="16"/>
+      <c r="Q17" s="51"/>
       <c r="R17" s="16"/>
     </row>
     <row r="18" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
-      <c r="Q18" s="16"/>
+      <c r="Q18" s="51"/>
       <c r="R18" s="16"/>
     </row>
     <row r="19" spans="8:18" x14ac:dyDescent="0.25">
@@ -3668,21 +3683,21 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
-      <c r="Q21" s="16"/>
+      <c r="Q21" s="51"/>
       <c r="R21" s="16"/>
     </row>
     <row r="22" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
-      <c r="Q22" s="16"/>
+      <c r="Q22" s="51"/>
       <c r="R22" s="16"/>
     </row>
     <row r="23" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
-      <c r="Q23" s="16"/>
+      <c r="Q23" s="51"/>
       <c r="R23" s="16"/>
     </row>
     <row r="24" spans="8:18" x14ac:dyDescent="0.25">
@@ -3741,304 +3756,304 @@
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="O36"/>
+      <c r="O36" s="50"/>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="O37"/>
+      <c r="O37" s="50"/>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="O38"/>
+      <c r="O38" s="50"/>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
-      <c r="O39"/>
+      <c r="O39" s="50"/>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
-      <c r="O40"/>
+      <c r="O40" s="50"/>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
-      <c r="O41"/>
+      <c r="O41" s="50"/>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
-      <c r="O42"/>
+      <c r="O42" s="50"/>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
-      <c r="O43"/>
+      <c r="O43" s="50"/>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="N44"/>
-      <c r="O44"/>
+      <c r="O44" s="50"/>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
-      <c r="O45"/>
+      <c r="O45" s="50"/>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
-      <c r="O46"/>
+      <c r="O46" s="50"/>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
-      <c r="O47"/>
+      <c r="O47" s="50"/>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
-      <c r="O48"/>
+      <c r="O48" s="50"/>
     </row>
     <row r="49" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
-      <c r="O49"/>
+      <c r="O49" s="50"/>
     </row>
     <row r="50" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
-      <c r="O50"/>
+      <c r="O50" s="50"/>
     </row>
     <row r="51" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
-      <c r="O51"/>
+      <c r="O51" s="50"/>
     </row>
     <row r="52" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
-      <c r="O52"/>
+      <c r="O52" s="50"/>
     </row>
     <row r="53" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
-      <c r="O53"/>
+      <c r="O53" s="50"/>
     </row>
     <row r="54" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
-      <c r="O54"/>
+      <c r="O54" s="50"/>
     </row>
     <row r="55" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
-      <c r="O55"/>
+      <c r="O55" s="50"/>
     </row>
     <row r="56" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
-      <c r="O56"/>
+      <c r="O56" s="50"/>
     </row>
     <row r="57" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
-      <c r="O57"/>
+      <c r="O57" s="50"/>
     </row>
     <row r="58" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
-      <c r="O58"/>
+      <c r="O58" s="50"/>
     </row>
     <row r="59" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
-      <c r="O59"/>
+      <c r="O59" s="50"/>
     </row>
     <row r="60" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
-      <c r="O60"/>
+      <c r="O60" s="50"/>
     </row>
     <row r="61" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
-      <c r="O61"/>
+      <c r="O61" s="50"/>
     </row>
     <row r="62" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
-      <c r="O62"/>
+      <c r="O62" s="50"/>
     </row>
     <row r="63" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
-      <c r="O63"/>
+      <c r="O63" s="50"/>
     </row>
     <row r="64" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
-      <c r="O64"/>
+      <c r="O64" s="50"/>
     </row>
     <row r="65" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
-      <c r="O65"/>
+      <c r="O65" s="50"/>
     </row>
     <row r="66" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
-      <c r="O66"/>
+      <c r="O66" s="50"/>
     </row>
     <row r="67" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
-      <c r="O67"/>
+      <c r="O67" s="50"/>
     </row>
     <row r="68" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
-      <c r="O68"/>
+      <c r="O68" s="50"/>
     </row>
     <row r="69" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
-      <c r="O69"/>
+      <c r="O69" s="50"/>
     </row>
     <row r="70" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
-      <c r="O70"/>
+      <c r="O70" s="50"/>
     </row>
     <row r="71" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
-      <c r="O71"/>
+      <c r="O71" s="50"/>
     </row>
     <row r="72" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
-      <c r="O72"/>
+      <c r="O72" s="50"/>
     </row>
     <row r="73" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
-      <c r="O73"/>
+      <c r="O73" s="50"/>
     </row>
     <row r="74" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
-      <c r="O74"/>
+      <c r="O74" s="50"/>
     </row>
     <row r="75" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
-      <c r="O75"/>
+      <c r="O75" s="50"/>
     </row>
     <row r="76" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
-      <c r="O76"/>
+      <c r="O76" s="50"/>
     </row>
     <row r="77" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
-      <c r="O77"/>
+      <c r="O77" s="50"/>
     </row>
     <row r="78" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
-      <c r="O78"/>
+      <c r="O78" s="50"/>
     </row>
     <row r="79" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
-      <c r="O79"/>
+      <c r="O79" s="50"/>
     </row>
     <row r="80" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
-      <c r="O80"/>
+      <c r="O80" s="50"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
-      <c r="O81"/>
+      <c r="O81" s="50"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
-      <c r="O82"/>
+      <c r="O82" s="50"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
-      <c r="O83"/>
+      <c r="O83" s="50"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
-      <c r="O84"/>
+      <c r="O84" s="50"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
-      <c r="O85"/>
+      <c r="O85" s="50"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N86"/>
-      <c r="O86"/>
+      <c r="O86" s="50"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
@@ -4049,31 +4064,31 @@
       <c r="I87" s="4"/>
       <c r="M87" s="4"/>
       <c r="N87"/>
-      <c r="O87"/>
+      <c r="O87" s="50"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
-      <c r="O88"/>
+      <c r="O88" s="50"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
-      <c r="O89"/>
+      <c r="O89" s="50"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
-      <c r="O90"/>
+      <c r="O90" s="50"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
-      <c r="O91"/>
+      <c r="O91" s="50"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:T3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}"/>
@@ -4146,7 +4161,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>67</v>
@@ -8923,27 +8938,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -9206,10 +9200,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9232,20 +9258,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added: - Indicator mappings are now available in ScenarioData - Method to check fill method requirements (currently only method stub, no actual check currently) - Flow topology can now change per year (experimental) - FlowSolver now uses indicator mappings from ScenarioData - Building ODYM MFASystem now skips non-existent flows and uses value 0.0 for that flow
Fixed:
- Whitespace was not stripped when checking value for parameter fill_method. This caused false error saying "Fill method not allowed"

Removed:
- Removed "Conversion factor used", "Carbon content factor", and "Carbon content source" properties from Flow because Indicators allow general way to introduce conversion factors

Updated:
- Updated example_data.xlsx
- Updated example.ipynb
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B11B4C-CC0E-4E7D-B81F-E8C366A6227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8A1DE8-1B73-45B7-B8E9-12A1ECC36140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
@@ -24,8 +24,8 @@
     <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$T$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Processes!$D$3:$S$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$P$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Processes!$D$3:$R$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Settings!$B$6:$E$6</definedName>
     <definedName name="Boolean">'Data validation parameters'!$C$6:$C$7</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="263">
   <si>
     <t>Years</t>
   </si>
@@ -875,61 +875,6 @@
     <t>Ignore Excel columns defined in the list when reading data from Flows sheet. Each column name must be separated by comma (',')</t>
   </si>
   <si>
-    <t>Arbitrary extra metadata provided by user</t>
-  </si>
-  <si>
-    <t>User can add Excel column names parameter</t>
-  </si>
-  <si>
-    <t>Column names must be separated by comma</t>
-  </si>
-  <si>
-    <t>A,S</t>
-  </si>
-  <si>
-    <t>like this: A,S</t>
-  </si>
-  <si>
-    <t>All column names that are found on that list</t>
-  </si>
-  <si>
-    <t>are ignored when loading the data.</t>
-  </si>
-  <si>
-    <t>This column is ignored, check column S in this sheet for more details.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ignore_columns_processes</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in Settings-sheet.</t>
-    </r>
-  </si>
-  <si>
-    <t>This allows to add extra columns for notes or</t>
-  </si>
-  <si>
-    <t>other metadata.</t>
-  </si>
-  <si>
     <t>Process location</t>
   </si>
   <si>
@@ -987,27 +932,9 @@
     <t>Data source comment</t>
   </si>
   <si>
-    <t>Conversion factor used</t>
-  </si>
-  <si>
-    <t>Carbon content conversion</t>
-  </si>
-  <si>
-    <t>Carbon content conversion source</t>
-  </si>
-  <si>
     <t>Assumed density of a furniture product 450 kg/m3</t>
   </si>
   <si>
-    <t>Ignored column, indicators start after this column</t>
-  </si>
-  <si>
-    <t>Ignored column</t>
-  </si>
-  <si>
-    <t>A,R</t>
-  </si>
-  <si>
     <t>baseline_value_name</t>
   </si>
   <si>
@@ -1029,13 +956,22 @@
     <t>2 columns needed for each indicator (name and comment)</t>
   </si>
   <si>
-    <t>New parameter</t>
-  </si>
-  <si>
     <t>Reduce sawmilling residues by 50%</t>
   </si>
   <si>
     <t>Solid wood equivalent</t>
+  </si>
+  <si>
+    <t>show_plots</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>This column is ignored (check parameter ignore_columns_processes in Settings-sheet)</t>
+  </si>
+  <si>
+    <t>This column is ignored (check parameter ignore_columns_flows in Settings-sheet)</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +983,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1112,17 +1048,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1150,18 +1077,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1220,7 +1135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1295,9 +1210,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1310,15 +1222,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1399,7 +1303,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1002229</xdr:colOff>
+      <xdr:colOff>192604</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>167367</xdr:rowOff>
     </xdr:to>
@@ -1756,10 +1660,10 @@
       <c r="B1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="44"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
@@ -1768,10 +1672,10 @@
       <c r="B2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,10 +1685,10 @@
       <c r="B3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:5" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
@@ -1793,10 +1697,10 @@
       <c r="B4" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
@@ -1805,10 +1709,10 @@
       <c r="B5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
@@ -1817,10 +1721,10 @@
       <c r="B6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
@@ -1829,10 +1733,10 @@
       <c r="B7" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="D7" s="43"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
@@ -1841,10 +1745,10 @@
       <c r="B8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="45"/>
+      <c r="D8" s="42"/>
     </row>
     <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
@@ -1853,10 +1757,10 @@
       <c r="B9" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
@@ -1865,10 +1769,10 @@
       <c r="B10" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="43"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
@@ -1877,10 +1781,10 @@
       <c r="B11" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="40" t="s">
         <v>221</v>
       </c>
-      <c r="D11" s="43"/>
+      <c r="D11" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1903,32 +1807,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="A2:E31"/>
+  <dimension ref="B2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="91.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="115.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="25" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>144</v>
       </c>
@@ -1936,7 +1840,7 @@
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>125</v>
       </c>
@@ -1950,7 +1854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>126</v>
       </c>
@@ -1964,24 +1868,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B8" s="40" t="s">
+    <row r="8" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="D8" s="40" t="s">
+      <c r="C8" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="44" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>127</v>
       </c>
@@ -1995,7 +1896,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>128</v>
       </c>
@@ -2009,24 +1910,21 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B11" s="40" t="s">
+    <row r="11" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="C11" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="D11" s="40" t="s">
+      <c r="C11" s="44" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="44" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>129</v>
       </c>
@@ -2040,7 +1938,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>133</v>
       </c>
@@ -2054,7 +1952,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>135</v>
       </c>
@@ -2068,7 +1966,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>136</v>
       </c>
@@ -2082,7 +1980,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>139</v>
       </c>
@@ -2096,7 +1994,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>147</v>
       </c>
@@ -2110,41 +2008,35 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" s="40" t="s">
+    <row r="18" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="E18" s="40" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="D19" s="40" t="s">
+      <c r="E18" s="44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="D19" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="E19" s="40" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>141</v>
       </c>
@@ -2158,7 +2050,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>157</v>
       </c>
@@ -2172,7 +2064,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>156</v>
       </c>
@@ -2186,7 +2078,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>165</v>
       </c>
@@ -2200,7 +2092,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>172</v>
       </c>
@@ -2214,26 +2106,23 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="D25" s="40" t="s">
+    <row r="25" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="E25" s="40" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="44" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>175</v>
       </c>
       <c r="C26" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>159</v>
@@ -2242,12 +2131,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>177</v>
       </c>
       <c r="C27" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>159</v>
@@ -2256,7 +2145,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>197</v>
       </c>
@@ -2270,7 +2159,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>217</v>
       </c>
@@ -2284,21 +2173,25 @@
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="D30" s="40" t="s">
+    <row r="30" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="D30" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="E30" s="40" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E30" s="44" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>259</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B6:E6" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}"/>
   <conditionalFormatting sqref="C15:C16">
@@ -2349,10 +2242,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2374,10 +2267,9 @@
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -2428,11 +2320,8 @@
       <c r="R1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2457,47 +2346,46 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-    </row>
-    <row r="3" spans="1:19" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>87</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>122</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="H3" s="22" t="s">
         <v>151</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="L3" s="22" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="N3" s="22" t="s">
         <v>16</v>
@@ -2514,11 +2402,8 @@
       <c r="R3" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="22" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2554,11 +2439,8 @@
       <c r="R4" t="s">
         <v>201</v>
       </c>
-      <c r="S4" s="41" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2594,11 +2476,8 @@
       <c r="R5" t="s">
         <v>202</v>
       </c>
-      <c r="S5" s="41" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2633,11 +2512,8 @@
       <c r="R6" t="s">
         <v>203</v>
       </c>
-      <c r="S6" s="41" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2672,11 +2548,8 @@
       <c r="R7" t="s">
         <v>204</v>
       </c>
-      <c r="S7" s="41" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2711,9 +2584,8 @@
       <c r="R8" t="s">
         <v>205</v>
       </c>
-      <c r="S8" s="41"/>
-    </row>
-    <row r="9" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2748,11 +2620,8 @@
       <c r="R9" t="s">
         <v>209</v>
       </c>
-      <c r="S9" s="41" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2787,11 +2656,8 @@
       <c r="R10" t="s">
         <v>206</v>
       </c>
-      <c r="S10" s="41" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2826,11 +2692,8 @@
       <c r="R11" t="s">
         <v>207</v>
       </c>
-      <c r="S11" s="41" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2864,9 +2727,6 @@
       </c>
       <c r="R12" t="s">
         <v>208</v>
-      </c>
-      <c r="S12" s="41" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2907,37 +2767,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
-  <dimension ref="A1:T91"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26" style="49" customWidth="1"/>
-    <col min="16" max="16" width="29.28515625" style="50" customWidth="1"/>
-    <col min="17" max="17" width="45.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="45.7109375" customWidth="1"/>
-    <col min="19" max="19" width="57.42578125" customWidth="1"/>
-    <col min="20" max="20" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2980,24 +2836,14 @@
       <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3016,42 +2862,38 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="T2" s="3"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>265</v>
+      <c r="O2" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>262</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>253</v>
-      </c>
       <c r="E3" s="12" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>120</v>
@@ -3063,31 +2905,19 @@
         <v>46</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="O3" s="48" t="s">
-        <v>260</v>
-      </c>
-      <c r="P3" s="48" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q3" s="48" t="s">
-        <v>262</v>
-      </c>
-      <c r="R3" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="T3" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="P3" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -3131,19 +2961,13 @@
       <c r="N4" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="50">
+      <c r="O4">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="16"/>
-      <c r="S4">
-        <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.20342399999999999</v>
-      </c>
-      <c r="T4" s="16"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P4" s="16"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -3187,19 +3011,13 @@
       <c r="N5" t="s">
         <v>62</v>
       </c>
-      <c r="P5" s="50">
+      <c r="O5">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="16"/>
-      <c r="S5">
-        <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.20342399999999999</v>
-      </c>
-      <c r="T5" s="16"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -3243,19 +3061,13 @@
       <c r="N6" t="s">
         <v>62</v>
       </c>
-      <c r="P6" s="50">
+      <c r="O6">
         <f>0.395*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.18959999999999999</v>
       </c>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="16"/>
-      <c r="S6">
-        <f>0.395*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.18959999999999999</v>
-      </c>
-      <c r="T6" s="16"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P6" s="16"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3299,22 +3111,15 @@
       <c r="N7" t="s">
         <v>62</v>
       </c>
-      <c r="P7" s="50">
+      <c r="O7">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
-      <c r="Q7" s="50" t="s">
+      <c r="P7" t="s">
         <v>60</v>
       </c>
-      <c r="S7">
-        <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.23039999999999999</v>
-      </c>
-      <c r="T7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -3358,22 +3163,15 @@
       <c r="N8" t="s">
         <v>62</v>
       </c>
-      <c r="P8" s="50">
+      <c r="O8">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
-      <c r="Q8" s="50" t="s">
+      <c r="P8" t="s">
         <v>61</v>
       </c>
-      <c r="S8">
-        <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.216</v>
-      </c>
-      <c r="T8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -3417,22 +3215,15 @@
       <c r="N9" t="s">
         <v>62</v>
       </c>
-      <c r="P9" s="50">
+      <c r="O9">
         <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.23039999999999999</v>
       </c>
-      <c r="Q9" s="50" t="s">
+      <c r="P9" t="s">
         <v>60</v>
       </c>
-      <c r="S9">
-        <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.23039999999999999</v>
-      </c>
-      <c r="T9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -3476,22 +3267,15 @@
       <c r="N10" t="s">
         <v>62</v>
       </c>
-      <c r="P10" s="50">
+      <c r="O10">
         <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.216</v>
       </c>
-      <c r="Q10" s="50" t="s">
-        <v>263</v>
-      </c>
-      <c r="S10">
-        <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.216</v>
-      </c>
-      <c r="T10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -3534,11 +3318,9 @@
       <c r="N11" t="s">
         <v>62</v>
       </c>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="16"/>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -3582,11 +3364,9 @@
       <c r="N12" t="s">
         <v>62</v>
       </c>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="16"/>
-      <c r="T12" s="16"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -3630,432 +3410,363 @@
       <c r="N13" t="s">
         <v>62</v>
       </c>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="16"/>
-      <c r="T13" s="16"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="N14"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="9"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="16"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="16"/>
-    </row>
-    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="16"/>
-    </row>
-    <row r="18" spans="8:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="16"/>
-    </row>
-    <row r="19" spans="8:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="16"/>
-    </row>
-    <row r="22" spans="8:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="16"/>
-    </row>
-    <row r="23" spans="8:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="16"/>
-    </row>
-    <row r="24" spans="8:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E35" s="16" t="s">
         <v>155</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="O36" s="50"/>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="O37" s="50"/>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="O38" s="50"/>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
-      <c r="O39" s="50"/>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
-      <c r="O40" s="50"/>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
-      <c r="O41" s="50"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
-      <c r="O42" s="50"/>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
-      <c r="O43" s="50"/>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="N44"/>
-      <c r="O44" s="50"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
-      <c r="O45" s="50"/>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
-      <c r="O46" s="50"/>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
-      <c r="O47" s="50"/>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
-      <c r="O48" s="50"/>
-    </row>
-    <row r="49" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
-      <c r="O49" s="50"/>
-    </row>
-    <row r="50" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
-      <c r="O50" s="50"/>
-    </row>
-    <row r="51" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
-      <c r="O51" s="50"/>
-    </row>
-    <row r="52" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
-      <c r="O52" s="50"/>
-    </row>
-    <row r="53" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
-      <c r="O53" s="50"/>
-    </row>
-    <row r="54" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
-      <c r="O54" s="50"/>
-    </row>
-    <row r="55" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
-      <c r="O55" s="50"/>
-    </row>
-    <row r="56" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
-      <c r="O56" s="50"/>
-    </row>
-    <row r="57" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
-      <c r="O57" s="50"/>
-    </row>
-    <row r="58" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
-      <c r="O58" s="50"/>
-    </row>
-    <row r="59" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
-      <c r="O59" s="50"/>
-    </row>
-    <row r="60" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
-      <c r="O60" s="50"/>
-    </row>
-    <row r="61" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
-      <c r="O61" s="50"/>
-    </row>
-    <row r="62" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
-      <c r="O62" s="50"/>
-    </row>
-    <row r="63" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
-      <c r="O63" s="50"/>
-    </row>
-    <row r="64" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
-      <c r="O64" s="50"/>
-    </row>
-    <row r="65" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
-      <c r="O65" s="50"/>
-    </row>
-    <row r="66" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
-      <c r="O66" s="50"/>
-    </row>
-    <row r="67" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
-      <c r="O67" s="50"/>
-    </row>
-    <row r="68" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
-      <c r="O68" s="50"/>
-    </row>
-    <row r="69" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
-      <c r="O69" s="50"/>
-    </row>
-    <row r="70" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
-      <c r="O70" s="50"/>
-    </row>
-    <row r="71" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
-      <c r="O71" s="50"/>
-    </row>
-    <row r="72" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
-      <c r="O72" s="50"/>
-    </row>
-    <row r="73" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
-      <c r="O73" s="50"/>
-    </row>
-    <row r="74" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
-      <c r="O74" s="50"/>
-    </row>
-    <row r="75" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
-      <c r="O75" s="50"/>
-    </row>
-    <row r="76" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
-      <c r="O76" s="50"/>
-    </row>
-    <row r="77" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
-      <c r="O77" s="50"/>
-    </row>
-    <row r="78" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
-      <c r="O78" s="50"/>
-    </row>
-    <row r="79" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
-      <c r="O79" s="50"/>
-    </row>
-    <row r="80" spans="8:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
-      <c r="O80" s="50"/>
-    </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
-      <c r="O81" s="50"/>
-    </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
-      <c r="O82" s="50"/>
-    </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
-      <c r="O83" s="50"/>
-    </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
-      <c r="O84" s="50"/>
-    </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
-      <c r="O85" s="50"/>
-    </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N86"/>
-      <c r="O86" s="50"/>
-    </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -4064,34 +3775,29 @@
       <c r="I87" s="4"/>
       <c r="M87" s="4"/>
       <c r="N87"/>
-      <c r="O87" s="50"/>
-    </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
-      <c r="O88" s="50"/>
-    </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
-      <c r="O89" s="50"/>
-    </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
-      <c r="O90" s="50"/>
-    </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
-      <c r="O91" s="50"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:T3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}"/>
+  <autoFilter ref="A3:P3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E35" r:id="rId1" location="json=TH95eCDBsN1pfqczsMf84,S3TGIZvZiI-AUl8oZJcUYg" xr:uid="{26F0F99B-4281-4D67-B3C8-B1BC12D732B7}"/>
@@ -4161,7 +3867,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>67</v>
@@ -4217,7 +3923,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8938,6 +8644,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -9200,28 +8927,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9238,29 +8969,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed: - Updated example_data.xlsx
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8A1DE8-1B73-45B7-B8E9-12A1ECC36140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A93CEB9-3C8D-4050-876E-D7DFB7429751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="265">
   <si>
     <t>Years</t>
   </si>
@@ -690,9 +690,6 @@
     <t>Change in value (delta)</t>
   </si>
   <si>
-    <t>Target value (potentially)</t>
-  </si>
-  <si>
     <t>Change type (Value or % = proportional)</t>
   </si>
   <si>
@@ -972,6 +969,15 @@
   </si>
   <si>
     <t>This column is ignored (check parameter ignore_columns_flows in Settings-sheet)</t>
+  </si>
+  <si>
+    <t>use_scenarios</t>
+  </si>
+  <si>
+    <t>Run scenarios. Default value is True.</t>
+  </si>
+  <si>
+    <t>Target value</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1222,7 +1228,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1782,7 +1787,7 @@
         <v>100</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D11" s="40"/>
     </row>
@@ -1807,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E31"/>
+  <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,18 +1873,18 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>260</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>228</v>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -1910,18 +1915,18 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
-        <v>227</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>260</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>229</v>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -2008,32 +2013,32 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>250</v>
       </c>
-      <c r="C18" s="44" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="44" t="s">
+      <c r="C19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D19" t="s">
         <v>161</v>
       </c>
-      <c r="E18" s="44" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="44" t="s">
+      <c r="E19" t="s">
         <v>251</v>
-      </c>
-      <c r="C19" s="44" t="s">
-        <v>254</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -2089,51 +2094,51 @@
         <v>162</v>
       </c>
       <c r="E23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>172</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>173</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>161</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="s">
-        <v>237</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>175</v>
-      </c>
-      <c r="C26" s="30" t="b">
-        <v>1</v>
+        <v>236</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="E26" t="s">
-        <v>176</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C27" s="30" t="b">
         <v>1</v>
@@ -2142,53 +2147,67 @@
         <v>159</v>
       </c>
       <c r="E27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>197</v>
-      </c>
-      <c r="C28" t="s">
-        <v>200</v>
+        <v>177</v>
+      </c>
+      <c r="C28" s="30" t="b">
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="D30" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" t="s">
         <v>218</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="E29" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="44" t="s">
-        <v>238</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>259</v>
-      </c>
-      <c r="C31" t="b">
+        <v>237</v>
+      </c>
+      <c r="D31" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C32" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2210,7 +2229,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+  <conditionalFormatting sqref="C27:C28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -2219,7 +2238,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C21:C22 C26:C27" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C21:C22 C27:C28" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
@@ -2232,7 +2251,7 @@
           <x14:formula1>
             <xm:f>'Data validation parameters'!$D$6:$D$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C23</xm:sqref>
+          <xm:sqref>C23:C24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2349,43 +2368,43 @@
     </row>
     <row r="3" spans="1:18" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>87</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>122</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H3" s="22" t="s">
         <v>151</v>
       </c>
       <c r="I3" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="K3" s="22" t="s">
         <v>234</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>235</v>
       </c>
       <c r="L3" s="22" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N3" s="22" t="s">
         <v>16</v>
@@ -2437,7 +2456,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -2474,7 +2493,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2510,7 +2529,7 @@
         <v>0.05</v>
       </c>
       <c r="R6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2546,7 +2565,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2582,7 +2601,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2618,7 +2637,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2654,7 +2673,7 @@
         <v>0.9</v>
       </c>
       <c r="R10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2690,7 +2709,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2726,7 +2745,7 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2863,37 +2882,37 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>246</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>120</v>
@@ -2905,13 +2924,13 @@
         <v>46</v>
       </c>
       <c r="M3" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>248</v>
-      </c>
       <c r="O3" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>17</v>
@@ -3272,7 +3291,7 @@
         <v>0.216</v>
       </c>
       <c r="P10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3812,8 +3831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,30 +3863,30 @@
         <v>182</v>
       </c>
       <c r="E1" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="F1" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="J1" s="32" t="s">
-        <v>188</v>
-      </c>
       <c r="K1" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>67</v>
@@ -3888,7 +3907,7 @@
         <v>2030</v>
       </c>
       <c r="I2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3934,10 +3953,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3945,7 +3964,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3953,7 +3972,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3961,7 +3980,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3969,7 +3988,7 @@
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3977,7 +3996,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3985,7 +4004,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3993,18 +4012,18 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -4033,12 +4052,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -4052,10 +4071,10 @@
         <v>165</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -4072,7 +4091,7 @@
         <v>120</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -4089,7 +4108,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -4100,7 +4119,7 @@
         <v>169</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -4111,7 +4130,7 @@
         <v>170</v>
       </c>
       <c r="F9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated: added LandfillDecayWood and LandfillDecay paper distribution types / stock decays and updated message on the stock distribution parameters. Included: prioritize_locations and prioritize_transformation_stage parameters in settings.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25526E34-0A8C-498B-99FB-E725FD5F9B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119AD5DF-2ABA-4563-BF0B-54C763DCB429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="236">
   <si>
     <t>Years</t>
   </si>
@@ -533,9 +533,6 @@
     <t>fill_method</t>
   </si>
   <si>
-    <t>Previous</t>
-  </si>
-  <si>
     <t>Interpolate</t>
   </si>
   <si>
@@ -872,6 +869,27 @@
   </si>
   <si>
     <t xml:space="preserve">Target value </t>
+  </si>
+  <si>
+    <t>prioritize_locations</t>
+  </si>
+  <si>
+    <t>stddev=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priotize flows based on their transformation stage (e.g., Second). This functionality prioritizes / reduces the specific flows from entering the stock so they occur on the same timestep. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priotize flows based on their location (e.g., Export). This functionality prioritizes / reduces exports from entering the stock so they occur on the same timestep. </t>
+  </si>
+  <si>
+    <t>LandfillDecayWood</t>
+  </si>
+  <si>
+    <t>LandfillDecayPaper</t>
+  </si>
+  <si>
+    <t>prioritize_transformation_stage</t>
   </si>
 </sst>
 </file>
@@ -1243,6 +1261,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1684,7 +1706,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11" s="36"/>
     </row>
@@ -1709,10 +1731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E32"/>
+  <dimension ref="B2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,16 +1794,16 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -1814,16 +1836,16 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1912,30 +1934,30 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D18" t="s">
         <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D19" t="s">
         <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1985,18 +2007,18 @@
         <v>130</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D23" t="s">
         <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C24" s="27" t="b">
         <v>0</v>
@@ -2005,37 +2027,37 @@
         <v>124</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" t="s">
         <v>137</v>
-      </c>
-      <c r="C25" t="s">
-        <v>138</v>
       </c>
       <c r="D25" t="s">
         <v>126</v>
       </c>
       <c r="E25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C27" s="27" t="b">
         <v>1</v>
@@ -2044,12 +2066,12 @@
         <v>124</v>
       </c>
       <c r="E27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" s="27" t="b">
         <v>1</v>
@@ -2058,54 +2080,73 @@
         <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" t="s">
         <v>161</v>
-      </c>
-      <c r="C29" t="s">
-        <v>164</v>
-      </c>
-      <c r="D29" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>182</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>223</v>
-      </c>
-      <c r="C32" t="b">
-        <v>0</v>
+        <v>222</v>
+      </c>
+      <c r="D32" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>229</v>
+      </c>
+      <c r="D33" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2142,7 +2183,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C21:C22 C27:C28 C24" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
       <formula1>Boolean</formula1>
     </dataValidation>
@@ -2151,7 +2192,7 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A95900C-A9EB-48AB-A762-0F120DA62856}">
           <x14:formula1>
             <xm:f>'Data validation parameters'!$D$6:$D$9</xm:f>
@@ -2169,7 +2210,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,43 +2314,43 @@
     </row>
     <row r="3" spans="1:18" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>65</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>119</v>
       </c>
       <c r="I3" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>198</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>199</v>
       </c>
       <c r="L3" s="19" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N3" s="19" t="s">
         <v>16</v>
@@ -2350,9 +2391,6 @@
       <c r="H4" t="s">
         <v>84</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="M4" s="5"/>
       <c r="P4">
         <v>3.6999999999999998E-2</v>
@@ -2361,7 +2399,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -2387,9 +2425,6 @@
       <c r="H5" t="s">
         <v>84</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="M5" s="5"/>
       <c r="P5">
         <v>0.24299999999999999</v>
@@ -2398,7 +2433,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2424,9 +2459,6 @@
       <c r="H6" t="s">
         <v>84</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
       <c r="P6">
         <v>0.40899999999999997</v>
       </c>
@@ -2434,7 +2466,7 @@
         <v>0.05</v>
       </c>
       <c r="R6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2460,9 +2492,6 @@
       <c r="H7" t="s">
         <v>84</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
       <c r="P7">
         <v>0.40899999999999997</v>
       </c>
@@ -2470,7 +2499,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2496,8 +2525,8 @@
       <c r="H8" t="s">
         <v>58</v>
       </c>
-      <c r="I8">
-        <v>1</v>
+      <c r="I8" t="s">
+        <v>230</v>
       </c>
       <c r="P8">
         <v>0.752</v>
@@ -2506,7 +2535,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2532,8 +2561,8 @@
       <c r="H9" t="s">
         <v>58</v>
       </c>
-      <c r="I9">
-        <v>1</v>
+      <c r="I9" t="s">
+        <v>230</v>
       </c>
       <c r="P9">
         <v>0.65600000000000003</v>
@@ -2542,7 +2571,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2568,9 +2597,6 @@
       <c r="H10" t="s">
         <v>84</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
       <c r="P10">
         <v>0.24299999999999999</v>
       </c>
@@ -2578,7 +2604,7 @@
         <v>0.9</v>
       </c>
       <c r="R10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2604,9 +2630,6 @@
       <c r="H11" t="s">
         <v>84</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
       <c r="P11">
         <v>0.69099999999999995</v>
       </c>
@@ -2614,7 +2637,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2640,9 +2663,6 @@
       <c r="H12" t="s">
         <v>84</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
       <c r="P12">
         <v>0.96599999999999997</v>
       </c>
@@ -2650,38 +2670,26 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations xWindow="794" yWindow="485" count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameter" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I4:I1048576" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
+  <dataValidations xWindow="1088" yWindow="385" count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="see parameters.py for more info" prompt="tuple = number or list of parameters separated by comma. Example: stddev=1. For shape and scale list separated by comma e.g., shape=1, scale=1.5_x000a_Normal: stddev_x000a_LogNormal: stddev_x000a_FoldedNormal: stddev_x000a_Weibull: shape, scale_x000a_LandfillDecayWood /Pap: condition_x000a_" sqref="I4:I1048576" xr:uid="{564AD8C3-F96D-40DD-BFD1-1C6E073701B7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sankey diagram positioning" prompt="Sankey diagram X and Y node positioning. Check / adjust positioning after you run case and see coordinates. " sqref="Q2 P4:Q1048576" xr:uid="{167D7519-74A2-4731-8D99-C2A980321CC9}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="794" yWindow="485" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{0258C8E4-0AAB-48FF-93D5-AADF99BF39C4}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1088" yWindow="385" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA69398A-0340-441A-BF0A-578EFEF6082C}">
           <x14:formula1>
-            <xm:f>'Data validation parameters'!$B$6:$B$10</xm:f>
+            <xm:f>'Data validation parameters'!$B$6:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>H16:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{61770E9E-9EFD-4B63-8C83-80C1E833E691}">
-          <x14:formula1>
-            <xm:f>'Data validation parameters'!$B$6:$B$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>H4:H8 H10:H15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. _x000a_-Simple only uses lifetimes so no parameter is used." xr:uid="{23F636B4-40CE-4150-A9BF-BE3BC7637520}">
-          <x14:formula1>
-            <xm:f>'Data validation parameters'!$B$6:$B$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>H9</xm:sqref>
+          <xm:sqref>H4:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2693,8 +2701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,37 +2795,37 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>210</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>88</v>
@@ -2829,13 +2837,13 @@
         <v>46</v>
       </c>
       <c r="M3" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>212</v>
-      </c>
       <c r="O3" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>17</v>
@@ -3196,7 +3204,7 @@
         <v>0.216</v>
       </c>
       <c r="P10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3737,7 +3745,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3756,42 +3764,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="H1" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="I1" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="28" t="s">
-        <v>152</v>
-      </c>
       <c r="K1" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>63</v>
@@ -3812,7 +3820,7 @@
         <v>2030</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3858,10 +3866,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3869,7 +3877,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3877,7 +3885,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,7 +3893,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3893,7 +3901,7 @@
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3901,7 +3909,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3909,7 +3917,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3917,18 +3925,18 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3939,10 +3947,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
-  <dimension ref="B2:F11"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3957,12 +3965,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -3976,10 +3984,10 @@
         <v>130</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -3990,13 +3998,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
         <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -4007,13 +4015,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -4021,10 +4029,10 @@
         <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -4032,10 +4040,10 @@
         <v>87</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -4045,7 +4053,17 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4091,27 +4109,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -4374,32 +4371,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4416,4 +4409,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated: - Updated example_data.xlsx to include parameter scenario_type with data validation - Updated example.ipynb
Added:
- Added logging using the logger in FlowModifierSolver.py
- Added colors to logger.py depending on level of logging ("info"=green, "error"=red, "debug"=red)
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119AD5DF-2ABA-4563-BF0B-54C763DCB429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ACA156-5638-4DCF-B94B-4979D3CE4BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="239">
   <si>
     <t>Years</t>
   </si>
@@ -850,9 +850,6 @@
     <t>Solid wood equivalent</t>
   </si>
   <si>
-    <t>show_plots</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -890,12 +887,24 @@
   </si>
   <si>
     <t>prioritize_transformation_stage</t>
+  </si>
+  <si>
+    <t>scenario_type</t>
+  </si>
+  <si>
+    <t>Scenario Type</t>
+  </si>
+  <si>
+    <t>Constrained</t>
+  </si>
+  <si>
+    <t>Unconstrained</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1195,7 +1204,9 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{BFED7886-AC9B-497E-9417-A24357F5C604}"/>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFCC0000"/>
@@ -1259,10 +1270,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1733,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="B2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1804,7 @@
         <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
         <v>162</v>
@@ -1839,7 +1846,7 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" t="s">
         <v>162</v>
@@ -2018,7 +2025,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C24" s="27" t="b">
         <v>0</v>
@@ -2027,51 +2034,45 @@
         <v>124</v>
       </c>
       <c r="E24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>136</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" t="s">
-        <v>138</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>200</v>
+        <v>136</v>
+      </c>
+      <c r="C26" t="s">
+        <v>137</v>
       </c>
       <c r="D26" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="E26" t="s">
-        <v>202</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="27" t="b">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="E27" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" s="27" t="b">
         <v>1</v>
@@ -2080,62 +2081,65 @@
         <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" t="s">
-        <v>163</v>
+        <v>141</v>
+      </c>
+      <c r="C29" s="27" t="b">
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="E29" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>180</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>126</v>
+        <v>160</v>
+      </c>
+      <c r="C30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" t="s">
+        <v>162</v>
       </c>
       <c r="E30" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>201</v>
-      </c>
-      <c r="D31" t="s">
-        <v>162</v>
-      </c>
-      <c r="E31" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>222</v>
       </c>
       <c r="D32" t="s">
         <v>162</v>
       </c>
       <c r="E32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D33" t="s">
         <v>162</v>
@@ -2146,7 +2150,13 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="D34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2175,7 +2185,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:C28">
+  <conditionalFormatting sqref="C28:C29">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -2183,8 +2193,8 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C21:C22 C27:C28 C24" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C21:C22 C28:C29 C24" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
@@ -2192,12 +2202,18 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A95900C-A9EB-48AB-A762-0F120DA62856}">
           <x14:formula1>
             <xm:f>'Data validation parameters'!$D$6:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>C23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A04E2A2-4928-4E28-9F6D-7D556381B8E8}">
+          <x14:formula1>
+            <xm:f>'Data validation parameters'!$G$6:$G$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2210,7 +2226,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2330,7 @@
     </row>
     <row r="3" spans="1:18" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>89</v>
@@ -2526,7 +2542,7 @@
         <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P8">
         <v>0.752</v>
@@ -2562,7 +2578,7 @@
         <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P9">
         <v>0.65600000000000003</v>
@@ -2801,7 +2817,7 @@
     </row>
     <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>204</v>
@@ -3776,7 +3792,7 @@
         <v>146</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F1" s="28" t="s">
         <v>147</v>
@@ -3947,10 +3963,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3960,20 +3976,21 @@
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>119</v>
       </c>
@@ -3989,8 +4006,11 @@
       <c r="F5" s="21" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>84</v>
       </c>
@@ -4006,8 +4026,11 @@
       <c r="F6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -4023,8 +4046,11 @@
       <c r="F7" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>85</v>
       </c>
@@ -4035,7 +4061,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>87</v>
       </c>
@@ -4046,24 +4072,24 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4109,6 +4135,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -4371,7 +4409,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4380,19 +4418,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4411,27 +4454,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated: - Toggled on scenarios in example_data.xlsx - Added description to parameter scenario_type in example_data.xlsx - Constrained scenario solving uses now Unconstrained solver until implementation is ready, message can be seen in runtime about this (FlowModifierSolver.py)
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ACA156-5638-4DCF-B94B-4979D3CE4BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85440CF2-9352-474B-B1EF-C544CA4C5415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="240">
   <si>
     <t>Years</t>
   </si>
@@ -899,6 +899,9 @@
   </si>
   <si>
     <t>Unconstrained</t>
+  </si>
+  <si>
+    <t>Scenario type (Constrained / Unconstrained)</t>
   </si>
 </sst>
 </file>
@@ -1740,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="B2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2031,7 @@
         <v>225</v>
       </c>
       <c r="C24" s="27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
         <v>124</v>
@@ -2042,7 +2045,13 @@
         <v>235</v>
       </c>
       <c r="C25" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="D25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated: Step 5 so removal / sink results are negative and emissions positive. Also made some changes related to this on the captions. Make sure that conversion_factor_c_to_co2 is defined as negative parameter (-44/12) in the input file.
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85440CF2-9352-474B-B1EF-C544CA4C5415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC38B5B6-B695-45B5-9DFB-3D9D97B8282A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28910" yWindow="30" windowWidth="29020" windowHeight="15700" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -1578,16 +1578,16 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" style="30" customWidth="1"/>
     <col min="3" max="3" width="29" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="10"/>
+    <col min="4" max="4" width="69.54296875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="D1" s="37"/>
     </row>
-    <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="135.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -1612,7 +1612,7 @@
       <c r="D2" s="36"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="D3" s="36"/>
     </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>30</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="D4" s="39"/>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>39</v>
       </c>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="D5" s="36"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
         <v>28</v>
       </c>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="D6" s="38"/>
     </row>
-    <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>33</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="D7" s="36"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>35</v>
       </c>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="D8" s="38"/>
     </row>
-    <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="31" t="s">
         <v>44</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="D9" s="36"/>
     </row>
-    <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
         <v>66</v>
       </c>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="D10" s="36"/>
     </row>
-    <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>68</v>
       </c>
@@ -1744,29 +1744,29 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="91.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="115.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="2" width="91.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="115.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>112</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
         <v>93</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>94</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>189</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>95</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>96</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>190</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>97</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>101</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>103</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>104</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>107</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>115</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>213</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>214</v>
       </c>
@@ -1970,12 +1970,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>109</v>
       </c>
       <c r="C20" s="23">
-        <v>3.67</v>
+        <v>-3.6666666666666701</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>128</v>
@@ -1984,7 +1984,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>122</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>121</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>130</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>225</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>235</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>136</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>200</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>139</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>141</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>160</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>180</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>201</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>228</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>234</v>
       </c>
@@ -2238,28 +2238,28 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" customWidth="1"/>
+    <col min="13" max="13" width="18.26953125" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -2311,7 +2311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2337,7 +2337,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="20" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>223</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations xWindow="1088" yWindow="385" count="2">
@@ -2730,27 +2730,27 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7265625" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>224</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -2924,7 +2924,7 @@
       </c>
       <c r="P4" s="16"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="P5" s="16"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="P6" s="16"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="P11" s="16"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -3323,7 +3323,7 @@
       </c>
       <c r="P12" s="16"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -3369,361 +3369,361 @@
       </c>
       <c r="P13" s="16"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
     </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.35">
       <c r="E35" s="16" t="s">
         <v>120</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
     </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
     </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="N44"/>
     </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
     </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
     </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
     </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.35">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
     </row>
-    <row r="49" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
     </row>
-    <row r="50" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
     </row>
-    <row r="51" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
     </row>
-    <row r="52" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
     </row>
-    <row r="53" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
     </row>
-    <row r="54" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
     </row>
-    <row r="55" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
     </row>
-    <row r="56" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
     </row>
-    <row r="57" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
     </row>
-    <row r="58" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
     </row>
-    <row r="59" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
     </row>
-    <row r="60" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
     </row>
-    <row r="61" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
     </row>
-    <row r="62" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
     </row>
-    <row r="63" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
     </row>
-    <row r="64" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
     </row>
-    <row r="65" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
     </row>
-    <row r="66" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
     </row>
-    <row r="67" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
     </row>
-    <row r="68" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
     </row>
-    <row r="69" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
     </row>
-    <row r="70" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
     </row>
-    <row r="71" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
     </row>
-    <row r="72" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
     </row>
-    <row r="73" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
     </row>
-    <row r="74" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
     </row>
-    <row r="75" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
     </row>
-    <row r="76" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
     </row>
-    <row r="77" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
     </row>
-    <row r="79" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:14" x14ac:dyDescent="0.35">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.35">
       <c r="N86"/>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3733,22 +3733,22 @@
       <c r="M87" s="4"/>
       <c r="N87"/>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.35">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
@@ -3773,21 +3773,21 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="52.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>143</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>220</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
@@ -3883,13 +3883,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>173</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -3978,28 +3978,28 @@
       <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
         <v>119</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>84</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>85</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>87</v>
       </c>
@@ -4081,22 +4081,22 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>233</v>
       </c>
@@ -4115,19 +4115,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>71</v>
       </c>
@@ -4144,18 +4144,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -4418,6 +4406,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4428,23 +4428,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4463,6 +4446,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Changed: - Updated example data to include sheet "Process positions" - Updated example.ipynb
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\aiphoria\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC38B5B6-B695-45B5-9DFB-3D9D97B8282A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB3299C-762D-469F-BAE7-BA1855023F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28910" yWindow="30" windowWidth="29020" windowHeight="15700" firstSheet="1" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
     <sheet name="Settings" sheetId="11" r:id="rId2"/>
     <sheet name="Processes" sheetId="6" r:id="rId3"/>
     <sheet name="Flows" sheetId="1" r:id="rId4"/>
-    <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
-    <sheet name="Colors" sheetId="13" r:id="rId6"/>
-    <sheet name="Data validation parameters" sheetId="9" r:id="rId7"/>
-    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId8"/>
+    <sheet name="Process positions" sheetId="14" r:id="rId5"/>
+    <sheet name="Scenarios" sheetId="12" r:id="rId6"/>
+    <sheet name="Colors" sheetId="13" r:id="rId7"/>
+    <sheet name="Data validation parameters" sheetId="9" r:id="rId8"/>
+    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$P$3</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="251">
   <si>
     <t>Years</t>
   </si>
@@ -902,6 +903,39 @@
   </si>
   <si>
     <t>Scenario type (Constrained / Unconstrained)</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>sheet_name_process_positions</t>
+  </si>
+  <si>
+    <t>Process positions</t>
+  </si>
+  <si>
+    <t>Sheet name that contains data for process positions in normalized format (position data in range [0,1])</t>
+  </si>
+  <si>
+    <t>Industrial_roundwood:FI</t>
+  </si>
+  <si>
+    <t>Sawnwood:FI</t>
+  </si>
+  <si>
+    <t>Construction:FI</t>
+  </si>
+  <si>
+    <t>Furniture:FI</t>
+  </si>
+  <si>
+    <t>Incineration:FI</t>
+  </si>
+  <si>
+    <t>Sawnwood:Export</t>
+  </si>
+  <si>
+    <t>Sawnwood:Import</t>
   </si>
 </sst>
 </file>
@@ -1578,16 +1612,16 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="30" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="30" customWidth="1"/>
     <col min="3" max="3" width="29" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="10"/>
+    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -1599,7 +1633,7 @@
       </c>
       <c r="D1" s="37"/>
     </row>
-    <row r="2" spans="1:5" ht="135.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -1612,7 +1646,7 @@
       <c r="D2" s="36"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
@@ -1624,7 +1658,7 @@
       </c>
       <c r="D3" s="36"/>
     </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>30</v>
       </c>
@@ -1636,7 +1670,7 @@
       </c>
       <c r="D4" s="39"/>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>39</v>
       </c>
@@ -1648,7 +1682,7 @@
       </c>
       <c r="D5" s="36"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>28</v>
       </c>
@@ -1660,7 +1694,7 @@
       </c>
       <c r="D6" s="38"/>
     </row>
-    <row r="7" spans="1:5" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>33</v>
       </c>
@@ -1672,7 +1706,7 @@
       </c>
       <c r="D7" s="36"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>35</v>
       </c>
@@ -1684,7 +1718,7 @@
       </c>
       <c r="D8" s="38"/>
     </row>
-    <row r="9" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>44</v>
       </c>
@@ -1696,7 +1730,7 @@
       </c>
       <c r="D9" s="36"/>
     </row>
-    <row r="10" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>66</v>
       </c>
@@ -1708,7 +1742,7 @@
       </c>
       <c r="D10" s="36"/>
     </row>
-    <row r="11" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>68</v>
       </c>
@@ -1741,32 +1775,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="B2:E34"/>
+  <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="2" max="2" width="91.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="115.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="115.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>112</v>
       </c>
@@ -1774,7 +1808,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>93</v>
       </c>
@@ -1788,7 +1822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>94</v>
       </c>
@@ -1802,7 +1836,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>189</v>
       </c>
@@ -1816,7 +1850,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>95</v>
       </c>
@@ -1830,7 +1864,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>96</v>
       </c>
@@ -1844,7 +1878,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>190</v>
       </c>
@@ -1858,7 +1892,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>97</v>
       </c>
@@ -1872,7 +1906,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>101</v>
       </c>
@@ -1886,7 +1920,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>103</v>
       </c>
@@ -1900,7 +1934,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>104</v>
       </c>
@@ -1914,7 +1948,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>107</v>
       </c>
@@ -1928,7 +1962,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>115</v>
       </c>
@@ -1942,7 +1976,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>240</v>
+      </c>
       <c r="B18" t="s">
         <v>213</v>
       </c>
@@ -1956,7 +1993,10 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>240</v>
+      </c>
       <c r="B19" t="s">
         <v>214</v>
       </c>
@@ -1970,7 +2010,10 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>240</v>
+      </c>
       <c r="B20" t="s">
         <v>109</v>
       </c>
@@ -1984,7 +2027,10 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>240</v>
+      </c>
       <c r="B21" t="s">
         <v>122</v>
       </c>
@@ -1998,7 +2044,10 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
       <c r="B22" t="s">
         <v>121</v>
       </c>
@@ -2012,7 +2061,10 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>240</v>
+      </c>
       <c r="B23" t="s">
         <v>130</v>
       </c>
@@ -2026,7 +2078,10 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>240</v>
+      </c>
       <c r="B24" t="s">
         <v>225</v>
       </c>
@@ -2040,7 +2095,10 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>240</v>
+      </c>
       <c r="B25" t="s">
         <v>235</v>
       </c>
@@ -2054,7 +2112,10 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>240</v>
+      </c>
       <c r="B26" t="s">
         <v>136</v>
       </c>
@@ -2068,7 +2129,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>240</v>
+      </c>
       <c r="B27" t="s">
         <v>200</v>
       </c>
@@ -2079,7 +2143,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>240</v>
+      </c>
       <c r="B28" t="s">
         <v>139</v>
       </c>
@@ -2093,7 +2160,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>240</v>
+      </c>
       <c r="B29" t="s">
         <v>141</v>
       </c>
@@ -2107,7 +2177,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>240</v>
+      </c>
       <c r="B30" t="s">
         <v>160</v>
       </c>
@@ -2121,7 +2194,10 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>240</v>
+      </c>
       <c r="B31" t="s">
         <v>180</v>
       </c>
@@ -2135,7 +2211,10 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>240</v>
+      </c>
       <c r="B32" t="s">
         <v>201</v>
       </c>
@@ -2146,7 +2225,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>240</v>
+      </c>
       <c r="B33" t="s">
         <v>228</v>
       </c>
@@ -2157,7 +2239,10 @@
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>240</v>
+      </c>
       <c r="B34" t="s">
         <v>234</v>
       </c>
@@ -2166,6 +2251,23 @@
       </c>
       <c r="E34" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>240</v>
+      </c>
+      <c r="B35" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2238,28 +2340,28 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" customWidth="1"/>
-    <col min="11" max="11" width="24.54296875" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" customWidth="1"/>
-    <col min="13" max="13" width="18.26953125" customWidth="1"/>
-    <col min="14" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -2311,7 +2413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2337,7 +2439,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="20" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>223</v>
       </c>
@@ -2393,7 +2495,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2427,7 +2529,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2461,7 +2563,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2494,7 +2596,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2527,7 +2629,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2563,7 +2665,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2599,7 +2701,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2632,7 +2734,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2665,7 +2767,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2698,7 +2800,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations xWindow="1088" yWindow="385" count="2">
@@ -2730,27 +2832,27 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" customWidth="1"/>
-    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
-    <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2800,7 +2902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2824,7 +2926,7 @@
       </c>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>224</v>
       </c>
@@ -2874,7 +2976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -2924,7 +3026,7 @@
       </c>
       <c r="P4" s="16"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2974,7 +3076,7 @@
       </c>
       <c r="P5" s="16"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -3024,7 +3126,7 @@
       </c>
       <c r="P6" s="16"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -3076,7 +3178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3128,7 +3230,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3180,7 +3282,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -3232,7 +3334,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -3277,7 +3379,7 @@
       </c>
       <c r="P11" s="16"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -3323,7 +3425,7 @@
       </c>
       <c r="P12" s="16"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -3369,361 +3471,361 @@
       </c>
       <c r="P13" s="16"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
     </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E35" s="16" t="s">
         <v>120</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
     </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
     </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="N44"/>
     </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
     </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
     </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
     </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
     </row>
-    <row r="49" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
     </row>
-    <row r="50" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
     </row>
-    <row r="51" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
     </row>
-    <row r="52" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
     </row>
-    <row r="53" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
     </row>
-    <row r="54" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
     </row>
-    <row r="55" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
     </row>
-    <row r="56" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
     </row>
-    <row r="57" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
     </row>
-    <row r="58" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
     </row>
-    <row r="59" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
     </row>
-    <row r="60" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
     </row>
-    <row r="61" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
     </row>
-    <row r="62" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
     </row>
-    <row r="63" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
     </row>
-    <row r="64" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
     </row>
-    <row r="65" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
     </row>
-    <row r="66" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
     </row>
-    <row r="67" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
     </row>
-    <row r="68" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
     </row>
-    <row r="69" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
     </row>
-    <row r="70" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
     </row>
-    <row r="71" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
     </row>
-    <row r="72" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
     </row>
-    <row r="73" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
     </row>
-    <row r="74" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
     </row>
-    <row r="75" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
     </row>
-    <row r="76" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
     </row>
-    <row r="77" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
     </row>
-    <row r="79" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="8:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N86"/>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3733,22 +3835,22 @@
       <c r="M87" s="4"/>
       <c r="N87"/>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
@@ -3766,6 +3868,1301 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715F83D3-09E8-436B-8662-E6CF9B40F02C}">
+  <dimension ref="A1:D91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2021</v>
+      </c>
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2021</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D4">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2021</v>
+      </c>
+      <c r="B6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6">
+        <v>0.752</v>
+      </c>
+      <c r="D6">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2021</v>
+      </c>
+      <c r="B7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D7">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2021</v>
+      </c>
+      <c r="B8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D8">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2021</v>
+      </c>
+      <c r="B9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D9">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2021</v>
+      </c>
+      <c r="B10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2022</v>
+      </c>
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2022</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D12">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2022</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D13">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2022</v>
+      </c>
+      <c r="B15" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15">
+        <v>0.752</v>
+      </c>
+      <c r="D15">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2022</v>
+      </c>
+      <c r="B16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C16">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D16">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2022</v>
+      </c>
+      <c r="B17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C17">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D17">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2022</v>
+      </c>
+      <c r="B18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D18">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2022</v>
+      </c>
+      <c r="B19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2023</v>
+      </c>
+      <c r="B20" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2023</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2023</v>
+      </c>
+      <c r="B22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C22">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D22">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2023</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D23">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2023</v>
+      </c>
+      <c r="B24" t="s">
+        <v>246</v>
+      </c>
+      <c r="C24">
+        <v>0.752</v>
+      </c>
+      <c r="D24">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2023</v>
+      </c>
+      <c r="B25" t="s">
+        <v>247</v>
+      </c>
+      <c r="C25">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D25">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2023</v>
+      </c>
+      <c r="B26" t="s">
+        <v>248</v>
+      </c>
+      <c r="C26">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D26">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2023</v>
+      </c>
+      <c r="B27" t="s">
+        <v>249</v>
+      </c>
+      <c r="C27">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D27">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2023</v>
+      </c>
+      <c r="B28" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D28">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2024</v>
+      </c>
+      <c r="B29" t="s">
+        <v>244</v>
+      </c>
+      <c r="C29">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2024</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D30">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2024</v>
+      </c>
+      <c r="B31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D31">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2024</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D32">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2024</v>
+      </c>
+      <c r="B33" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33">
+        <v>0.752</v>
+      </c>
+      <c r="D33">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2024</v>
+      </c>
+      <c r="B34" t="s">
+        <v>247</v>
+      </c>
+      <c r="C34">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D34">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2024</v>
+      </c>
+      <c r="B35" t="s">
+        <v>248</v>
+      </c>
+      <c r="C35">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D35">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2024</v>
+      </c>
+      <c r="B36" t="s">
+        <v>249</v>
+      </c>
+      <c r="C36">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D36">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2024</v>
+      </c>
+      <c r="B37" t="s">
+        <v>250</v>
+      </c>
+      <c r="C37">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D37">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2025</v>
+      </c>
+      <c r="B38" t="s">
+        <v>244</v>
+      </c>
+      <c r="C38">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D38">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2025</v>
+      </c>
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D39">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2025</v>
+      </c>
+      <c r="B40" t="s">
+        <v>245</v>
+      </c>
+      <c r="C40">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D40">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2025</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D41">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42">
+        <v>0.752</v>
+      </c>
+      <c r="D42">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2025</v>
+      </c>
+      <c r="B43" t="s">
+        <v>247</v>
+      </c>
+      <c r="C43">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D43">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2025</v>
+      </c>
+      <c r="B44" t="s">
+        <v>248</v>
+      </c>
+      <c r="C44">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D44">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2025</v>
+      </c>
+      <c r="B45" t="s">
+        <v>249</v>
+      </c>
+      <c r="C45">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D45">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2025</v>
+      </c>
+      <c r="B46" t="s">
+        <v>250</v>
+      </c>
+      <c r="C46">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D46">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2026</v>
+      </c>
+      <c r="B47" t="s">
+        <v>244</v>
+      </c>
+      <c r="C47">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D47">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2026</v>
+      </c>
+      <c r="B48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D48">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2026</v>
+      </c>
+      <c r="B49" t="s">
+        <v>245</v>
+      </c>
+      <c r="C49">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D49">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2026</v>
+      </c>
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D50">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2026</v>
+      </c>
+      <c r="B51" t="s">
+        <v>246</v>
+      </c>
+      <c r="C51">
+        <v>0.752</v>
+      </c>
+      <c r="D51">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2026</v>
+      </c>
+      <c r="B52" t="s">
+        <v>247</v>
+      </c>
+      <c r="C52">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D52">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2026</v>
+      </c>
+      <c r="B53" t="s">
+        <v>248</v>
+      </c>
+      <c r="C53">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D53">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2026</v>
+      </c>
+      <c r="B54" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D54">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2026</v>
+      </c>
+      <c r="B55" t="s">
+        <v>250</v>
+      </c>
+      <c r="C55">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D55">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2027</v>
+      </c>
+      <c r="B56" t="s">
+        <v>244</v>
+      </c>
+      <c r="C56">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D56">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2027</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D57">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2027</v>
+      </c>
+      <c r="B58" t="s">
+        <v>245</v>
+      </c>
+      <c r="C58">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D58">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2027</v>
+      </c>
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D59">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2027</v>
+      </c>
+      <c r="B60" t="s">
+        <v>246</v>
+      </c>
+      <c r="C60">
+        <v>0.752</v>
+      </c>
+      <c r="D60">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2027</v>
+      </c>
+      <c r="B61" t="s">
+        <v>247</v>
+      </c>
+      <c r="C61">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D61">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2027</v>
+      </c>
+      <c r="B62" t="s">
+        <v>248</v>
+      </c>
+      <c r="C62">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D62">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2027</v>
+      </c>
+      <c r="B63" t="s">
+        <v>249</v>
+      </c>
+      <c r="C63">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D63">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2027</v>
+      </c>
+      <c r="B64" t="s">
+        <v>250</v>
+      </c>
+      <c r="C64">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D64">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2028</v>
+      </c>
+      <c r="B65" t="s">
+        <v>244</v>
+      </c>
+      <c r="C65">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D65">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2028</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D66">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2028</v>
+      </c>
+      <c r="B67" t="s">
+        <v>245</v>
+      </c>
+      <c r="C67">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D67">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2028</v>
+      </c>
+      <c r="B68" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D68">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2028</v>
+      </c>
+      <c r="B69" t="s">
+        <v>246</v>
+      </c>
+      <c r="C69">
+        <v>0.752</v>
+      </c>
+      <c r="D69">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2028</v>
+      </c>
+      <c r="B70" t="s">
+        <v>247</v>
+      </c>
+      <c r="C70">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D70">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2028</v>
+      </c>
+      <c r="B71" t="s">
+        <v>248</v>
+      </c>
+      <c r="C71">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D71">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2028</v>
+      </c>
+      <c r="B72" t="s">
+        <v>249</v>
+      </c>
+      <c r="C72">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D72">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2028</v>
+      </c>
+      <c r="B73" t="s">
+        <v>250</v>
+      </c>
+      <c r="C73">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D73">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2029</v>
+      </c>
+      <c r="B74" t="s">
+        <v>244</v>
+      </c>
+      <c r="C74">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D74">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2029</v>
+      </c>
+      <c r="B75" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D75">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2029</v>
+      </c>
+      <c r="B76" t="s">
+        <v>245</v>
+      </c>
+      <c r="C76">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D76">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2029</v>
+      </c>
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2029</v>
+      </c>
+      <c r="B78" t="s">
+        <v>246</v>
+      </c>
+      <c r="C78">
+        <v>0.752</v>
+      </c>
+      <c r="D78">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2029</v>
+      </c>
+      <c r="B79" t="s">
+        <v>247</v>
+      </c>
+      <c r="C79">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D79">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2029</v>
+      </c>
+      <c r="B80" t="s">
+        <v>248</v>
+      </c>
+      <c r="C80">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D80">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2029</v>
+      </c>
+      <c r="B81" t="s">
+        <v>249</v>
+      </c>
+      <c r="C81">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D81">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2029</v>
+      </c>
+      <c r="B82" t="s">
+        <v>250</v>
+      </c>
+      <c r="C82">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D82">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2030</v>
+      </c>
+      <c r="B83" t="s">
+        <v>244</v>
+      </c>
+      <c r="C83">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D83">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2030</v>
+      </c>
+      <c r="B84" t="s">
+        <v>63</v>
+      </c>
+      <c r="C84">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D84">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2030</v>
+      </c>
+      <c r="B85" t="s">
+        <v>245</v>
+      </c>
+      <c r="C85">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D85">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2030</v>
+      </c>
+      <c r="B86" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D86">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2030</v>
+      </c>
+      <c r="B87" t="s">
+        <v>246</v>
+      </c>
+      <c r="C87">
+        <v>0.752</v>
+      </c>
+      <c r="D87">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2030</v>
+      </c>
+      <c r="B88" t="s">
+        <v>247</v>
+      </c>
+      <c r="C88">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="D88">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2030</v>
+      </c>
+      <c r="B89" t="s">
+        <v>248</v>
+      </c>
+      <c r="C89">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="D89">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2030</v>
+      </c>
+      <c r="B90" t="s">
+        <v>249</v>
+      </c>
+      <c r="C90">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D90">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2030</v>
+      </c>
+      <c r="B91" t="s">
+        <v>250</v>
+      </c>
+      <c r="C91">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="D91">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -3773,21 +5170,21 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="52.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>143</v>
       </c>
@@ -3822,7 +5219,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>220</v>
       </c>
@@ -3848,7 +5245,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
@@ -3875,7 +5272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA92C4F1-884F-4740-8793-4A0AB47EED3D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -3883,13 +5280,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>173</v>
       </c>
@@ -3897,7 +5294,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3905,7 +5302,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3913,7 +5310,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3921,7 +5318,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -3929,7 +5326,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3937,7 +5334,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -3945,7 +5342,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -3953,7 +5350,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -3970,7 +5367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
   <dimension ref="B2:G13"/>
   <sheetViews>
@@ -3978,28 +5375,28 @@
       <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>119</v>
       </c>
@@ -4019,7 +5416,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>84</v>
       </c>
@@ -4039,7 +5436,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -4059,7 +5456,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>85</v>
       </c>
@@ -4070,7 +5467,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>87</v>
       </c>
@@ -4081,22 +5478,22 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>233</v>
       </c>
@@ -4107,7 +5504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
   <dimension ref="B1:D2"/>
   <sheetViews>
@@ -4115,19 +5512,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>71</v>
       </c>
@@ -4144,6 +5541,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -4406,42 +5824,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4464,9 +5850,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added: - Updated documentation + screenshots - Updated example_data.xlsx
Updated:
- Cleaned flowmodifiersolver.py
- Removed redundant sheets from example_data.xlsx
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,32 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB3299C-762D-469F-BAE7-BA1855023F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD981D5-6964-4A88-A4B8-76B1023ADCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Readme" sheetId="4" r:id="rId1"/>
-    <sheet name="Settings" sheetId="11" r:id="rId2"/>
-    <sheet name="Processes" sheetId="6" r:id="rId3"/>
-    <sheet name="Flows" sheetId="1" r:id="rId4"/>
-    <sheet name="Process positions" sheetId="14" r:id="rId5"/>
-    <sheet name="Scenarios" sheetId="12" r:id="rId6"/>
-    <sheet name="Colors" sheetId="13" r:id="rId7"/>
-    <sheet name="Data validation parameters" sheetId="9" r:id="rId8"/>
-    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId9"/>
+    <sheet name="Settings" sheetId="11" r:id="rId1"/>
+    <sheet name="Processes" sheetId="6" r:id="rId2"/>
+    <sheet name="Flows" sheetId="1" r:id="rId3"/>
+    <sheet name="Process positions" sheetId="14" r:id="rId4"/>
+    <sheet name="Scenarios" sheetId="12" r:id="rId5"/>
+    <sheet name="Colors" sheetId="13" r:id="rId6"/>
+    <sheet name="Data validation parameters" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$A$3:$P$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Processes!$D$3:$R$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Settings!$B$6:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Flows!$A$3:$P$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Processes!$D$3:$R$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Settings!$B$6:$E$6</definedName>
     <definedName name="Boolean">'Data validation parameters'!$C$6:$C$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -50,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="216">
   <si>
     <t>Years</t>
   </si>
@@ -61,21 +59,9 @@
     <t>Flows</t>
   </si>
   <si>
-    <t>Tab name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Source data processes normalized</t>
-  </si>
-  <si>
-    <t>Source data flows normalized</t>
-  </si>
-  <si>
     <t>Data type</t>
   </si>
   <si>
@@ -136,57 +122,9 @@
     <t xml:space="preserve">float </t>
   </si>
   <si>
-    <t>Please note</t>
-  </si>
-  <si>
-    <t>Process IDs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other topics </t>
-  </si>
-  <si>
-    <t>About</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtual flows </t>
-  </si>
-  <si>
-    <t>Unbalanced system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units of flows </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute values </t>
-  </si>
-  <si>
-    <t>aiphoria does not recognize between absolute units but only between absolute and relative (%)</t>
-  </si>
-  <si>
-    <t>Make sure that no whitespaces exist on the process IDs (at the end or beginning)</t>
-  </si>
-  <si>
-    <t>General information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">About aiphoria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positioning of flows in the sankey </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Columns P and Q in the process sheet give the possibility to the user to automatically position the processes and flows in the sankey diagram. Firstly, the user needs to run aiphoria, then when the sankey diagram pops up the user should manually position the processes and flows to the preferred position; get the x and y information from the graph, then paste them into excel and run again. </t>
-  </si>
-  <si>
     <t>Label shown in graph</t>
   </si>
   <si>
-    <t>Process sheet: Normalized x and y columns</t>
-  </si>
-  <si>
     <t>m3, kg, %</t>
   </si>
   <si>
@@ -229,15 +167,6 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>https://doi.org/10.1016/j.resconrec.2024.107476</t>
-  </si>
-  <si>
-    <t>Assumed density of CLT 480 kg/m3</t>
-  </si>
-  <si>
-    <t>Assumer density of a furniture product 450 kg/m3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Random input values </t>
   </si>
   <si>
@@ -250,82 +179,6 @@
     <t>Process ID</t>
   </si>
   <si>
-    <t>DMFA results (example) sheet</t>
-  </si>
-  <si>
-    <t>The DMFA results content is pasted here to illustrate the results deriving from the demo case taken place in the example.ipynb</t>
-  </si>
-  <si>
-    <t>Carbon fraction (will be moved) sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbon accounting </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results </t>
-  </si>
-  <si>
-    <t>Carbon fraction</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This sheets represent the flows/arrows/edges in the flowchart. The idea is to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>create IDs in an string style "Process-Process location"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (e.g., P1:EU) for both, the source and target processes. With that, and the transformation stages from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Processes sheet </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">it is also possible to create the flowchart. In the flows sheet define the source process name on the source process cell. Then fill in the source process location, target process name and target process location. Fill in the value, year and run. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Columns B to L need be filled in for aiphoria to run.</t>
-    </r>
-  </si>
-  <si>
     <t>Mm3 SWE</t>
   </si>
   <si>
@@ -458,46 +311,6 @@
     <t>If using virtual flows, create virtual flow to process if process total inputs and outputs difference is greater than this value</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the input file of aiphoria where the user defines the processes/nodes and flows/arrows/edges within the preferred system. aiphoria supports both static and dynamic assessments (e.g from 2021 to 2050). If can be used to assess any system and both product or process based MFAs. </t>
-  </si>
-  <si>
-    <r>
-      <t>This sheet is the starting point for aiphoria.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> User define what process/nodes to be included in the study</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. With the transformation stages it's possible to locate the nodes in a graph. Life time (LT) and LT distribution are included to consider stock distribution in ODYM. Define the name of the process, its stage within the system boundaries, location, distribution type and distribution parameters (see ODYM tutorials/guides). At the end you should have a process ID with the name and location (e.g. P1:EU). After you have described all the processes within you system, you can move to the flows spreadsheet. It is advised to visualise your system (e.g. using https://excalidraw.com/) before you start implimenting in aiphoria. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Columns B to I need be filled in for aiphoria to run.</t>
-    </r>
-  </si>
-  <si>
     <t>Distribution type</t>
   </si>
   <si>
@@ -526,9 +339,6 @@
   </si>
   <si>
     <t>Float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from Settings. </t>
   </si>
   <si>
     <t>fill_method</t>
@@ -737,9 +547,6 @@
     <t>#808080</t>
   </si>
   <si>
-    <t xml:space="preserve">The carbon fraction sheet is only temporary here and it is being used by the Flows sheet. In the next version of aiphoria this will be moved. </t>
-  </si>
-  <si>
     <t>#7dda60</t>
   </si>
   <si>
@@ -819,9 +626,6 @@
   </si>
   <si>
     <t>Data source comment</t>
-  </si>
-  <si>
-    <t>Assumed density of a furniture product 450 kg/m3</t>
   </si>
   <si>
     <t>baseline_value_name</t>
@@ -1011,7 +815,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1027,12 +831,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,11 +889,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1108,12 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1141,39 +930,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1605,180 +1361,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240816D1-B4FF-41BE-B292-8CF7D349FFB2}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.85546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="29" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="37"/>
-    </row>
-    <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="36"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="38"/>
-    </row>
-    <row r="7" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="36"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="38"/>
-    </row>
-    <row r="9" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="36"/>
-    </row>
-    <row r="10" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="36"/>
-    </row>
-    <row r="11" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>184</v>
-      </c>
-      <c r="D11" s="36"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C9:D9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,483 +1378,483 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
-        <v>92</v>
+      <c r="B2" s="19" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
-        <v>113</v>
+      <c r="B3" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+        <v>82</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>4</v>
+      <c r="B6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>127</v>
+      <c r="D7" s="23" t="s">
+        <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="25">
+        <v>65</v>
+      </c>
+      <c r="C9" s="22">
         <v>2</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>125</v>
+      <c r="D9" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="26" t="s">
-        <v>126</v>
+      <c r="D10" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="25">
+        <v>67</v>
+      </c>
+      <c r="C12" s="22">
         <v>2</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>125</v>
+      <c r="D12" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="25">
+        <v>71</v>
+      </c>
+      <c r="C13" s="22">
         <v>2021</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>125</v>
+      <c r="D13" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="25">
+        <v>73</v>
+      </c>
+      <c r="C14" s="22">
         <v>2030</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>125</v>
+      <c r="D14" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="27" t="b">
+        <v>74</v>
+      </c>
+      <c r="C15" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="27" t="b">
+        <v>77</v>
+      </c>
+      <c r="C16" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="17">
+        <v>85</v>
+      </c>
+      <c r="C17" s="14">
         <v>0.1</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>128</v>
+      <c r="D17" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="C19" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="D19" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="23">
+        <v>79</v>
+      </c>
+      <c r="C20" s="20">
         <v>-3.6666666666666701</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>128</v>
+      <c r="D20" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="27" t="b">
+        <v>90</v>
+      </c>
+      <c r="C21" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="27" t="b">
+        <v>89</v>
+      </c>
+      <c r="C22" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="E22" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
-      </c>
-      <c r="C24" s="27" t="b">
+        <v>190</v>
+      </c>
+      <c r="C24" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="E24" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B25" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="C25" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="E25" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B27" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="D27" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E27" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="27" t="b">
+        <v>106</v>
+      </c>
+      <c r="C28" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
-      </c>
-      <c r="C29" s="27" t="b">
+        <v>108</v>
+      </c>
+      <c r="C29" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E30" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>126</v>
+        <v>147</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="D32" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E32" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E34" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B35" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="D35" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2332,12 +1919,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,137 +1949,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="M3" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -2500,25 +2087,25 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D12" si="0">_xlfn.CONCAT(B4,":",C4)</f>
         <v>Industrial_roundwood:FI</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="M4" s="4"/>
       <c r="P4">
         <v>3.6999999999999998E-2</v>
       </c>
@@ -2526,7 +2113,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -2534,25 +2121,25 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>Sawmilling:FI</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="M5" s="4"/>
       <c r="P5">
         <v>0.24299999999999999</v>
       </c>
@@ -2560,7 +2147,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2568,23 +2155,23 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Residues:FI</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="P6">
         <v>0.40899999999999997</v>
@@ -2593,7 +2180,7 @@
         <v>0.05</v>
       </c>
       <c r="R6" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2601,23 +2188,23 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>Sawnwood:FI</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="P7">
         <v>0.40899999999999997</v>
@@ -2626,7 +2213,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2634,26 +2221,26 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="P8">
         <v>0.752</v>
@@ -2662,7 +2249,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2670,26 +2257,26 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>Furniture:FI</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="P9">
         <v>0.65600000000000003</v>
@@ -2698,7 +2285,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2706,23 +2293,23 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>Sawnwood:Import</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="P10">
         <v>0.24299999999999999</v>
@@ -2731,7 +2318,7 @@
         <v>0.9</v>
       </c>
       <c r="R10" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2739,23 +2326,23 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>Sawnwood:Export</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="P11">
         <v>0.69099999999999995</v>
@@ -2764,7 +2351,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2772,23 +2359,23 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>Incineration:FI</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="P12">
         <v>0.96599999999999997</v>
@@ -2797,7 +2384,7 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2824,12 +2411,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,164 +2434,164 @@
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
     <col min="16" max="16" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="P2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>17</v>
+      <c r="A3" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C4" t="str">
         <f>+_xlfn.XLOOKUP(H4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Source</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F4" t="str">
         <f>+_xlfn.XLOOKUP(I4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="str">
         <f t="shared" ref="H4:H13" si="0">_xlfn.CONCAT(B4,":",D4)</f>
         <v>Industrial_roundwood:FI</v>
       </c>
-      <c r="I4" s="4" t="str">
+      <c r="I4" s="3" t="str">
         <f t="shared" ref="I4:I13" si="1">_xlfn.CONCAT(E4,":",G4)</f>
         <v>Sawmilling:FI</v>
       </c>
@@ -3012,49 +2599,45 @@
         <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="L4">
         <v>2021</v>
       </c>
       <c r="N4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4">
-        <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.20342399999999999</v>
-      </c>
-      <c r="P4" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="P4" s="13"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C5" t="str">
         <f>+_xlfn.XLOOKUP(H5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F5" t="str">
         <f>+_xlfn.XLOOKUP(I5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Sawmilling:FI</v>
       </c>
-      <c r="I5" s="4" t="str">
+      <c r="I5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sawnwood:FI</v>
       </c>
@@ -3062,49 +2645,45 @@
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L5">
         <v>2021</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5">
-        <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.20342399999999999</v>
-      </c>
-      <c r="P5" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="P5" s="13"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C6" t="str">
         <f>+_xlfn.XLOOKUP(H6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="F6" t="str">
         <f>+_xlfn.XLOOKUP(I6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>by_prod</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Sawmilling:FI</v>
       </c>
-      <c r="I6" s="4" t="str">
+      <c r="I6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Residues:FI</v>
       </c>
@@ -3112,49 +2691,45 @@
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>2021</v>
       </c>
       <c r="N6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6">
-        <f>0.395*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.18959999999999999</v>
-      </c>
-      <c r="P6" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="P6" s="13"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C7" t="str">
         <f>+_xlfn.XLOOKUP(H7,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="F7" t="str">
         <f>+_xlfn.XLOOKUP(I7,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Sawnwood:FI</v>
       </c>
-      <c r="I7" s="4" t="str">
+      <c r="I7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Construction:FI</v>
       </c>
@@ -3162,51 +2737,47 @@
         <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L7">
         <v>2021</v>
       </c>
       <c r="N7" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O7">
-        <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.23039999999999999</v>
-      </c>
-      <c r="P7" t="s">
-        <v>60</v>
+        <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C8" t="str">
         <f>+_xlfn.XLOOKUP(H8,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F8" t="str">
         <f>+_xlfn.XLOOKUP(I8,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H8" s="3" t="str">
         <f>_xlfn.CONCAT(B8,":",D8)</f>
         <v>Sawnwood:FI</v>
       </c>
-      <c r="I8" s="4" t="str">
+      <c r="I8" s="3" t="str">
         <f>_xlfn.CONCAT(E8,":",G8)</f>
         <v>Furniture:FI</v>
       </c>
@@ -3214,51 +2785,47 @@
         <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L8">
         <v>2021</v>
       </c>
       <c r="N8" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O8">
-        <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.216</v>
-      </c>
-      <c r="P8" t="s">
-        <v>61</v>
+        <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C9" t="str">
         <f>+_xlfn.XLOOKUP(H9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F9" t="str">
         <f>+_xlfn.XLOOKUP(I9,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I9" s="4" t="str">
+      <c r="I9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sawmilling:FI</v>
       </c>
@@ -3266,51 +2833,44 @@
         <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L9">
         <v>2021</v>
       </c>
       <c r="N9" t="s">
-        <v>62</v>
-      </c>
-      <c r="O9">
-        <f>0.48*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.23039999999999999</v>
-      </c>
-      <c r="P9" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C10" t="str">
         <f>+_xlfn.XLOOKUP(H10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>VAM</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="F10" t="str">
         <f>+_xlfn.XLOOKUP(I10,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Construction:FI</v>
       </c>
-      <c r="I10" s="4" t="str">
+      <c r="I10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Incineration:FI</v>
       </c>
@@ -3318,50 +2878,43 @@
         <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L10">
         <v>2021</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10">
-        <f>0.45*'Carbon fraction (will be moved)'!$C$2</f>
-        <v>0.216</v>
-      </c>
-      <c r="P10" t="s">
-        <v>212</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="F11" t="str">
         <f>+_xlfn.XLOOKUP(I11,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>EoL</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Furniture:FI</v>
       </c>
-      <c r="I11" s="4" t="str">
+      <c r="I11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Incineration:FI</v>
       </c>
@@ -3369,45 +2922,45 @@
         <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L11">
         <v>2021</v>
       </c>
       <c r="N11" t="s">
-        <v>62</v>
-      </c>
-      <c r="P11" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="P11" s="13"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C12" t="str">
         <f>+_xlfn.XLOOKUP(H12,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F12" t="str">
         <f>+_xlfn.XLOOKUP(I12,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>RoW</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="4" t="str">
+        <v>19</v>
+      </c>
+      <c r="H12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Sawnwood:FI</v>
       </c>
-      <c r="I12" s="4" t="str">
+      <c r="I12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sawnwood:Export</v>
       </c>
@@ -3415,45 +2968,45 @@
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="L12">
         <v>2021</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
-      </c>
-      <c r="P12" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="P12" s="13"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C13" t="str">
         <f>+_xlfn.XLOOKUP(H13,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>RoW</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F13" t="str">
         <f>+_xlfn.XLOOKUP(I13,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="4" t="str">
+        <v>27</v>
+      </c>
+      <c r="H13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Sawnwood:Import</v>
       </c>
-      <c r="I13" s="4" t="str">
+      <c r="I13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sawnwood:FI</v>
       </c>
@@ -3461,402 +3014,402 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="L13">
         <v>2021</v>
       </c>
       <c r="N13" t="s">
-        <v>62</v>
-      </c>
-      <c r="P13" s="16"/>
+        <v>39</v>
+      </c>
+      <c r="P13" s="13"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
       <c r="N14"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
       <c r="N15"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
       <c r="N16"/>
     </row>
     <row r="17" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
       <c r="N17"/>
     </row>
     <row r="18" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
       <c r="N18"/>
     </row>
     <row r="19" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
       <c r="N19"/>
     </row>
     <row r="20" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
       <c r="N20"/>
     </row>
     <row r="21" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
       <c r="N21"/>
     </row>
     <row r="22" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
       <c r="N22"/>
     </row>
     <row r="23" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
       <c r="N23"/>
     </row>
     <row r="24" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="N28" s="7"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="N28" s="6"/>
     </row>
     <row r="29" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="N29" s="7"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
     <row r="31" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
     </row>
     <row r="32" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E35" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="E35" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
       <c r="N39"/>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
       <c r="N40"/>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
       <c r="N41"/>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
       <c r="N42"/>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
       <c r="N43"/>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
       <c r="N44"/>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C45" s="9"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
+      <c r="C45" s="8"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
       <c r="N45"/>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
       <c r="N46"/>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
       <c r="N47"/>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
       <c r="N48"/>
     </row>
     <row r="49" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
       <c r="N49"/>
     </row>
     <row r="50" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
       <c r="N50"/>
     </row>
     <row r="51" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
       <c r="N51"/>
     </row>
     <row r="52" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
       <c r="N52"/>
     </row>
     <row r="53" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
       <c r="N53"/>
     </row>
     <row r="54" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
       <c r="N54"/>
     </row>
     <row r="55" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
       <c r="N55"/>
     </row>
     <row r="56" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
       <c r="N56"/>
     </row>
     <row r="57" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
       <c r="N57"/>
     </row>
     <row r="58" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
       <c r="N58"/>
     </row>
     <row r="59" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
       <c r="N59"/>
     </row>
     <row r="60" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
       <c r="N60"/>
     </row>
     <row r="61" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
       <c r="N61"/>
     </row>
     <row r="62" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
       <c r="N62"/>
     </row>
     <row r="63" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
       <c r="N63"/>
     </row>
     <row r="64" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
       <c r="N64"/>
     </row>
     <row r="65" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
       <c r="N65"/>
     </row>
     <row r="66" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
       <c r="N66"/>
     </row>
     <row r="67" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
       <c r="N67"/>
     </row>
     <row r="68" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
       <c r="N68"/>
     </row>
     <row r="69" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
       <c r="N69"/>
     </row>
     <row r="70" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
       <c r="N70"/>
     </row>
     <row r="71" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
       <c r="N71"/>
     </row>
     <row r="72" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
       <c r="N72"/>
     </row>
     <row r="73" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
       <c r="N73"/>
     </row>
     <row r="74" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
       <c r="N74"/>
     </row>
     <row r="75" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
       <c r="N75"/>
     </row>
     <row r="76" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
       <c r="N76"/>
     </row>
     <row r="77" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
       <c r="N77"/>
     </row>
     <row r="78" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
       <c r="N78"/>
     </row>
     <row r="79" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
       <c r="N79"/>
     </row>
     <row r="80" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
       <c r="N80"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
       <c r="N81"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
       <c r="N82"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
       <c r="N83"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
       <c r="N84"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
       <c r="N85"/>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N86"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="M87" s="4"/>
+      <c r="B87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="M87" s="3"/>
       <c r="N87"/>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
       <c r="N88"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H89" s="4"/>
-      <c r="I89" s="4"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
       <c r="N89"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
       <c r="N90"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
       <c r="N91"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:P3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}"/>
+  <autoFilter ref="A3:P13" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E35" r:id="rId1" location="json=TH95eCDBsN1pfqczsMf84,S3TGIZvZiI-AUl8oZJcUYg" xr:uid="{26F0F99B-4281-4D67-B3C8-B1BC12D732B7}"/>
@@ -3867,11 +3420,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715F83D3-09E8-436B-8662-E6CF9B40F02C}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -3885,16 +3438,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3902,7 +3455,7 @@
         <v>2021</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C2">
         <v>3.6999999999999998E-2</v>
@@ -3916,7 +3469,7 @@
         <v>2021</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>0.24299999999999999</v>
@@ -3930,7 +3483,7 @@
         <v>2021</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C4">
         <v>0.40899999999999997</v>
@@ -3944,7 +3497,7 @@
         <v>2021</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>0.40899999999999997</v>
@@ -3958,7 +3511,7 @@
         <v>2021</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C6">
         <v>0.752</v>
@@ -3972,7 +3525,7 @@
         <v>2021</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C7">
         <v>0.65600000000000003</v>
@@ -3986,7 +3539,7 @@
         <v>2021</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C8">
         <v>0.96599999999999997</v>
@@ -4000,7 +3553,7 @@
         <v>2021</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C9">
         <v>0.69099999999999995</v>
@@ -4014,7 +3567,7 @@
         <v>2021</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C10">
         <v>0.24299999999999999</v>
@@ -4028,7 +3581,7 @@
         <v>2022</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C11">
         <v>3.6999999999999998E-2</v>
@@ -4042,7 +3595,7 @@
         <v>2022</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>0.24299999999999999</v>
@@ -4056,7 +3609,7 @@
         <v>2022</v>
       </c>
       <c r="B13" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C13">
         <v>0.40899999999999997</v>
@@ -4070,7 +3623,7 @@
         <v>2022</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>0.40899999999999997</v>
@@ -4084,7 +3637,7 @@
         <v>2022</v>
       </c>
       <c r="B15" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C15">
         <v>0.752</v>
@@ -4098,7 +3651,7 @@
         <v>2022</v>
       </c>
       <c r="B16" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C16">
         <v>0.65600000000000003</v>
@@ -4112,7 +3665,7 @@
         <v>2022</v>
       </c>
       <c r="B17" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C17">
         <v>0.96599999999999997</v>
@@ -4126,7 +3679,7 @@
         <v>2022</v>
       </c>
       <c r="B18" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C18">
         <v>0.69099999999999995</v>
@@ -4140,7 +3693,7 @@
         <v>2022</v>
       </c>
       <c r="B19" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C19">
         <v>0.24299999999999999</v>
@@ -4154,7 +3707,7 @@
         <v>2023</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C20">
         <v>3.6999999999999998E-2</v>
@@ -4168,7 +3721,7 @@
         <v>2023</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C21">
         <v>0.24299999999999999</v>
@@ -4182,7 +3735,7 @@
         <v>2023</v>
       </c>
       <c r="B22" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C22">
         <v>0.40899999999999997</v>
@@ -4196,7 +3749,7 @@
         <v>2023</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C23">
         <v>0.40899999999999997</v>
@@ -4210,7 +3763,7 @@
         <v>2023</v>
       </c>
       <c r="B24" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C24">
         <v>0.752</v>
@@ -4224,7 +3777,7 @@
         <v>2023</v>
       </c>
       <c r="B25" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C25">
         <v>0.65600000000000003</v>
@@ -4238,7 +3791,7 @@
         <v>2023</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C26">
         <v>0.96599999999999997</v>
@@ -4252,7 +3805,7 @@
         <v>2023</v>
       </c>
       <c r="B27" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C27">
         <v>0.69099999999999995</v>
@@ -4266,7 +3819,7 @@
         <v>2023</v>
       </c>
       <c r="B28" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C28">
         <v>0.24299999999999999</v>
@@ -4280,7 +3833,7 @@
         <v>2024</v>
       </c>
       <c r="B29" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C29">
         <v>3.6999999999999998E-2</v>
@@ -4294,7 +3847,7 @@
         <v>2024</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C30">
         <v>0.24299999999999999</v>
@@ -4308,7 +3861,7 @@
         <v>2024</v>
       </c>
       <c r="B31" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C31">
         <v>0.40899999999999997</v>
@@ -4322,7 +3875,7 @@
         <v>2024</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>0.40899999999999997</v>
@@ -4336,7 +3889,7 @@
         <v>2024</v>
       </c>
       <c r="B33" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C33">
         <v>0.752</v>
@@ -4350,7 +3903,7 @@
         <v>2024</v>
       </c>
       <c r="B34" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C34">
         <v>0.65600000000000003</v>
@@ -4364,7 +3917,7 @@
         <v>2024</v>
       </c>
       <c r="B35" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C35">
         <v>0.96599999999999997</v>
@@ -4378,7 +3931,7 @@
         <v>2024</v>
       </c>
       <c r="B36" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C36">
         <v>0.69099999999999995</v>
@@ -4392,7 +3945,7 @@
         <v>2024</v>
       </c>
       <c r="B37" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C37">
         <v>0.24299999999999999</v>
@@ -4406,7 +3959,7 @@
         <v>2025</v>
       </c>
       <c r="B38" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C38">
         <v>3.6999999999999998E-2</v>
@@ -4420,7 +3973,7 @@
         <v>2025</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>0.24299999999999999</v>
@@ -4434,7 +3987,7 @@
         <v>2025</v>
       </c>
       <c r="B40" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C40">
         <v>0.40899999999999997</v>
@@ -4448,7 +4001,7 @@
         <v>2025</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>0.40899999999999997</v>
@@ -4462,7 +4015,7 @@
         <v>2025</v>
       </c>
       <c r="B42" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C42">
         <v>0.752</v>
@@ -4476,7 +4029,7 @@
         <v>2025</v>
       </c>
       <c r="B43" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C43">
         <v>0.65600000000000003</v>
@@ -4490,7 +4043,7 @@
         <v>2025</v>
       </c>
       <c r="B44" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C44">
         <v>0.96599999999999997</v>
@@ -4504,7 +4057,7 @@
         <v>2025</v>
       </c>
       <c r="B45" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C45">
         <v>0.69099999999999995</v>
@@ -4518,7 +4071,7 @@
         <v>2025</v>
       </c>
       <c r="B46" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C46">
         <v>0.24299999999999999</v>
@@ -4532,7 +4085,7 @@
         <v>2026</v>
       </c>
       <c r="B47" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C47">
         <v>3.6999999999999998E-2</v>
@@ -4546,7 +4099,7 @@
         <v>2026</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C48">
         <v>0.24299999999999999</v>
@@ -4560,7 +4113,7 @@
         <v>2026</v>
       </c>
       <c r="B49" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C49">
         <v>0.40899999999999997</v>
@@ -4574,7 +4127,7 @@
         <v>2026</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C50">
         <v>0.40899999999999997</v>
@@ -4588,7 +4141,7 @@
         <v>2026</v>
       </c>
       <c r="B51" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C51">
         <v>0.752</v>
@@ -4602,7 +4155,7 @@
         <v>2026</v>
       </c>
       <c r="B52" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C52">
         <v>0.65600000000000003</v>
@@ -4616,7 +4169,7 @@
         <v>2026</v>
       </c>
       <c r="B53" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C53">
         <v>0.96599999999999997</v>
@@ -4630,7 +4183,7 @@
         <v>2026</v>
       </c>
       <c r="B54" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C54">
         <v>0.69099999999999995</v>
@@ -4644,7 +4197,7 @@
         <v>2026</v>
       </c>
       <c r="B55" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C55">
         <v>0.24299999999999999</v>
@@ -4658,7 +4211,7 @@
         <v>2027</v>
       </c>
       <c r="B56" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C56">
         <v>3.6999999999999998E-2</v>
@@ -4672,7 +4225,7 @@
         <v>2027</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C57">
         <v>0.24299999999999999</v>
@@ -4686,7 +4239,7 @@
         <v>2027</v>
       </c>
       <c r="B58" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C58">
         <v>0.40899999999999997</v>
@@ -4700,7 +4253,7 @@
         <v>2027</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C59">
         <v>0.40899999999999997</v>
@@ -4714,7 +4267,7 @@
         <v>2027</v>
       </c>
       <c r="B60" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C60">
         <v>0.752</v>
@@ -4728,7 +4281,7 @@
         <v>2027</v>
       </c>
       <c r="B61" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C61">
         <v>0.65600000000000003</v>
@@ -4742,7 +4295,7 @@
         <v>2027</v>
       </c>
       <c r="B62" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C62">
         <v>0.96599999999999997</v>
@@ -4756,7 +4309,7 @@
         <v>2027</v>
       </c>
       <c r="B63" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C63">
         <v>0.69099999999999995</v>
@@ -4770,7 +4323,7 @@
         <v>2027</v>
       </c>
       <c r="B64" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C64">
         <v>0.24299999999999999</v>
@@ -4784,7 +4337,7 @@
         <v>2028</v>
       </c>
       <c r="B65" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C65">
         <v>3.6999999999999998E-2</v>
@@ -4798,7 +4351,7 @@
         <v>2028</v>
       </c>
       <c r="B66" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C66">
         <v>0.24299999999999999</v>
@@ -4812,7 +4365,7 @@
         <v>2028</v>
       </c>
       <c r="B67" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C67">
         <v>0.40899999999999997</v>
@@ -4826,7 +4379,7 @@
         <v>2028</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C68">
         <v>0.40899999999999997</v>
@@ -4840,7 +4393,7 @@
         <v>2028</v>
       </c>
       <c r="B69" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C69">
         <v>0.752</v>
@@ -4854,7 +4407,7 @@
         <v>2028</v>
       </c>
       <c r="B70" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C70">
         <v>0.65600000000000003</v>
@@ -4868,7 +4421,7 @@
         <v>2028</v>
       </c>
       <c r="B71" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C71">
         <v>0.96599999999999997</v>
@@ -4882,7 +4435,7 @@
         <v>2028</v>
       </c>
       <c r="B72" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C72">
         <v>0.69099999999999995</v>
@@ -4896,7 +4449,7 @@
         <v>2028</v>
       </c>
       <c r="B73" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C73">
         <v>0.24299999999999999</v>
@@ -4910,7 +4463,7 @@
         <v>2029</v>
       </c>
       <c r="B74" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C74">
         <v>3.6999999999999998E-2</v>
@@ -4924,7 +4477,7 @@
         <v>2029</v>
       </c>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C75">
         <v>0.24299999999999999</v>
@@ -4938,7 +4491,7 @@
         <v>2029</v>
       </c>
       <c r="B76" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C76">
         <v>0.40899999999999997</v>
@@ -4952,7 +4505,7 @@
         <v>2029</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C77">
         <v>0.40899999999999997</v>
@@ -4966,7 +4519,7 @@
         <v>2029</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C78">
         <v>0.752</v>
@@ -4980,7 +4533,7 @@
         <v>2029</v>
       </c>
       <c r="B79" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C79">
         <v>0.65600000000000003</v>
@@ -4994,7 +4547,7 @@
         <v>2029</v>
       </c>
       <c r="B80" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C80">
         <v>0.96599999999999997</v>
@@ -5008,7 +4561,7 @@
         <v>2029</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C81">
         <v>0.69099999999999995</v>
@@ -5022,7 +4575,7 @@
         <v>2029</v>
       </c>
       <c r="B82" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C82">
         <v>0.24299999999999999</v>
@@ -5036,7 +4589,7 @@
         <v>2030</v>
       </c>
       <c r="B83" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="C83">
         <v>3.6999999999999998E-2</v>
@@ -5050,7 +4603,7 @@
         <v>2030</v>
       </c>
       <c r="B84" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C84">
         <v>0.24299999999999999</v>
@@ -5064,7 +4617,7 @@
         <v>2030</v>
       </c>
       <c r="B85" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C85">
         <v>0.40899999999999997</v>
@@ -5078,7 +4631,7 @@
         <v>2030</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C86">
         <v>0.40899999999999997</v>
@@ -5092,7 +4645,7 @@
         <v>2030</v>
       </c>
       <c r="B87" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C87">
         <v>0.752</v>
@@ -5106,7 +4659,7 @@
         <v>2030</v>
       </c>
       <c r="B88" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="C88">
         <v>0.65600000000000003</v>
@@ -5120,7 +4673,7 @@
         <v>2030</v>
       </c>
       <c r="B89" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="C89">
         <v>0.96599999999999997</v>
@@ -5134,7 +4687,7 @@
         <v>2030</v>
       </c>
       <c r="B90" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C90">
         <v>0.69099999999999995</v>
@@ -5148,7 +4701,7 @@
         <v>2030</v>
       </c>
       <c r="B91" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="C91">
         <v>0.24299999999999999</v>
@@ -5162,12 +4715,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5185,55 +4738,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>151</v>
+      <c r="A1" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>64</v>
+        <v>185</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D2">
         <v>-50</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G2">
         <v>2025</v>
@@ -5242,12 +4795,12 @@
         <v>2030</v>
       </c>
       <c r="I2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5272,7 +4825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA92C4F1-884F-4740-8793-4A0AB47EED3D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -5287,78 +4840,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>174</v>
+      <c r="A1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -5367,12 +4920,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12935D7-39CC-4336-870D-98DAC14A69ED}">
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G7"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5388,114 +4941,114 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>236</v>
+      <c r="B5" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="G7" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="F9" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -5504,52 +5057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
-  <dimension ref="B1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2">
-        <v>0.48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
@@ -5561,7 +5069,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -5824,15 +5332,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -5849,7 +5358,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5866,4 +5375,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated: - Cleaned example_data.xlsx
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD981D5-6964-4A88-A4B8-76B1023ADCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1338C6F-D901-4097-AA7E-B0832331462A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="215">
   <si>
     <t>Years</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>Distribution type</t>
-  </si>
-  <si>
-    <t>https://excalidraw.com/#json=TH95eCDBsN1pfqczsMf84,S3TGIZvZiI-AUl8oZJcUYg</t>
   </si>
   <si>
     <t>fill_missing_relative_flows</t>
@@ -1364,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
         <v>68</v>
@@ -1425,16 +1422,16 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -1445,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
         <v>69</v>
@@ -1459,7 +1456,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
         <v>70</v>
@@ -1467,16 +1464,16 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1487,7 +1484,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
         <v>69</v>
@@ -1501,7 +1498,7 @@
         <v>2021</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
         <v>72</v>
@@ -1515,7 +1512,7 @@
         <v>2030</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
         <v>81</v>
@@ -1529,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
         <v>76</v>
@@ -1543,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
         <v>78</v>
@@ -1557,7 +1554,7 @@
         <v>0.1</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
         <v>86</v>
@@ -1565,41 +1562,41 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
         <v>179</v>
-      </c>
-      <c r="C19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s">
         <v>79</v>
@@ -1608,7 +1605,7 @@
         <v>-3.6666666666666701</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
         <v>80</v>
@@ -1616,245 +1613,245 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C24" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
         <v>103</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" t="s">
         <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C29" s="24" t="b">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" t="s">
         <v>127</v>
-      </c>
-      <c r="C30" t="s">
-        <v>130</v>
-      </c>
-      <c r="D30" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="D31" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" t="s">
         <v>148</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" t="s">
         <v>205</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>206</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" t="s">
         <v>207</v>
-      </c>
-      <c r="D35" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1923,9 +1920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2028,43 +2023,43 @@
     </row>
     <row r="3" spans="1:18" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>60</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>163</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>164</v>
       </c>
       <c r="L3" s="16" t="s">
         <v>11</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N3" s="16" t="s">
         <v>12</v>
@@ -2113,7 +2108,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
@@ -2147,7 +2142,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2180,7 +2175,7 @@
         <v>0.05</v>
       </c>
       <c r="R6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2213,7 +2208,7 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2240,7 +2235,7 @@
         <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P8">
         <v>0.752</v>
@@ -2249,7 +2244,7 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="R8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2276,7 +2271,7 @@
         <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P9">
         <v>0.65600000000000003</v>
@@ -2285,7 +2280,7 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="R9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2318,7 +2313,7 @@
         <v>0.9</v>
       </c>
       <c r="R10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2351,7 +2346,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2384,7 +2379,7 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="R12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2415,9 +2410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2509,37 +2502,37 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>58</v>
@@ -2551,13 +2544,13 @@
         <v>26</v>
       </c>
       <c r="M3" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="N3" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="O3" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>13</v>
@@ -3121,9 +3114,7 @@
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E35" s="13" t="s">
-        <v>88</v>
-      </c>
+      <c r="E35" s="13"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
@@ -3411,12 +3402,9 @@
   </sheetData>
   <autoFilter ref="A3:P13" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}"/>
   <phoneticPr fontId="5" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E35" r:id="rId1" location="json=TH95eCDBsN1pfqczsMf84,S3TGIZvZiI-AUl8oZJcUYg" xr:uid="{26F0F99B-4281-4D67-B3C8-B1BC12D732B7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3455,7 +3443,7 @@
         <v>2021</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C2">
         <v>3.6999999999999998E-2</v>
@@ -3483,7 +3471,7 @@
         <v>2021</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C4">
         <v>0.40899999999999997</v>
@@ -3511,7 +3499,7 @@
         <v>2021</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6">
         <v>0.752</v>
@@ -3525,7 +3513,7 @@
         <v>2021</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C7">
         <v>0.65600000000000003</v>
@@ -3539,7 +3527,7 @@
         <v>2021</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8">
         <v>0.96599999999999997</v>
@@ -3553,7 +3541,7 @@
         <v>2021</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C9">
         <v>0.69099999999999995</v>
@@ -3567,7 +3555,7 @@
         <v>2021</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C10">
         <v>0.24299999999999999</v>
@@ -3581,7 +3569,7 @@
         <v>2022</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C11">
         <v>3.6999999999999998E-2</v>
@@ -3609,7 +3597,7 @@
         <v>2022</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13">
         <v>0.40899999999999997</v>
@@ -3637,7 +3625,7 @@
         <v>2022</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C15">
         <v>0.752</v>
@@ -3651,7 +3639,7 @@
         <v>2022</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16">
         <v>0.65600000000000003</v>
@@ -3665,7 +3653,7 @@
         <v>2022</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C17">
         <v>0.96599999999999997</v>
@@ -3679,7 +3667,7 @@
         <v>2022</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C18">
         <v>0.69099999999999995</v>
@@ -3693,7 +3681,7 @@
         <v>2022</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19">
         <v>0.24299999999999999</v>
@@ -3707,7 +3695,7 @@
         <v>2023</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C20">
         <v>3.6999999999999998E-2</v>
@@ -3735,7 +3723,7 @@
         <v>2023</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22">
         <v>0.40899999999999997</v>
@@ -3763,7 +3751,7 @@
         <v>2023</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C24">
         <v>0.752</v>
@@ -3777,7 +3765,7 @@
         <v>2023</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C25">
         <v>0.65600000000000003</v>
@@ -3791,7 +3779,7 @@
         <v>2023</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C26">
         <v>0.96599999999999997</v>
@@ -3805,7 +3793,7 @@
         <v>2023</v>
       </c>
       <c r="B27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C27">
         <v>0.69099999999999995</v>
@@ -3819,7 +3807,7 @@
         <v>2023</v>
       </c>
       <c r="B28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C28">
         <v>0.24299999999999999</v>
@@ -3833,7 +3821,7 @@
         <v>2024</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C29">
         <v>3.6999999999999998E-2</v>
@@ -3861,7 +3849,7 @@
         <v>2024</v>
       </c>
       <c r="B31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31">
         <v>0.40899999999999997</v>
@@ -3889,7 +3877,7 @@
         <v>2024</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C33">
         <v>0.752</v>
@@ -3903,7 +3891,7 @@
         <v>2024</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C34">
         <v>0.65600000000000003</v>
@@ -3917,7 +3905,7 @@
         <v>2024</v>
       </c>
       <c r="B35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C35">
         <v>0.96599999999999997</v>
@@ -3931,7 +3919,7 @@
         <v>2024</v>
       </c>
       <c r="B36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C36">
         <v>0.69099999999999995</v>
@@ -3945,7 +3933,7 @@
         <v>2024</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C37">
         <v>0.24299999999999999</v>
@@ -3959,7 +3947,7 @@
         <v>2025</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C38">
         <v>3.6999999999999998E-2</v>
@@ -3987,7 +3975,7 @@
         <v>2025</v>
       </c>
       <c r="B40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C40">
         <v>0.40899999999999997</v>
@@ -4015,7 +4003,7 @@
         <v>2025</v>
       </c>
       <c r="B42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C42">
         <v>0.752</v>
@@ -4029,7 +4017,7 @@
         <v>2025</v>
       </c>
       <c r="B43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C43">
         <v>0.65600000000000003</v>
@@ -4043,7 +4031,7 @@
         <v>2025</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C44">
         <v>0.96599999999999997</v>
@@ -4057,7 +4045,7 @@
         <v>2025</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C45">
         <v>0.69099999999999995</v>
@@ -4071,7 +4059,7 @@
         <v>2025</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C46">
         <v>0.24299999999999999</v>
@@ -4085,7 +4073,7 @@
         <v>2026</v>
       </c>
       <c r="B47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C47">
         <v>3.6999999999999998E-2</v>
@@ -4113,7 +4101,7 @@
         <v>2026</v>
       </c>
       <c r="B49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C49">
         <v>0.40899999999999997</v>
@@ -4141,7 +4129,7 @@
         <v>2026</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C51">
         <v>0.752</v>
@@ -4155,7 +4143,7 @@
         <v>2026</v>
       </c>
       <c r="B52" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C52">
         <v>0.65600000000000003</v>
@@ -4169,7 +4157,7 @@
         <v>2026</v>
       </c>
       <c r="B53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C53">
         <v>0.96599999999999997</v>
@@ -4183,7 +4171,7 @@
         <v>2026</v>
       </c>
       <c r="B54" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C54">
         <v>0.69099999999999995</v>
@@ -4197,7 +4185,7 @@
         <v>2026</v>
       </c>
       <c r="B55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C55">
         <v>0.24299999999999999</v>
@@ -4211,7 +4199,7 @@
         <v>2027</v>
       </c>
       <c r="B56" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C56">
         <v>3.6999999999999998E-2</v>
@@ -4239,7 +4227,7 @@
         <v>2027</v>
       </c>
       <c r="B58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C58">
         <v>0.40899999999999997</v>
@@ -4267,7 +4255,7 @@
         <v>2027</v>
       </c>
       <c r="B60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C60">
         <v>0.752</v>
@@ -4281,7 +4269,7 @@
         <v>2027</v>
       </c>
       <c r="B61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C61">
         <v>0.65600000000000003</v>
@@ -4295,7 +4283,7 @@
         <v>2027</v>
       </c>
       <c r="B62" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C62">
         <v>0.96599999999999997</v>
@@ -4309,7 +4297,7 @@
         <v>2027</v>
       </c>
       <c r="B63" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C63">
         <v>0.69099999999999995</v>
@@ -4323,7 +4311,7 @@
         <v>2027</v>
       </c>
       <c r="B64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C64">
         <v>0.24299999999999999</v>
@@ -4337,7 +4325,7 @@
         <v>2028</v>
       </c>
       <c r="B65" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C65">
         <v>3.6999999999999998E-2</v>
@@ -4365,7 +4353,7 @@
         <v>2028</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C67">
         <v>0.40899999999999997</v>
@@ -4393,7 +4381,7 @@
         <v>2028</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C69">
         <v>0.752</v>
@@ -4407,7 +4395,7 @@
         <v>2028</v>
       </c>
       <c r="B70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C70">
         <v>0.65600000000000003</v>
@@ -4421,7 +4409,7 @@
         <v>2028</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C71">
         <v>0.96599999999999997</v>
@@ -4435,7 +4423,7 @@
         <v>2028</v>
       </c>
       <c r="B72" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C72">
         <v>0.69099999999999995</v>
@@ -4449,7 +4437,7 @@
         <v>2028</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C73">
         <v>0.24299999999999999</v>
@@ -4463,7 +4451,7 @@
         <v>2029</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C74">
         <v>3.6999999999999998E-2</v>
@@ -4491,7 +4479,7 @@
         <v>2029</v>
       </c>
       <c r="B76" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C76">
         <v>0.40899999999999997</v>
@@ -4519,7 +4507,7 @@
         <v>2029</v>
       </c>
       <c r="B78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C78">
         <v>0.752</v>
@@ -4533,7 +4521,7 @@
         <v>2029</v>
       </c>
       <c r="B79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C79">
         <v>0.65600000000000003</v>
@@ -4547,7 +4535,7 @@
         <v>2029</v>
       </c>
       <c r="B80" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C80">
         <v>0.96599999999999997</v>
@@ -4561,7 +4549,7 @@
         <v>2029</v>
       </c>
       <c r="B81" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C81">
         <v>0.69099999999999995</v>
@@ -4575,7 +4563,7 @@
         <v>2029</v>
       </c>
       <c r="B82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C82">
         <v>0.24299999999999999</v>
@@ -4589,7 +4577,7 @@
         <v>2030</v>
       </c>
       <c r="B83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C83">
         <v>3.6999999999999998E-2</v>
@@ -4617,7 +4605,7 @@
         <v>2030</v>
       </c>
       <c r="B85" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C85">
         <v>0.40899999999999997</v>
@@ -4645,7 +4633,7 @@
         <v>2030</v>
       </c>
       <c r="B87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C87">
         <v>0.752</v>
@@ -4659,7 +4647,7 @@
         <v>2030</v>
       </c>
       <c r="B88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C88">
         <v>0.65600000000000003</v>
@@ -4673,7 +4661,7 @@
         <v>2030</v>
       </c>
       <c r="B89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C89">
         <v>0.96599999999999997</v>
@@ -4687,7 +4675,7 @@
         <v>2030</v>
       </c>
       <c r="B90" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C90">
         <v>0.69099999999999995</v>
@@ -4701,7 +4689,7 @@
         <v>2030</v>
       </c>
       <c r="B91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C91">
         <v>0.24299999999999999</v>
@@ -4739,42 +4727,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="25" t="s">
-        <v>118</v>
-      </c>
       <c r="K1" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>40</v>
@@ -4795,7 +4783,7 @@
         <v>2030</v>
       </c>
       <c r="I2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4841,10 +4829,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4840,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4860,7 +4848,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4868,7 +4856,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4876,7 +4864,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4884,7 +4872,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4892,7 +4880,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4900,18 +4888,18 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4941,12 +4929,12 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -4957,16 +4945,16 @@
         <v>75</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -4977,16 +4965,16 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
         <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -4997,16 +4985,16 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -5014,10 +5002,10 @@
         <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -5025,10 +5013,10 @@
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -5038,17 +5026,17 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -5058,18 +5046,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -5332,6 +5308,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5342,23 +5330,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5377,6 +5348,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated: - Improved documentation for data structures - Cleaned FlowModifierSolver.py - Updated example_data.xlsx
Added:
- Parameter for skipping data checking step
- Using parameter "check_errors" in settings file enables/disables data checking when building data
- FlowModifier: utility method to return list of opposite flow IDs
- FlowSolver: utility method to clamp flow values to minimum of 0.0
- Checking and recalculating relative flow shares after applying flow modifications
- Added more detailed error message when flow modifier opposite targets do not have enough flow to allow applying rule

Fixed:
- Opposite flow shares are now proportionally calculated to allow arbitrary opposite target flow shares
</commit_message>
<xml_diff>
--- a/data/example_data.xlsx
+++ b/data/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1338C6F-D901-4097-AA7E-B0832331462A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DD79D2-AF61-461E-AA21-24C1B4CAFB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="216">
   <si>
     <t>Years</t>
   </si>
@@ -737,6 +737,9 @@
   </si>
   <si>
     <t>Sawnwood:Import</t>
+  </si>
+  <si>
+    <t>Apply to targets</t>
   </si>
 </sst>
 </file>
@@ -932,7 +935,22 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1361,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
   <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,34 +1875,34 @@
   </sheetData>
   <autoFilter ref="B6:E6" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}"/>
   <conditionalFormatting sqref="C15:C16">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="notEqual">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C22">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="notEqual">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C29">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3413,7 +3431,7 @@
   <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4705,10 +4723,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43406F76-D4E1-4DE8-A811-C2AB881D41ED}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4722,10 +4740,11 @@
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>109</v>
       </c>
@@ -4754,13 +4773,16 @@
         <v>116</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -4785,12 +4807,28 @@
       <c r="I2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{008CAED9-3C22-4095-9218-2455CD3CED8E}">
+      <formula1>Boolean</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4805,7 +4843,7 @@
           <x14:formula1>
             <xm:f>'Data validation parameters'!$F$6:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>I2:I1048576 J3:J1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5046,6 +5084,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -5308,42 +5367,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5366,9 +5393,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>